<commit_message>
Kernel 0.92, Issue List #103
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Suggestions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$F$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$6:$G$42</definedName>
   </definedNames>
   <calcPr calcId="145621" calcMode="manual"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="68">
   <si>
     <t>Issue No.</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Something is causing the system to lock up at the shell prompt right in the middle of typing a new command (you go to type CAT and after typing C the system hangs).  I am not sure what command(s) is leading to this.</t>
   </si>
   <si>
-    <t>1004/1026</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -230,13 +227,28 @@
   </si>
   <si>
     <t xml:space="preserve"> Fixed in…</t>
+  </si>
+  <si>
+    <t>1004/1016</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Which NIC/Driver ?</t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>Same correction applied to ARP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,16 +264,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -284,11 +323,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -300,9 +456,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -315,6 +468,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +839,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A2:F43"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,598 +851,635 @@
     <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="46.26953125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.26953125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B6" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1004</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="1">
-        <v>100</v>
+        <f>B7+1</f>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2">
         <v>1004</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="58.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1">
-        <f>B8+1</f>
-        <v>101</v>
+        <f t="shared" ref="B9:B33" si="0">B8+1</f>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
         <v>1004</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="58.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="1">
-        <f t="shared" ref="B10:B34" si="0">B9+1</f>
-        <v>102</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2">
         <v>1004</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="0"/>
-        <v>104</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2">
         <v>1004</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2">
         <v>1004</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="E17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="B19" s="1">
+        <f t="shared" ref="B19:B20" si="1">B18+1</f>
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="1">
-        <f t="shared" si="0"/>
-        <v>110</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1004</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1">
-        <f t="shared" si="0"/>
-        <v>111</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="B20" s="1">
-        <f t="shared" ref="B20:B21" si="1">B19+1</f>
-        <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="1">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1004</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="203" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D21" s="2">
         <v>1004</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="203" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="E21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2">
         <v>1004</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="E22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1016</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1016</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1016</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1016</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="2">
-        <v>1004</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B24" s="1">
-        <f t="shared" si="0"/>
-        <v>116</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1026</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="1">
-        <f t="shared" si="0"/>
-        <v>117</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1026</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B26" s="1">
-        <f t="shared" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1026</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B27" s="1">
-        <f t="shared" si="0"/>
-        <v>119</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
       <c r="D27" s="2">
-        <v>1026</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>1016</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2">
-        <v>1026</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+        <v>1016</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>121</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1026</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>122</v>
-      </c>
-      <c r="F30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-      <c r="F31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-      <c r="F32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-      <c r="F33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="1">
-        <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="F34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F43" t="s">
+      <c r="G33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G42" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:F43">
+  <autoFilter ref="A6:G42">
     <filterColumn colId="0">
-      <filters blank="1">
+      <filters>
         <filter val="V"/>
       </filters>
     </filterColumn>
@@ -1256,7 +1502,7 @@
     <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.6328125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1270,7 +1516,7 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E1" t="s">
@@ -1289,7 +1535,7 @@
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="E3" t="s">
@@ -1300,7 +1546,7 @@
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>40</v>
       </c>
       <c r="E4" t="s">
@@ -1311,7 +1557,7 @@
       <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E5" t="s">

</xml_diff>

<commit_message>
Kernel 0.92, MD5 hash FIX #108
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
   <si>
     <t>Issue No.</t>
   </si>
@@ -830,7 +830,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -842,7 +842,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1123,8 +1123,8 @@
         <v>34</v>
       </c>
       <c r="F15" s="7"/>
-      <c r="G15" t="s">
-        <v>28</v>
+      <c r="G15">
+        <v>1019</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="58" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Kernel 0.92, Shell, PAUSE & SLEEP
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="69">
   <si>
     <t>Issue No.</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>Same correction applied to ARP</t>
+  </si>
+  <si>
+    <t>quick fix for PAUSE:limited to CR</t>
   </si>
 </sst>
 </file>
@@ -841,8 +844,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,7 +1261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <f t="shared" si="0"/>
         <v>115</v>
@@ -1277,7 +1280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <f t="shared" si="0"/>
         <v>116</v>
@@ -1296,7 +1299,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
         <f t="shared" si="0"/>
         <v>117</v>
@@ -1314,7 +1317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="1">
         <f t="shared" si="0"/>
         <v>118</v>
@@ -1328,11 +1331,11 @@
       <c r="E25" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <f t="shared" si="0"/>
         <v>119</v>
@@ -1350,7 +1353,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B27" s="1">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -1368,7 +1371,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="B28" s="1">
         <f t="shared" si="0"/>
         <v>121</v>
@@ -1382,11 +1385,14 @@
       <c r="E28" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" s="1">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -1395,7 +1401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
         <f t="shared" si="0"/>
         <v>123</v>
@@ -1404,7 +1410,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
         <f t="shared" si="0"/>
         <v>124</v>
@@ -1413,7 +1419,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -1422,7 +1428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
         <f t="shared" si="0"/>
         <v>126</v>
@@ -1431,47 +1437,47 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G42" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Kernel 0.92 : SHELL, Added IF ELSE FI and I/O redirection
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="70">
   <si>
     <t>Issue No.</t>
   </si>
@@ -245,6 +245,10 @@
   </si>
   <si>
     <t>quick fix for PAUSE:limited to CR</t>
+  </si>
+  <si>
+    <t>-N implemented
+(Pipe is SHELL related)</t>
   </si>
 </sst>
 </file>
@@ -833,7 +837,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -844,23 +848,23 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="2"/>
-    <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="46.26953125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>66</v>
       </c>
@@ -875,7 +879,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16" t="s">
         <v>57</v>
@@ -888,7 +892,7 @@
       <c r="F3" s="18"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="20"/>
       <c r="B4" s="21" t="s">
         <v>55</v>
@@ -901,12 +905,12 @@
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
@@ -929,7 +933,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -950,7 +954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -994,7 +998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="29.45" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="29.1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -1108,7 +1112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>55</v>
       </c>
@@ -1130,7 +1134,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1147,8 +1151,11 @@
       <c r="E16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G16" t="s">
-        <v>28</v>
+      <c r="F16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16">
+        <v>1022</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1173,7 +1180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -1195,7 +1202,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -1217,7 +1224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="57.95" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -1239,7 +1246,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="203" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="203.1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1261,7 +1268,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="57.95" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <f t="shared" si="0"/>
         <v>115</v>
@@ -1280,7 +1287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <f t="shared" si="0"/>
         <v>116</v>
@@ -1299,7 +1306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
         <f t="shared" si="0"/>
         <v>117</v>
@@ -1317,7 +1324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="B25" s="1">
         <f t="shared" si="0"/>
         <v>118</v>
@@ -1335,7 +1342,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <f t="shared" si="0"/>
         <v>119</v>
@@ -1353,7 +1360,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="B27" s="1">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -1392,7 +1399,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="1">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -1401,7 +1408,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
         <f t="shared" si="0"/>
         <v>123</v>
@@ -1410,7 +1417,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
         <f t="shared" si="0"/>
         <v>124</v>
@@ -1419,7 +1426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -1428,7 +1435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
         <f t="shared" si="0"/>
         <v>126</v>
@@ -1437,47 +1444,47 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="G42" t="s">
         <v>28</v>
       </c>
@@ -1503,16 +1510,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1529,7 +1536,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>45</v>
       </c>
@@ -1548,7 +1555,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>43</v>
       </c>
@@ -1559,7 +1566,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="57.95" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>44</v>
       </c>
@@ -1570,127 +1577,127 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E30" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Kernel 0.92 : EDIT, DNSINFO, REN
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ADC317-8959-4F30-B426-EE19767A79DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$43</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="145621" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="157">
   <si>
     <t>Issue No.</t>
   </si>
@@ -518,11 +512,50 @@
   <si>
     <t>TELNET WORKS FINE for connecting.  The Linux problem was I was trying to go to boxes that only have SSH.  I forgot that I have a special non-SSH regular TELNET box setup (the one you have tested against) and it works fine.  Note though that ALL Telnet sessions (A80s, linux, etc.) end with the Socket Error, but otherwise work fine.</t>
   </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>A2OSX.SRC is FULL
+- Will merge BUILD+SRC in a HD image (32mb) booting MASM3.SYSTEM
+- Rename BUILD -&gt; BOOT800, booting A2osX
+- Create a script MAKEB800 to build BOOT800</t>
+  </si>
+  <si>
+    <t>UNAME, instead ?</t>
+  </si>
+  <si>
+    <t>Planned to close an old issue at GH</t>
+  </si>
+  <si>
+    <t>Multi Protocol stack
+- Remove Config Code in LIBTCPIP
+- Merge Config Code+DHCPCLNT -&gt; IPCONFIG (new switches : -d -s -r)
+- Rename TCPIPD -&gt; NETD
+- Make LIBTCPIP,LIBETLK... to be bound to ETHx by NETD
+- Add etc/netd.conf for protocol binding</t>
+  </si>
+  <si>
+    <t>REN works win file dir, and volume</t>
+  </si>
+  <si>
+    <t>it's a BUG, to be moved in ISSUES
+Should already behave like this!!!</t>
+  </si>
+  <si>
+    <t>Linked to S0022, see comment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -730,9 +763,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -795,14 +825,20 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1110,115 +1146,116 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="2"/>
+    <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.26953125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="18"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1231,15 +1268,15 @@
       <c r="D8" s="2">
         <v>1004</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
       <c r="G8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1253,15 +1290,15 @@
       <c r="D9" s="2">
         <v>1004</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="4"/>
       <c r="G9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1275,15 +1312,15 @@
       <c r="D10" s="2">
         <v>1004</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="4"/>
       <c r="G10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1297,17 +1334,17 @@
       <c r="D11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>120</v>
       </c>
       <c r="G11">
         <v>1018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
@@ -1321,17 +1358,17 @@
       <c r="D12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
@@ -1345,17 +1382,17 @@
       <c r="D13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1369,15 +1406,15 @@
       <c r="D14" s="2">
         <v>1004</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="4"/>
       <c r="G14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1391,15 +1428,15 @@
       <c r="D15" s="2">
         <v>1004</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="4"/>
       <c r="G15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1413,15 +1450,15 @@
       <c r="D16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
       <c r="G16">
         <v>1019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -1445,7 +1482,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -1459,15 +1496,15 @@
       <c r="D18" s="2">
         <v>1004</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
       <c r="G18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -1481,15 +1518,15 @@
       <c r="D19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
       <c r="G19">
         <v>1027</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -1503,15 +1540,15 @@
       <c r="D20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
       <c r="G20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1525,15 +1562,15 @@
       <c r="D21" s="2">
         <v>1004</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="4"/>
       <c r="G21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="203" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -1547,15 +1584,15 @@
       <c r="D22" s="2">
         <v>1004</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
       <c r="G22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <f t="shared" si="0"/>
         <v>115</v>
@@ -1566,15 +1603,15 @@
       <c r="D23" s="2">
         <v>1004</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="4"/>
       <c r="G23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -1588,17 +1625,17 @@
       <c r="D24" s="2">
         <v>1016</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>146</v>
       </c>
       <c r="G24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -1618,11 +1655,11 @@
       <c r="F25" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -1643,7 +1680,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -1667,7 +1704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -1691,7 +1728,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -1715,7 +1752,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -1733,7 +1770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
         <f t="shared" si="0"/>
         <v>123</v>
@@ -1751,7 +1788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <f t="shared" si="0"/>
         <v>124</v>
@@ -1769,7 +1806,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -1783,11 +1820,14 @@
       <c r="E33" s="3" t="s">
         <v>141</v>
       </c>
+      <c r="F33" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="G33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B34" s="1">
         <f t="shared" si="0"/>
         <v>126</v>
@@ -1805,445 +1845,463 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G43" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G43" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A7:G43">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="HT"/>
+        <filter val="V"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="54.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="5"/>
+    <col min="1" max="1" width="6.1796875" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="62.1796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8" style="3" customWidth="1"/>
+    <col min="6" max="6" width="60.90625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+      <c r="F1" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="5" t="s">
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="5" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="5" t="s">
+    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="5" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="5" t="s">
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="5" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="5" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="5" t="s">
+    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="5" t="s">
+    <row r="18" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="5" t="s">
+    <row r="19" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="5" t="s">
+    <row r="20" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="5" t="s">
+    <row r="21" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="F21" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="F24" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="5" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="5" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E27" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E22" s="5" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E28" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="5" t="s">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E29" s="3" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kernel 0.92 : PFT fix,PING fix
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BDECE4-0197-4EBE-BF63-2A0114A4254D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$57</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="145621" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="299">
   <si>
     <t>Issue No.</t>
   </si>
@@ -471,9 +465,6 @@
   </si>
   <si>
     <t>0.92</t>
-  </si>
-  <si>
-    <t>0.9</t>
   </si>
   <si>
     <t>0.93</t>
@@ -494,9 +485,6 @@
 - Rename TCPIPD -&gt; NETD
 - Make LIBTCPIP,LIBETLK... to be bound to ETHx by NETD
 - Add etc/netd.conf for protocol binding</t>
-  </si>
-  <si>
-    <t>REN works win file dir, and volume</t>
   </si>
   <si>
     <r>
@@ -951,11 +939,43 @@
   <si>
     <t>GH #35</t>
   </si>
+  <si>
+    <t>missing stz hFrameIn in LIBTCPIP.S.ICMP</t>
+  </si>
+  <si>
+    <t>0,93</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implemented in…</t>
+  </si>
+  <si>
+    <t>SHELL will handle SYS files, calling API shutown with arg=.SYS file
+this will pass .SYS file to A2osX QC</t>
+  </si>
+  <si>
+    <t>0,92</t>
+  </si>
+  <si>
+    <t>my son did it ! Coming soon…</t>
+  </si>
+  <si>
+    <t>Some already impemented, see GH readme.md</t>
+  </si>
+  <si>
+    <t>CSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUI….
+Same for "FNT": A2osX bitmap font format </t>
+  </si>
+  <si>
+    <t>REN works with file dir, and volume</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1578,22 +1598,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
@@ -1687,7 +1707,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1708,7 +1728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1730,12 +1750,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ref="B10:B57" si="0">B9+1</f>
+        <f t="shared" ref="B10:B34" si="0">B9+1</f>
         <v>102</v>
       </c>
       <c r="C10" t="s">
@@ -1752,7 +1772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1776,7 +1796,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -1846,7 +1866,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1868,7 +1888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1890,7 +1910,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -1936,7 +1956,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -1954,10 +1974,10 @@
         <v>32</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G19">
-        <v>1027</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2004,7 +2024,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -2041,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -2062,14 +2082,14 @@
         <v>1016</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2093,7 +2113,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2138,7 +2158,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2162,7 +2182,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -2255,7 +2275,7 @@
         <v>140</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G33" t="s">
         <v>28</v>
@@ -2279,22 +2299,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <f>B34+1</f>
         <v>127</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D35" s="2">
         <v>1034</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G35" t="s">
         <v>28</v>
@@ -2306,10 +2326,10 @@
         <v>128</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G36" t="s">
         <v>28</v>
@@ -2327,10 +2347,13 @@
         <v>1034</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G37" t="s">
-        <v>28</v>
+        <v>260</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G37">
+        <v>1039</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="90" x14ac:dyDescent="0.25">
@@ -2339,16 +2362,16 @@
         <v>130</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D38" s="2">
         <v>1034</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G38" t="s">
         <v>28</v>
@@ -2484,10 +2507,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G57" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A7:G57">
     <filterColumn colId="0">
       <filters blank="1">
-        <filter val="C"/>
         <filter val="HT"/>
         <filter val="V"/>
       </filters>
@@ -2499,25 +2521,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="62.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="8" style="3" customWidth="1"/>
-    <col min="6" max="6" width="60.85546875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="4"/>
+    <col min="6" max="6" width="62.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>3</v>
       </c>
@@ -2536,8 +2559,11 @@
       <c r="F1" s="30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
@@ -2548,21 +2574,24 @@
         <v>38</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>293</v>
+      </c>
       <c r="F3" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>44</v>
       </c>
@@ -2570,13 +2599,13 @@
         <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>65</v>
       </c>
@@ -2587,10 +2616,10 @@
         <v>87</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>67</v>
       </c>
@@ -2601,10 +2630,10 @@
         <v>69</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>46</v>
       </c>
@@ -2618,7 +2647,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>73</v>
       </c>
@@ -2632,7 +2661,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
@@ -2643,10 +2672,13 @@
         <v>110</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>78</v>
       </c>
@@ -2660,7 +2692,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>81</v>
       </c>
@@ -2674,7 +2706,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>84</v>
       </c>
@@ -2688,7 +2720,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>88</v>
       </c>
@@ -2702,7 +2734,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>91</v>
       </c>
@@ -2716,7 +2748,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>94</v>
       </c>
@@ -2730,7 +2762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>97</v>
       </c>
@@ -2741,10 +2773,10 @@
         <v>99</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>100</v>
       </c>
@@ -2758,7 +2790,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>101</v>
       </c>
@@ -2771,8 +2803,11 @@
       <c r="E18" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>102</v>
       </c>
@@ -2785,8 +2820,11 @@
       <c r="E19" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>103</v>
       </c>
@@ -2800,10 +2838,10 @@
         <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>104</v>
       </c>
@@ -2817,10 +2855,10 @@
         <v>45</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>105</v>
       </c>
@@ -2834,10 +2872,10 @@
         <v>145</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>46</v>
       </c>
@@ -2850,14 +2888,11 @@
       <c r="D23" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>107</v>
       </c>
@@ -2868,152 +2903,164 @@
         <v>142</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F26" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="C31" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>235</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3023,14 +3070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620F4F3B-4970-4434-93DB-A4807F82A4E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J111"/>
   <sheetViews>
     <sheetView topLeftCell="B73" workbookViewId="0">
       <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.5703125" style="39" customWidth="1"/>
     <col min="9" max="9" width="45.7109375" style="31" customWidth="1"/>
@@ -3041,24 +3088,24 @@
         <v>1</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E4" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="34" t="s">
         <v>158</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -3073,108 +3120,108 @@
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="38" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -3182,97 +3229,97 @@
         <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="38" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J25" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="38" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -3295,7 +3342,7 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
@@ -3303,95 +3350,95 @@
         <v>7</v>
       </c>
       <c r="J41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J43" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J44" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J45" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J47" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="38" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J49" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J51" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J52" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -3399,34 +3446,34 @@
         <v>11</v>
       </c>
       <c r="J53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J54" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I55" s="31" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J55" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J56" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -3434,55 +3481,55 @@
         <v>14</v>
       </c>
       <c r="J57" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J58" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" s="38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" s="38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J60" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J61" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J62" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" s="38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J63" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -3490,55 +3537,55 @@
         <v>19</v>
       </c>
       <c r="J64" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B65" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J65" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" s="38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J66" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J67" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" s="38" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J68" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" s="38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J69" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J70" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -3546,47 +3593,47 @@
         <v>23</v>
       </c>
       <c r="J71" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" s="38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J72" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" s="38" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J73" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" s="38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J74" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" s="38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J75" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" s="38" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J76" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -3594,7 +3641,7 @@
         <v>24</v>
       </c>
       <c r="J77" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -3602,7 +3649,7 @@
         <v>30</v>
       </c>
       <c r="J78" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -3610,230 +3657,230 @@
         <v>25</v>
       </c>
       <c r="J79" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" s="38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J80" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J81" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" s="38" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J82" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" s="38" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J83" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B84" s="38" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J84" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" s="38" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J85" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J86" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J87" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B88" s="35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J88" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J89" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J90" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="91" spans="2:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B91" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I91" s="31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J91" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J92" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B93" s="39" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I93" s="31" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J93" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B94" s="39" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J94" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95" s="39" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J95" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96" s="40" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J96" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B97" s="40" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J97" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98" s="40" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J98" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J99" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B100" s="40" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J100" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101" s="40" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J101" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J102" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="103" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B103" s="40" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I103" s="31" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J103" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B104" s="40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I104" s="31" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J104" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I105" s="31" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J105" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B106" s="40" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I106" s="31" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J106" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J107" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J108" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -3841,20 +3888,20 @@
         <v>58</v>
       </c>
       <c r="I109" s="31" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J109" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J110" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J111" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated based on testing of 1047
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA952096-73E6-4FC4-B220-FACCCD7F5199}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$57</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="327">
   <si>
     <t>Issue No.</t>
   </si>
@@ -211,9 +218,6 @@
     <t xml:space="preserve"> Fixed in…</t>
   </si>
   <si>
-    <t>1004/1016</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -392,9 +396,6 @@
     <t>Same correction applied to ARP.  Fixed.</t>
   </si>
   <si>
-    <t>1004/1027</t>
-  </si>
-  <si>
     <t>Verified in latest.  Boot, -run, at prompt EDIT A.  Then type some stuff, then ctrl-S  PRESS ESCAPE and then type aaa and return.  Error 40</t>
   </si>
   <si>
@@ -420,12 +421,6 @@
   </si>
   <si>
     <t>The Version of ProDOS on BUILD (and I assume BOOT) is V2.0.3.  The most current version is 2.4.2.  We should update the version of ProDOS on our discs to match (largley to keep up with the date/clock corrections) and bug fixes.</t>
-  </si>
-  <si>
-    <t>SysInfo</t>
-  </si>
-  <si>
-    <t>Make a new Program called SYSINFO.  Be default it should return the HOSTNAME, System Type (//e, gs. Etc), OS Name, Version (0.92), boot device, etc.  Their should also be options (-H hostname, -S systype, -V version, etc), for each data item so one can write programs that get just the bit they want (like current os version).</t>
   </si>
   <si>
     <t>When you CAT IFTEST you see the whole file, but if you MORE IFTEST, the screen clears and then the file displays.  I believe it is processing the \f on the first line of the file.  This may be good for things like MAN pages that are designed to be formatted, but not desirable for displaying code like IFTEST.  I suggest a option be added to MORE (-S process screen codes) that will do the clears and other VT100 codes, but that the default behavior is to NOT process these codes and behave more like CAT.</t>
@@ -474,9 +469,6 @@
 - Will merge BUILD+SRC in a HD image (32mb) booting MASM3.SYSTEM
 - Rename BUILD -&gt; BOOT800, booting A2osX
 - Create a script MAKEB800 to build BOOT800</t>
-  </si>
-  <si>
-    <t>UNAME, instead ?</t>
   </si>
   <si>
     <t>Multi Protocol stack
@@ -886,9 +878,6 @@
     <t>ls test</t>
   </si>
   <si>
-    <t>Here is one thought on this, how about a SET +U/SET -U option that says Uppercase all file names, no lowercase support.</t>
-  </si>
-  <si>
     <t>Open-Apple</t>
   </si>
   <si>
@@ -934,13 +923,7 @@
     <t>Startup Bypass</t>
   </si>
   <si>
-    <t>From GH #35, implement Ctrl-D bypass of startup file.  Tested, confirm bypass works, but when you get the prompt, if you press Ctrl-D again it locks up the system.  This becomes a problem because people might hit ctrl-d multiple times at start to bypass and the extra one then locks you up.</t>
-  </si>
-  <si>
     <t>GH #35</t>
-  </si>
-  <si>
-    <t>missing stz hFrameIn in LIBTCPIP.S.ICMP</t>
   </si>
   <si>
     <t>0,93</t>
@@ -970,13 +953,155 @@
   </si>
   <si>
     <t>REN works with file dir, and volume</t>
+  </si>
+  <si>
+    <t>On a Linux host, if you are doing something that productes a lot of output (ls -l /usr/bin or ps -ef) there are times of noticable pauses and they grow longer and longer.  And in Linux if you want to abort the command and get back to prompt its Ctrl-C, which aborts TELNET (its handled locally rather than passed to session).  For Telnet you should pass Ctrl-C then have another abort key or sequence (maybe Escape Ctrl-C).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L </t>
+  </si>
+  <si>
+    <t>Boot, you are in A2/ROOT.  Type L, gives right listing.  Type CD .. You are moved to top of VOL.  Type L again and you get the listing for ROOT.  Ls dispplays the right listing.  Note too, the script file for L seems wrong, It should start with $1?  And for whats its worth, there is no L command so this should probably jsut go away.</t>
+  </si>
+  <si>
+    <t>PAUSE should accept any keystroke to continue not just return.</t>
+  </si>
+  <si>
+    <t>Planned 0.93 or after.</t>
+  </si>
+  <si>
+    <t>MD5 should return its result in all lowercase (as do most other MD5 utils/sites).</t>
+  </si>
+  <si>
+    <t>When you ping a host, sometimes it starts listing returns, other times it just sits there for 5 secs before giving timeouts and then sometimes you get 2-4 returns and then the time outs.  This is to know good hosts.</t>
+  </si>
+  <si>
+    <t>Always returns syntax error.  Tried NSCUTIL 12/21/21 17:12:35</t>
+  </si>
+  <si>
+    <t>LS -R /VOLNAME</t>
+  </si>
+  <si>
+    <t>If you do an LS -R /VOLname like "LS -R /A2OSX.BUILD" it will list only PART of the top dir and then give you a volume error $45.</t>
+  </si>
+  <si>
+    <t>L on etc, bin, anydir responds quickly.  L to / there is a little pause (to be expected) before listing volumes.  L /PKA2OSX (my virt drive) respomnds little delay but L /A2OSX.BUILD there is a long pause (+3sec) and then listing.</t>
+  </si>
+  <si>
+    <t>REN</t>
+  </si>
+  <si>
+    <t>REN /vol /newvol works.  But REN file newfile returns [$40]:Invalid path. REN dir newdir also error 40. if you REN /vol/file /vol/newfile it works.</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>Like there is MKDIR alias for MD, there should be an alias RMDIR for RD.  BTW, why is MKDIR BIN?  What extra is there as a bin rather then a script? Like L is to LS.</t>
+  </si>
+  <si>
+    <t>Control-C out of many programs (telnet, ping, memdump) end with [$03]:Unknown Error.</t>
+  </si>
+  <si>
+    <t>$# now reports 1 high.  It reports 1 when no args are passed, and 12 when I pass 11. This is in 1047</t>
+  </si>
+  <si>
+    <t>Closed CD/PWD issue fixed, but other/more problems see #133.</t>
+  </si>
+  <si>
+    <t>1) Boot, then EXIT then re-login (return/return) after 2nd return you get a "FreeMem:hMem already freed,BIN=/A2OSX.BUILD/SBIN/SHELL" message. Then prompt as expected.  2) Boot, then NET, then EXIT, then re-login try LS, CRASH to monitor or worse.</t>
+  </si>
+  <si>
+    <t>When you cancel a ping with Ctrl-C you get a [$03]:Unknown Error.</t>
+  </si>
+  <si>
+    <t>Merged into 138, its happens on all commands.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">missing stz hFrameIn in LIBTCPIP.S.ICMP   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Confirmed still in 1047</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>From GH #35, implement Ctrl-D bypass of startup file.  Tested, confirm bypass works, but when you get the prompt,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if you press Ctrl-D again it locks up the system. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This becomes a problem because people might hit ctrl-d multiple times at start to bypass and the extra one then locks you up.</t>
+    </r>
+  </si>
+  <si>
+    <t>echo \e does not seem to do anything.  This is inverse yes?  I tried in script ECHO "abc \e def \e hello" and no inverse. Tested \b \f \n \% \\ all ok.</t>
+  </si>
+  <si>
+    <t>Tested with multiple commands. No issues found 1047.</t>
+  </si>
+  <si>
+    <t>ARGTEST and SHIFTTEST created.</t>
+  </si>
+  <si>
+    <t>Make a new Program called UNAME.  By default it should return the HOSTNAME, System Type (//e, gs. Etc), OS Name, Version (0.92), boot device, etc.  Their should also be options (-H hostname, -S systype, -V version, etc), for each data item so one can write programs that get just the bit they want (like current os version).</t>
+  </si>
+  <si>
+    <t>UNAME</t>
+  </si>
+  <si>
+    <t>SHELL $PWD</t>
+  </si>
+  <si>
+    <t>RPCDUMP</t>
+  </si>
+  <si>
+    <t>Locks system regardless if NET loaded or not.</t>
+  </si>
+  <si>
+    <t>SHELL script</t>
+  </si>
+  <si>
+    <t>In a script file I have the line "CAT IFTEST" that when the script is run returns an Error 46:File Not Found and the debug ----^ ends 2 spaces after the end of the filename on the line.  If I put CAT /PKA2OSX/TESTS/IFTEST then it works. I think this is related to 141.</t>
+  </si>
+  <si>
+    <t>There should be a way to remove an entry to manually added.</t>
+  </si>
+  <si>
+    <t>If you add a host with DNSINFO myhost 10.0.0.88 and then add the same host again (repear command) the DNS table appears to get corrupted (pasted image in Slack)</t>
+  </si>
+  <si>
+    <t>At command line PWD shows right value, but in script it shows $HOME though I am in a different dir. If you change HOME at cmdline and then run script $PWD in script displays new HOME value.  MORE on this.  My current dir is /PKA2OSX/TESTS, I do LS no prob.  I do L and I get listing for /A2OSX.BUILD/ROOT.  I manually change HOME to PK/TESTS and do L again and I get the right dir.  Somehow L is looking at the same mem address the $PWD is to do the listing or something.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,8 +1139,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1031,6 +1185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1179,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1251,18 +1411,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1290,6 +1438,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1598,28 +1774,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="27" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1627,12 +1802,12 @@
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="28" t="s">
         <v>54</v>
       </c>
       <c r="D2" s="8"/>
@@ -1656,10 +1831,10 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="14"/>
@@ -1691,7 +1866,7 @@
       <c r="B7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23" t="s">
@@ -1701,13 +1876,13 @@
         <v>2</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1728,7 +1903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1750,7 +1925,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1772,7 +1947,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1783,20 +1958,20 @@
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>61</v>
+      <c r="D11" s="2">
+        <v>1004</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G11">
         <v>1018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -1804,17 +1979,17 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>121</v>
+      <c r="D12" s="2">
+        <v>1004</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G12">
         <v>1034</v>
@@ -1822,29 +1997,29 @@
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>61</v>
+      <c r="D13" s="2">
+        <v>1004</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1866,7 +2041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1888,7 +2063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1899,8 +2074,8 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>61</v>
+      <c r="D16" s="2">
+        <v>1004</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>34</v>
@@ -1910,7 +2085,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -1921,20 +2096,20 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>61</v>
+      <c r="D17" s="2">
+        <v>1004</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G17">
         <v>1022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -1956,7 +2131,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -1967,14 +2142,14 @@
       <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>61</v>
+      <c r="D19" s="2">
+        <v>1004</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G19">
         <v>1039</v>
@@ -1985,14 +2160,14 @@
         <v>53</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" ref="B20:B21" si="1">B19+1</f>
+        <f>B19+1</f>
         <v>112</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>61</v>
+      <c r="D20" s="2">
+        <v>1004</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>31</v>
@@ -2002,12 +2177,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="1"/>
+        <f>B20+1</f>
         <v>113</v>
       </c>
       <c r="C21" t="s">
@@ -2024,7 +2199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -2047,11 +2222,14 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="27" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="2">
@@ -2060,8 +2238,8 @@
       <c r="E23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="41" t="s">
-        <v>271</v>
+      <c r="F23" s="37" t="s">
+        <v>315</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -2075,21 +2253,21 @@
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="27" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="2">
         <v>1016</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2097,7 +2275,7 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="2">
@@ -2107,13 +2285,13 @@
         <v>49</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G25">
         <v>1034</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2142,7 +2320,7 @@
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="27" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2">
@@ -2152,13 +2330,13 @@
         <v>51</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2176,13 +2354,13 @@
         <v>52</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G28">
         <v>1026</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -2200,1712 +2378,2039 @@
         <v>59</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G29">
         <v>1020</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="27" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="2">
         <v>1017</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>307</v>
       </c>
       <c r="G30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
         <v>123</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="2">
         <v>1027</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G31" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="2">
         <v>1027</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B33" s="1">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="C33" s="31" t="s">
-        <v>139</v>
+      <c r="C33" s="27" t="s">
+        <v>135</v>
       </c>
       <c r="D33" s="2">
         <v>1027</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B34" s="1">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="C34" s="31" t="s">
-        <v>143</v>
+      <c r="C34" s="27" t="s">
+        <v>139</v>
       </c>
       <c r="D34" s="2">
         <v>1027</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>308</v>
       </c>
       <c r="G34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B35" s="1">
         <f>B34+1</f>
         <v>127</v>
       </c>
-      <c r="C35" s="31" t="s">
-        <v>151</v>
+      <c r="C35" s="27" t="s">
+        <v>146</v>
       </c>
       <c r="D35" s="2">
         <v>1034</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="B36" s="1">
-        <f t="shared" ref="B36:B57" si="2">B35+1</f>
+        <f t="shared" ref="B36:B57" si="1">B35+1</f>
         <v>128</v>
       </c>
-      <c r="C36" s="31" t="s">
-        <v>245</v>
+      <c r="C36" s="27" t="s">
+        <v>240</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D37" s="2">
         <v>1034</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="G37">
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="C38" s="31" t="s">
-        <v>286</v>
+      <c r="C38" s="27" t="s">
+        <v>280</v>
       </c>
       <c r="D38" s="2">
         <v>1034</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>131</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1037</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="G39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="G40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1037</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G40">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>133</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E41" s="47" t="s">
+        <v>309</v>
       </c>
       <c r="G41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>134</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="G42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="B43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>135</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F43" s="47" t="s">
+        <v>311</v>
       </c>
       <c r="G43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>137</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G45">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>141</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>143</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="27" t="s">
+        <v>320</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>145</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>146</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1047</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>149</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G57">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="HT"/>
-        <filter val="V"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <autoFilter ref="A7:G57" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8" style="3" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
     <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="E1" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="E2" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+    </row>
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="43"/>
+      <c r="B3" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="E3" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="44"/>
+    </row>
+    <row r="4" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="E4" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="43"/>
+      <c r="B5" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>282</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="C6" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+    </row>
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>287</v>
+      </c>
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+    </row>
+    <row r="11" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
+      <c r="B11" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="43"/>
+      <c r="B12" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+    </row>
+    <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="C13" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="43"/>
+      <c r="B15" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+    </row>
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+    </row>
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="G18" s="44"/>
+    </row>
+    <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
+      <c r="B19" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="G19" s="44"/>
+    </row>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="G20" s="44"/>
+    </row>
+    <row r="21" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
+      <c r="B21" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+    </row>
+    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="44" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="G22" s="44"/>
+    </row>
+    <row r="23" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="B23" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="44"/>
+    </row>
+    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="G24" s="44">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="43"/>
+      <c r="B25" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="E25" s="45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="F25" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="G25" s="44"/>
+    </row>
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="43"/>
+      <c r="B26" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>235</v>
+      </c>
+      <c r="E26" s="45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="F26" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="G26" s="44"/>
+    </row>
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="43"/>
+      <c r="B27" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="E27" s="45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="F27" s="44" t="s">
+        <v>289</v>
+      </c>
+      <c r="G27" s="44"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="43"/>
+      <c r="B28" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="E28" s="45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="F28" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="G28" s="44"/>
+    </row>
+    <row r="29" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="43"/>
+      <c r="B29" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>282</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="G29" s="44"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="43"/>
+      <c r="B30" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="E30" s="45"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="43"/>
+      <c r="B31" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="E31" s="45"/>
+      <c r="F31" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="G31" s="44"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
+      <c r="B32" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="E32" s="45"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+    </row>
+    <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="43"/>
+      <c r="B33" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="E33" s="45"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+    </row>
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+      <c r="B34" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="44" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="E34" s="45"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="44" t="s">
         <v>231</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="C35" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="E35" s="45"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="43"/>
+      <c r="B37" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="43"/>
+      <c r="B38" s="44" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>239</v>
-      </c>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:J111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B2:I109"/>
   <sheetViews>
-    <sheetView topLeftCell="B73" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="45.7109375" style="31" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C2" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="I7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="I14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="I15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="I16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="I18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="I20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="I21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="I22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="I23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="I24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="I25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="I28" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="I29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="34" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="34"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="34"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="34"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="34"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="34"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="34"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="I40" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="I41" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="I42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="I43" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="I44" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="I45" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="I46" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="I47" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="I48" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="I49" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="I50" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="I52" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="H53" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="I53" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="I54" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I55" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="I56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="I57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="I58" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="I59" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="I60" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="I61" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="I62" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="I63" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="I64" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="I65" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="I66" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="I67" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="I68" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I69" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="I70" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="I71" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="I72" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="I73" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="I74" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I75" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I77" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="I78" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="I79" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="I80" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="I81" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="I82" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="I83" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I84" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="I85" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="I86" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I88" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="B89" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="H89" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="I89" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B91" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="H91" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="I91" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="I92" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="I93" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="I94" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="I95" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="J9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="J10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="J11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="38" t="s">
+      <c r="I96" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I97" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="I98" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="I99" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I100" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B101" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="H101" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="I101" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="H102" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="I102" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H103" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="I103" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B104" s="36" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="J14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="J15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="J16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="J17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="J18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="J19" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="J20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="J22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="J23" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="J24" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="J25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="J26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="J27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="J28" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="J29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="J30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="J31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="38" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="38" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="38"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="38"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="38"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="38"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="38"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="38"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J40" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="J42" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="J43" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="J44" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="J45" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="J46" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="J47" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="38" t="s">
-        <v>186</v>
-      </c>
-      <c r="J48" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="J49" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="J50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="J51" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="J52" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="J53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="J54" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B55" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="I55" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="J55" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="J56" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="J58" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="J59" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="J60" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="J61" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="J62" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="J63" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="J64" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="J65" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="J66" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="J67" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="J68" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="J69" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="J70" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="J71" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="38" t="s">
-        <v>205</v>
-      </c>
-      <c r="J72" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="J73" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="38" t="s">
-        <v>207</v>
-      </c>
-      <c r="J74" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="J75" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="J76" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="J77" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="J78" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="J79" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80" s="38" t="s">
-        <v>210</v>
-      </c>
-      <c r="J80" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B81" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="J81" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B82" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="J82" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B83" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="J83" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B84" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="J84" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="J85" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J86" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B87" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="J87" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B88" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="J88" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J89" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J90" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="91" spans="2:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="B91" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="I91" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="J91" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J92" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B93" s="39" t="s">
-        <v>255</v>
-      </c>
-      <c r="I93" s="31" t="s">
-        <v>256</v>
-      </c>
-      <c r="J93" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B94" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="J94" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B95" s="39" t="s">
-        <v>249</v>
-      </c>
-      <c r="J95" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B96" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="J96" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B97" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="J97" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B98" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="J98" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J99" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B100" s="40" t="s">
-        <v>253</v>
-      </c>
-      <c r="J100" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B101" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="J101" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J102" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B103" s="40" t="s">
+      <c r="H104" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="I103" s="31" t="s">
-        <v>280</v>
-      </c>
-      <c r="J103" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B104" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="I104" s="31" t="s">
-        <v>269</v>
-      </c>
-      <c r="J104" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I105" s="31" t="s">
-        <v>270</v>
-      </c>
-      <c r="J105" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="106" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B106" s="40" t="s">
+      <c r="I104" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I105" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I106" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B107" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="H107" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="I106" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="J106" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J107" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J108" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B109" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="I109" s="31" t="s">
-        <v>278</v>
-      </c>
-      <c r="J109" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J110" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J111" t="s">
-        <v>218</v>
+      <c r="I107" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I108" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I109" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with 1050 testing notes, closed many items.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCBD785-95F0-4BE3-B3DD-7435C668B0EE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$57</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="339">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1128,11 +1134,17 @@
   <si>
     <t>$PWD always reset to $HOME</t>
   </si>
+  <si>
+    <t>In 1050, half fixed.  If you DNSINFO host ip  twice in row from command line no more problem.  but if DNSINFO host ip is in script, 2nd time you run script machine LOCKS at that line in script, so calling from script is bad some how.</t>
+  </si>
+  <si>
+    <t>Change name to RV or MV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1377,7 +1389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1508,6 +1520,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1815,34 +1830,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="27" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="45.26953125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="24.81640625" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -1857,7 +1872,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -1870,7 +1885,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>122</v>
@@ -1883,7 +1898,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>53</v>
@@ -1896,12 +1911,12 @@
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -1924,7 +1939,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1945,7 +1960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1967,7 +1982,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1989,7 +2004,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2037,7 +2052,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>122</v>
       </c>
@@ -2061,7 +2076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -2105,7 +2120,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2151,7 +2166,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -2173,7 +2188,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2197,7 +2212,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2219,7 +2234,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -2241,7 +2256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="217.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -2287,7 +2302,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2309,7 +2324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2354,7 +2369,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2378,7 +2393,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2426,7 +2441,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
@@ -2450,7 +2465,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2471,7 +2486,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
@@ -2492,7 +2507,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -2564,7 +2579,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>122</v>
       </c>
@@ -2582,7 +2597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
@@ -2606,7 +2621,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
@@ -2630,9 +2645,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="1"/>
@@ -2654,7 +2669,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -2675,7 +2690,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <f t="shared" si="1"/>
         <v>133</v>
@@ -2693,7 +2708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <f t="shared" si="1"/>
         <v>134</v>
@@ -2714,7 +2729,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -2738,7 +2753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <f t="shared" si="1"/>
         <v>136</v>
@@ -2756,7 +2771,10 @@
         <v>333</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="B45" s="1">
         <f t="shared" si="1"/>
         <v>137</v>
@@ -2777,7 +2795,10 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B46" s="1">
         <f t="shared" si="1"/>
         <v>138</v>
@@ -2798,7 +2819,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <f t="shared" si="1"/>
         <v>139</v>
@@ -2819,7 +2840,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -2834,7 +2855,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <f t="shared" si="1"/>
         <v>141</v>
@@ -2851,8 +2872,14 @@
       <c r="F49" s="48" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="G49" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B50" s="1">
         <f t="shared" si="1"/>
         <v>142</v>
@@ -2873,7 +2900,10 @@
         <v>330</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B51" s="1">
         <f t="shared" si="1"/>
         <v>143</v>
@@ -2894,7 +2924,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <f t="shared" si="1"/>
         <v>144</v>
@@ -2909,7 +2939,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <f t="shared" si="1"/>
         <v>145</v>
@@ -2924,7 +2954,10 @@
         <v>323</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B54" s="1">
         <f t="shared" si="1"/>
         <v>146</v>
@@ -2941,30 +2974,33 @@
       <c r="F54" s="48" t="s">
         <v>327</v>
       </c>
-      <c r="G54">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G54" s="49" t="s">
+        <v>337</v>
+      </c>
+      <c r="H54" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G57">
+  <autoFilter ref="A7:G57" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="V"/>
@@ -2977,26 +3013,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.7265625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="51.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
@@ -3036,7 +3072,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
     </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A3" s="43"/>
       <c r="B3" s="44" t="s">
         <v>43</v>
@@ -3053,7 +3089,7 @@
       </c>
       <c r="G3" s="44"/>
     </row>
-    <row r="4" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" s="44" t="s">
         <v>44</v>
@@ -3087,7 +3123,7 @@
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" s="44" t="s">
         <v>66</v>
@@ -3104,7 +3140,7 @@
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>46</v>
       </c>
@@ -3121,7 +3157,7 @@
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
     </row>
-    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="44" t="s">
         <v>72</v>
@@ -3157,7 +3193,7 @@
       </c>
       <c r="G9" s="44"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="44" t="s">
         <v>77</v>
@@ -3174,7 +3210,7 @@
       <c r="F10" s="44"/>
       <c r="G10" s="44"/>
     </row>
-    <row r="11" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="44" t="s">
         <v>80</v>
@@ -3191,7 +3227,7 @@
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="44" t="s">
         <v>83</v>
@@ -3208,7 +3244,7 @@
       <c r="F12" s="44"/>
       <c r="G12" s="44"/>
     </row>
-    <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="44" t="s">
         <v>87</v>
@@ -3225,7 +3261,7 @@
       <c r="F13" s="44"/>
       <c r="G13" s="44"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="44" t="s">
         <v>90</v>
@@ -3242,7 +3278,7 @@
       <c r="F14" s="44"/>
       <c r="G14" s="44"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="43"/>
       <c r="B15" s="44" t="s">
         <v>93</v>
@@ -3259,7 +3295,7 @@
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="44" t="s">
         <v>96</v>
@@ -3276,7 +3312,7 @@
       <c r="F16" s="44"/>
       <c r="G16" s="44"/>
     </row>
-    <row r="17" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
       <c r="B17" s="44" t="s">
         <v>99</v>
@@ -3293,7 +3329,7 @@
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
     </row>
-    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
         <v>46</v>
       </c>
@@ -3314,7 +3350,7 @@
       </c>
       <c r="G18" s="44"/>
     </row>
-    <row r="19" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="44" t="s">
         <v>101</v>
@@ -3333,7 +3369,7 @@
       </c>
       <c r="G19" s="44"/>
     </row>
-    <row r="20" spans="1:7" ht="52" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
       <c r="B20" s="44" t="s">
         <v>102</v>
@@ -3352,7 +3388,7 @@
       </c>
       <c r="G20" s="44"/>
     </row>
-    <row r="21" spans="1:7" ht="78" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21" s="44" t="s">
         <v>103</v>
@@ -3369,7 +3405,7 @@
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
     </row>
-    <row r="22" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
         <v>46</v>
       </c>
@@ -3390,7 +3426,7 @@
       </c>
       <c r="G22" s="44"/>
     </row>
-    <row r="23" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
         <v>46</v>
       </c>
@@ -3409,7 +3445,7 @@
       </c>
       <c r="G23" s="44"/>
     </row>
-    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
         <v>46</v>
       </c>
@@ -3432,7 +3468,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
       <c r="B25" s="44" t="s">
         <v>107</v>
@@ -3451,7 +3487,7 @@
       </c>
       <c r="G25" s="44"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="43"/>
       <c r="B26" s="44" t="s">
         <v>108</v>
@@ -3470,7 +3506,7 @@
       </c>
       <c r="G26" s="44"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="44" t="s">
         <v>223</v>
@@ -3489,7 +3525,7 @@
       </c>
       <c r="G27" s="44"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
       <c r="B28" s="44" t="s">
         <v>224</v>
@@ -3508,7 +3544,7 @@
       </c>
       <c r="G28" s="44"/>
     </row>
-    <row r="29" spans="1:7" ht="52" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A29" s="43"/>
       <c r="B29" s="44" t="s">
         <v>225</v>
@@ -3527,7 +3563,7 @@
       </c>
       <c r="G29" s="44"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="43"/>
       <c r="B30" s="44" t="s">
         <v>226</v>
@@ -3542,7 +3578,7 @@
       <c r="F30" s="44"/>
       <c r="G30" s="44"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
       <c r="B31" s="44" t="s">
         <v>227</v>
@@ -3559,7 +3595,7 @@
       </c>
       <c r="G31" s="44"/>
     </row>
-    <row r="32" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="43"/>
       <c r="B32" s="44" t="s">
         <v>228</v>
@@ -3574,7 +3610,7 @@
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
     </row>
-    <row r="33" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A33" s="43"/>
       <c r="B33" s="44" t="s">
         <v>229</v>
@@ -3589,7 +3625,7 @@
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
     </row>
-    <row r="34" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="43"/>
       <c r="B34" s="44" t="s">
         <v>230</v>
@@ -3604,7 +3640,7 @@
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="44" t="s">
         <v>231</v>
@@ -3619,7 +3655,7 @@
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="43"/>
       <c r="B36" s="44" t="s">
         <v>232</v>
@@ -3630,7 +3666,7 @@
       <c r="F36" s="44"/>
       <c r="G36" s="44"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="43"/>
       <c r="B37" s="44" t="s">
         <v>233</v>
@@ -3641,7 +3677,7 @@
       <c r="F37" s="44"/>
       <c r="G37" s="44"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="44" t="s">
         <v>234</v>
@@ -3659,23 +3695,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I109"/>
   <sheetViews>
     <sheetView topLeftCell="B79" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.7265625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="35" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" customWidth="1"/>
-    <col min="6" max="6" width="5.81640625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
@@ -3698,7 +3734,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
         <v>242</v>
       </c>
@@ -3708,7 +3744,7 @@
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="34" t="s">
         <v>65</v>
       </c>
@@ -3721,7 +3757,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
         <v>155</v>
       </c>
@@ -3737,7 +3773,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
         <v>157</v>
       </c>
@@ -3745,7 +3781,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="34" t="s">
         <v>158</v>
       </c>
@@ -3753,17 +3789,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="34" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="34" t="s">
         <v>159</v>
       </c>
@@ -3771,7 +3807,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="34" t="s">
         <v>160</v>
       </c>
@@ -3779,7 +3815,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="34" t="s">
         <v>161</v>
       </c>
@@ -3787,7 +3823,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
         <v>271</v>
       </c>
@@ -3795,7 +3831,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>162</v>
       </c>
@@ -3803,7 +3839,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="34" t="s">
         <v>163</v>
       </c>
@@ -3811,7 +3847,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="34" t="s">
         <v>164</v>
       </c>
@@ -3819,7 +3855,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
         <v>4</v>
       </c>
@@ -3827,7 +3863,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="34" t="s">
         <v>165</v>
       </c>
@@ -3835,7 +3871,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="34" t="s">
         <v>166</v>
       </c>
@@ -3843,7 +3879,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="34" t="s">
         <v>167</v>
       </c>
@@ -3851,7 +3887,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
         <v>168</v>
       </c>
@@ -3859,7 +3895,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="34" t="s">
         <v>169</v>
       </c>
@@ -3867,7 +3903,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="34" t="s">
         <v>170</v>
       </c>
@@ -3875,7 +3911,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="34" t="s">
         <v>171</v>
       </c>
@@ -3883,7 +3919,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="34" t="s">
         <v>172</v>
       </c>
@@ -3891,7 +3927,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="34" t="s">
         <v>173</v>
       </c>
@@ -3899,7 +3935,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="34" t="s">
         <v>174</v>
       </c>
@@ -3907,40 +3943,40 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="34" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="34"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="34"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="34"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="34"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="34"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="34"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I38" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="34" t="s">
         <v>7</v>
       </c>
@@ -3948,7 +3984,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="34" t="s">
         <v>175</v>
       </c>
@@ -3956,7 +3992,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="34" t="s">
         <v>176</v>
       </c>
@@ -3964,7 +4000,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="34" t="s">
         <v>177</v>
       </c>
@@ -3972,7 +4008,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="34" t="s">
         <v>178</v>
       </c>
@@ -3980,7 +4016,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="34" t="s">
         <v>179</v>
       </c>
@@ -3988,7 +4024,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="34" t="s">
         <v>180</v>
       </c>
@@ -3996,7 +4032,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="34" t="s">
         <v>181</v>
       </c>
@@ -4004,7 +4040,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="34" t="s">
         <v>182</v>
       </c>
@@ -4012,7 +4048,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="34" t="s">
         <v>183</v>
       </c>
@@ -4020,7 +4056,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="34" t="s">
         <v>184</v>
       </c>
@@ -4028,7 +4064,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="34" t="s">
         <v>185</v>
       </c>
@@ -4036,7 +4072,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="34" t="s">
         <v>11</v>
       </c>
@@ -4044,7 +4080,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="34" t="s">
         <v>186</v>
       </c>
@@ -4052,7 +4088,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="34" t="s">
         <v>187</v>
       </c>
@@ -4063,7 +4099,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="34" t="s">
         <v>188</v>
       </c>
@@ -4071,7 +4107,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="34" t="s">
         <v>14</v>
       </c>
@@ -4079,7 +4115,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="34" t="s">
         <v>189</v>
       </c>
@@ -4087,7 +4123,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="34" t="s">
         <v>190</v>
       </c>
@@ -4095,7 +4131,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="34" t="s">
         <v>191</v>
       </c>
@@ -4103,7 +4139,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="34" t="s">
         <v>221</v>
       </c>
@@ -4111,7 +4147,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="34" t="s">
         <v>192</v>
       </c>
@@ -4119,7 +4155,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="34" t="s">
         <v>193</v>
       </c>
@@ -4127,7 +4163,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="34" t="s">
         <v>19</v>
       </c>
@@ -4135,7 +4171,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="34" t="s">
         <v>194</v>
       </c>
@@ -4143,7 +4179,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="34" t="s">
         <v>195</v>
       </c>
@@ -4151,7 +4187,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="34" t="s">
         <v>196</v>
       </c>
@@ -4159,7 +4195,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="34" t="s">
         <v>197</v>
       </c>
@@ -4167,7 +4203,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="34" t="s">
         <v>198</v>
       </c>
@@ -4175,7 +4211,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="34" t="s">
         <v>199</v>
       </c>
@@ -4183,7 +4219,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="34" t="s">
         <v>23</v>
       </c>
@@ -4191,7 +4227,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="34" t="s">
         <v>200</v>
       </c>
@@ -4199,7 +4235,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="34" t="s">
         <v>201</v>
       </c>
@@ -4207,7 +4243,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="34" t="s">
         <v>202</v>
       </c>
@@ -4215,7 +4251,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="34" t="s">
         <v>203</v>
       </c>
@@ -4223,7 +4259,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="34" t="s">
         <v>204</v>
       </c>
@@ -4231,7 +4267,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="34" t="s">
         <v>24</v>
       </c>
@@ -4239,7 +4275,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="34" t="s">
         <v>30</v>
       </c>
@@ -4247,7 +4283,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="34" t="s">
         <v>25</v>
       </c>
@@ -4255,7 +4291,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="34" t="s">
         <v>205</v>
       </c>
@@ -4263,7 +4299,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="34" t="s">
         <v>206</v>
       </c>
@@ -4271,7 +4307,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="34" t="s">
         <v>207</v>
       </c>
@@ -4279,7 +4315,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="34" t="s">
         <v>208</v>
       </c>
@@ -4287,7 +4323,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="34" t="s">
         <v>209</v>
       </c>
@@ -4295,7 +4331,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="34" t="s">
         <v>210</v>
       </c>
@@ -4303,12 +4339,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I84" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="31" t="s">
         <v>218</v>
       </c>
@@ -4316,7 +4352,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="31" t="s">
         <v>215</v>
       </c>
@@ -4324,17 +4360,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I87" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I88" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="89" spans="2:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B89" s="35" t="s">
         <v>216</v>
       </c>
@@ -4345,12 +4381,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="91" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="35" t="s">
         <v>250</v>
       </c>
@@ -4361,7 +4397,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="35" t="s">
         <v>243</v>
       </c>
@@ -4369,7 +4405,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="35" t="s">
         <v>244</v>
       </c>
@@ -4377,7 +4413,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="36" t="s">
         <v>245</v>
       </c>
@@ -4385,7 +4421,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="36" t="s">
         <v>246</v>
       </c>
@@ -4393,7 +4429,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="36" t="s">
         <v>247</v>
       </c>
@@ -4401,12 +4437,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I97" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="36" t="s">
         <v>248</v>
       </c>
@@ -4414,7 +4450,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="36" t="s">
         <v>249</v>
       </c>
@@ -4422,12 +4458,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I100" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="101" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B101" s="36" t="s">
         <v>262</v>
       </c>
@@ -4438,7 +4474,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="36" t="s">
         <v>263</v>
       </c>
@@ -4449,7 +4485,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H103" s="27" t="s">
         <v>265</v>
       </c>
@@ -4457,7 +4493,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="104" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B104" s="36" t="s">
         <v>266</v>
       </c>
@@ -4468,17 +4504,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I105" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I106" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="107" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B107" s="35" t="s">
         <v>58</v>
       </c>
@@ -4489,12 +4525,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I108" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I109" t="s">
         <v>213</v>
       </c>

</xml_diff>

<commit_message>
Purged most of sheet 3 for now, moved doc items to suggestion list.  Any Doc item you can assume is mine.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCBD785-95F0-4BE3-B3DD-7435C668B0EE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1192773-6D67-48D4-88B4-D335560C8B0A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="283">
   <si>
     <t>Issue No.</t>
   </si>
@@ -528,190 +528,18 @@
     <t>Help (-h)</t>
   </si>
   <si>
-    <t>ECHO Hello</t>
-  </si>
-  <si>
-    <t>ECHO $TERM</t>
-  </si>
-  <si>
-    <t>Echo $term</t>
-  </si>
-  <si>
     <t>EXIT</t>
   </si>
   <si>
-    <t>IF -d -e -f filename</t>
-  </si>
-  <si>
-    <t>ELSE</t>
-  </si>
-  <si>
-    <t>FI</t>
-  </si>
-  <si>
     <t>PAUSE</t>
   </si>
   <si>
-    <t>SET</t>
-  </si>
-  <si>
-    <t>SET PK1=”Hello World”</t>
-  </si>
-  <si>
-    <t>SET PK1=</t>
-  </si>
-  <si>
-    <t>TIME</t>
-  </si>
-  <si>
-    <t>Redirection</t>
-  </si>
-  <si>
-    <t>&gt; </t>
-  </si>
-  <si>
-    <t>&gt;&gt; </t>
-  </si>
-  <si>
-    <t>1&gt;</t>
-  </si>
-  <si>
-    <t>2&gt;</t>
-  </si>
-  <si>
-    <t>1&gt;&gt;</t>
-  </si>
-  <si>
-    <t>2&gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt; </t>
-  </si>
-  <si>
-    <t>&amp;</t>
-  </si>
-  <si>
-    <t>CAT</t>
-  </si>
-  <si>
-    <t>CAT -A</t>
-  </si>
-  <si>
-    <t>CAT -N</t>
-  </si>
-  <si>
-    <t>CAT -S</t>
-  </si>
-  <si>
-    <t>CHTYP</t>
-  </si>
-  <si>
-    <t>CHTYP -C</t>
-  </si>
-  <si>
-    <t>CHTYP -R</t>
-  </si>
-  <si>
-    <t>CHGRP</t>
-  </si>
-  <si>
-    <t>CHOWN</t>
-  </si>
-  <si>
-    <t>CP etc/hosts /vol</t>
-  </si>
-  <si>
-    <t>CP ETC/HOSTS /vol</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">DNSINFO </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>hostname ipaddr</t>
-    </r>
-  </si>
-  <si>
-    <t>EDIT filename</t>
-  </si>
-  <si>
-    <t>FORMAT S6D2 VOLNAME</t>
-  </si>
-  <si>
-    <t>KILL</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L fn/wildcard</t>
-  </si>
-  <si>
-    <t>LSDEV</t>
-  </si>
-  <si>
-    <t>LSOF</t>
-  </si>
-  <si>
-    <t>MD5 -dhelloworld</t>
-  </si>
-  <si>
-    <t>MD5 -dHELLOWORLD</t>
-  </si>
-  <si>
-    <t>MEM</t>
-  </si>
-  <si>
-    <t>MORE filename</t>
-  </si>
-  <si>
-    <t>MORE -N filename</t>
-  </si>
-  <si>
-    <t>MORE -P filename</t>
-  </si>
-  <si>
-    <t>NETSTAT</t>
-  </si>
-  <si>
-    <t>NFSMOUNT</t>
-  </si>
-  <si>
     <t>NSCUTIL</t>
   </si>
   <si>
-    <t>NTPDATE</t>
-  </si>
-  <si>
-    <t>PASSWD</t>
-  </si>
-  <si>
-    <t>TELNET (TL2 script file)</t>
-  </si>
-  <si>
-    <t>TELNET hostname</t>
-  </si>
-  <si>
-    <t>TOUCH</t>
-  </si>
-  <si>
-    <t>UMOUNT</t>
-  </si>
-  <si>
     <t>USERADD</t>
   </si>
   <si>
-    <t>USERDEL</t>
-  </si>
-  <si>
     <t>Comp.</t>
   </si>
   <si>
@@ -721,15 +549,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>This new sheet has multiple purposes.  1) It is to make sure that every command is being tracked and we have 1 complete list somewhere.  2) To track completion of commands (Col C, RG), that doc is written if appropriate (B, PK), a MAN page is written (E, PK), a test script is written for the command (F, PK) and that each command has imbeded help/usage (-h option) (Col G, RG).</t>
-  </si>
-  <si>
-    <t>UNAME -a -s -n -v -m -o</t>
-  </si>
-  <si>
-    <t>Development</t>
-  </si>
-  <si>
     <t>We need a document that discusses the tools and processes one uses to work on the A2OSX project.  Examples include the TortoiseSVN package to contribute, MarkDownPad to edit MD and other DOC files on github.  Github tools and registration.  How to edit, compile and run a program under A2OSX.</t>
   </si>
   <si>
@@ -742,9 +561,6 @@
     <t>Assign to PK</t>
   </si>
   <si>
-    <t>LS -A -L -R wildcards</t>
-  </si>
-  <si>
     <t>Logo</t>
   </si>
   <si>
@@ -805,33 +621,6 @@
     <t>Need to verify that A2OSX works on real Apple with Thunderclock installed. Test Slots 1 2 and 3.</t>
   </si>
   <si>
-    <t>Control-D at boot</t>
-  </si>
-  <si>
-    <t>TCPIP.CONF file</t>
-  </si>
-  <si>
-    <t>HOSTS file</t>
-  </si>
-  <si>
-    <t>HOSTNAME file</t>
-  </si>
-  <si>
-    <t>STARTUP/INIT file</t>
-  </si>
-  <si>
-    <t>PROFILE files</t>
-  </si>
-  <si>
-    <t>Standard ENV Vars (PS1 PATH)</t>
-  </si>
-  <si>
-    <t>SET command</t>
-  </si>
-  <si>
-    <t>INSTALL</t>
-  </si>
-  <si>
     <t>We need a document on how to install A2OSX on your existing ProDOS HD/CF Card.</t>
   </si>
   <si>
@@ -853,33 +642,9 @@
     <t>PK to write spec sheet for a DB Engine or client/servier API for DB.</t>
   </si>
   <si>
-    <t>PUSHD</t>
-  </si>
-  <si>
-    <t>POPD</t>
-  </si>
-  <si>
-    <t>IF = != (strings)</t>
-  </si>
-  <si>
-    <t>IF -eq -ne -lt -gt -ge -le (int)</t>
-  </si>
-  <si>
-    <t>SSC/SSCI</t>
-  </si>
-  <si>
-    <t>TELNETD</t>
-  </si>
-  <si>
     <t>Same with setting up and using TELNETD</t>
   </si>
   <si>
-    <t>ls test</t>
-  </si>
-  <si>
-    <t>Open-Apple</t>
-  </si>
-  <si>
     <t>Need to document as a way to stop error messages if they start scrolling on screen (like FreeMem). Can also be used during boot to see msgs at each stage.</t>
   </si>
   <si>
@@ -892,9 +657,6 @@
     <t>PK</t>
   </si>
   <si>
-    <t>READ -P "Prompt Phrase" $var</t>
-  </si>
-  <si>
     <t>Write one doc for all SHELL internals, redirection, etc. and need to talk about "." before script.</t>
   </si>
   <si>
@@ -926,9 +688,6 @@
   </si>
   <si>
     <t>0,93</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implemented in…</t>
   </si>
   <si>
     <t>SHELL will handle SYS files, calling API shutown with arg=.SYS file
@@ -1139,6 +898,66 @@
   </si>
   <si>
     <t>Change name to RV or MV</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>A file comparison tool to see if too files are equal.  In the short term I can write a script that uses MD5 to hash both files and if the hash is the same the files are the same.</t>
+  </si>
+  <si>
+    <t>PROFILE</t>
+  </si>
+  <si>
+    <t>Have login run /etc/profile at user login ($SHELL -N $ROOT/ETC/PROFILE)</t>
+  </si>
+  <si>
+    <t>Should create an entry in etc/passwd with USER:PW:UID:GID:GECOS:HOME:SHELL</t>
+  </si>
+  <si>
+    <t>S0038</t>
+  </si>
+  <si>
+    <t>When editing a previous command (hit up arrow) and you move left and change a letter or two and press return to execute command it clears the remainder of the line.  Bash retains the whole line and executes edited command.</t>
+  </si>
+  <si>
+    <t>Future enhancement</t>
+  </si>
+  <si>
+    <t>S0039</t>
+  </si>
+  <si>
+    <t>S0040</t>
+  </si>
+  <si>
+    <t>S0041</t>
+  </si>
+  <si>
+    <t>S0042</t>
+  </si>
+  <si>
+    <t>S0043</t>
+  </si>
+  <si>
+    <t>S0044</t>
+  </si>
+  <si>
+    <t>S0045</t>
+  </si>
+  <si>
+    <t>S0046</t>
+  </si>
+  <si>
+    <t>S0047</t>
+  </si>
+  <si>
+    <t>S0048</t>
+  </si>
+  <si>
+    <t>Doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This new sheet has multiple purposes.  1) It is to make sure that every command is being tracked and we have 1 complete list somewhere.  2) To track completion of commands (Col C, RG), that doc is written if appropriate (B, PK), a MAN page is written (E, PK), a test script is written for the command (F, PK) and that each command has imbeded help/usage (-h option) (Col G, RG). </t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1470,23 +1289,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1512,9 +1314,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1523,6 +1322,33 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1841,19 +1667,19 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="27" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="44" style="3" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2206,7 +2032,7 @@
         <v>32</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
       <c r="G19">
         <v>1039</v>
@@ -2295,8 +2121,8 @@
       <c r="E23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="37" t="s">
-        <v>315</v>
+      <c r="F23" s="30" t="s">
+        <v>239</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -2458,8 +2284,8 @@
       <c r="E30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F30" s="47" t="s">
-        <v>307</v>
+      <c r="F30" s="39" t="s">
+        <v>231</v>
       </c>
       <c r="G30" t="s">
         <v>28</v>
@@ -2549,7 +2375,7 @@
         <v>140</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>308</v>
+        <v>232</v>
       </c>
       <c r="G34" t="s">
         <v>28</v>
@@ -2588,10 +2414,10 @@
         <v>128</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>240</v>
+        <v>183</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>241</v>
+        <v>184</v>
       </c>
       <c r="G36" t="s">
         <v>28</v>
@@ -2612,10 +2438,10 @@
         <v>1034</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>255</v>
+        <v>189</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>312</v>
+        <v>236</v>
       </c>
       <c r="G37">
         <v>1039</v>
@@ -2630,16 +2456,16 @@
         <v>130</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>280</v>
+        <v>205</v>
       </c>
       <c r="D38" s="2">
         <v>1034</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>313</v>
+        <v>237</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>281</v>
+        <v>206</v>
       </c>
       <c r="G38" t="s">
         <v>28</v>
@@ -2660,10 +2486,10 @@
         <v>1037</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="F39" s="48" t="s">
-        <v>335</v>
+        <v>215</v>
+      </c>
+      <c r="F39" s="40" t="s">
+        <v>259</v>
       </c>
       <c r="G39">
         <v>1050</v>
@@ -2678,13 +2504,13 @@
         <v>132</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>292</v>
+        <v>216</v>
       </c>
       <c r="D40" s="2">
         <v>1037</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
       <c r="G40">
         <v>1047</v>
@@ -2696,13 +2522,13 @@
         <v>133</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D41" s="2">
         <v>1047</v>
       </c>
-      <c r="E41" s="47" t="s">
-        <v>309</v>
+      <c r="E41" s="39" t="s">
+        <v>233</v>
       </c>
       <c r="G41" t="s">
         <v>28</v>
@@ -2714,16 +2540,16 @@
         <v>134</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D42" s="2">
         <v>1047</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>295</v>
+        <v>219</v>
       </c>
       <c r="G42" t="s">
         <v>28</v>
@@ -2744,10 +2570,10 @@
         <v>1047</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="F43" s="47" t="s">
-        <v>311</v>
+        <v>234</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>235</v>
       </c>
       <c r="G43" t="s">
         <v>28</v>
@@ -2765,10 +2591,10 @@
         <v>1047</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="F44" s="48" t="s">
-        <v>333</v>
+        <v>221</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2780,16 +2606,16 @@
         <v>137</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
       <c r="D45" s="2">
         <v>1047</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="F45" s="48" t="s">
-        <v>334</v>
+        <v>222</v>
+      </c>
+      <c r="F45" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="G45">
         <v>1050</v>
@@ -2810,10 +2636,10 @@
         <v>1047</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="F46" s="48" t="s">
-        <v>328</v>
+        <v>230</v>
+      </c>
+      <c r="F46" s="40" t="s">
+        <v>252</v>
       </c>
       <c r="G46">
         <v>1050</v>
@@ -2825,16 +2651,16 @@
         <v>139</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>299</v>
+        <v>223</v>
       </c>
       <c r="D47" s="2">
         <v>1047</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="F47" s="48" t="s">
-        <v>331</v>
+        <v>224</v>
+      </c>
+      <c r="F47" s="40" t="s">
+        <v>255</v>
       </c>
       <c r="G47">
         <v>1050</v>
@@ -2852,28 +2678,31 @@
         <v>1047</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <f t="shared" si="1"/>
         <v>141</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>302</v>
+        <v>226</v>
       </c>
       <c r="D49" s="2">
         <v>1047</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F49" s="48" t="s">
-        <v>332</v>
-      </c>
-      <c r="G49" t="s">
-        <v>338</v>
+        <v>227</v>
+      </c>
+      <c r="F49" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="G49" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="H49" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -2891,13 +2720,13 @@
         <v>1047</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="F50" s="48" t="s">
-        <v>329</v>
+        <v>238</v>
+      </c>
+      <c r="F50" s="40" t="s">
+        <v>253</v>
       </c>
       <c r="G50" t="s">
-        <v>330</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -2909,16 +2738,16 @@
         <v>143</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>319</v>
+        <v>243</v>
       </c>
       <c r="D51" s="2">
         <v>1047</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="F51" s="48" t="s">
-        <v>336</v>
+        <v>250</v>
+      </c>
+      <c r="F51" s="40" t="s">
+        <v>260</v>
       </c>
       <c r="G51">
         <v>1050</v>
@@ -2930,13 +2759,13 @@
         <v>144</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>320</v>
+        <v>244</v>
       </c>
       <c r="D52" s="2">
         <v>1047</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>321</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -2945,13 +2774,13 @@
         <v>145</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>322</v>
+        <v>246</v>
       </c>
       <c r="D53" s="2">
         <v>1047</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>323</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -2969,16 +2798,16 @@
         <v>1047</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="F54" s="48" t="s">
-        <v>327</v>
-      </c>
-      <c r="G54" s="49" t="s">
-        <v>337</v>
+        <v>249</v>
+      </c>
+      <c r="F54" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="G54" s="41" t="s">
+        <v>261</v>
       </c>
       <c r="H54" t="s">
-        <v>213</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3014,679 +2843,808 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
     <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="42" t="s">
-        <v>283</v>
+      <c r="G1" s="35" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="G3" s="44"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="36"/>
+      <c r="B4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="G4" s="44"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="45" t="s">
-        <v>282</v>
-      </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="E5" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44" t="s">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="F9" s="44" t="s">
-        <v>287</v>
-      </c>
-      <c r="G9" s="44"/>
+      <c r="E9" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="44" t="s">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="36"/>
+      <c r="B11" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="44" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="44" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44" t="s">
+      <c r="A15" s="36"/>
+      <c r="B15" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
+      <c r="E16" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="45" t="s">
+      <c r="E18" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="44" t="s">
-        <v>316</v>
-      </c>
-      <c r="G18" s="44"/>
+      <c r="F18" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="44" t="s">
+      <c r="A19" s="36"/>
+      <c r="B19" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E19" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="44" t="s">
-        <v>288</v>
-      </c>
-      <c r="G19" s="44"/>
+      <c r="F19" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="G19" s="37"/>
     </row>
     <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="44" t="s">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="44" t="s">
+      <c r="F20" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="G20" s="37"/>
+    </row>
+    <row r="21" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+    </row>
+    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="G22" s="37"/>
+    </row>
+    <row r="23" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="37"/>
+    </row>
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="G24" s="37">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="37"/>
+    </row>
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+      <c r="B26" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="G26" s="37"/>
+    </row>
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" s="37"/>
+    </row>
+    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
+      <c r="B29" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="36"/>
+      <c r="B30" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="38"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E31" s="38"/>
+      <c r="F31" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="G31" s="37"/>
+    </row>
+    <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="36"/>
+      <c r="B32" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" s="38"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+    </row>
+    <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="36"/>
+      <c r="B34" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34" s="38"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="36"/>
+      <c r="B35" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="E35" s="38"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+    </row>
+    <row r="36" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+      <c r="B36" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="E36" s="38"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+    </row>
+    <row r="37" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="36"/>
+      <c r="B37" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="E37" s="38"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
+      <c r="B38" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="E38" s="38"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+    </row>
+    <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G20" s="44"/>
-    </row>
-    <row r="21" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="E21" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-    </row>
-    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="44" t="s">
-        <v>290</v>
-      </c>
-      <c r="G22" s="44"/>
-    </row>
-    <row r="23" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="G23" s="44"/>
-    </row>
-    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="F24" s="44" t="s">
+      <c r="C47" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G24" s="44">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>219</v>
-      </c>
-      <c r="E25" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="G25" s="44"/>
-    </row>
-    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>286</v>
-      </c>
-      <c r="G26" s="44"/>
-    </row>
-    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="44" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>236</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>237</v>
-      </c>
-      <c r="E27" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>289</v>
-      </c>
-      <c r="G27" s="44"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="C28" s="44" t="s">
-        <v>238</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>239</v>
-      </c>
-      <c r="E28" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="G28" s="44"/>
-    </row>
-    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
-      <c r="B29" s="44" t="s">
-        <v>225</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>253</v>
-      </c>
-      <c r="E29" s="45" t="s">
-        <v>282</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>284</v>
-      </c>
-      <c r="G29" s="44"/>
-    </row>
-    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
-      <c r="B30" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="C30" s="44" t="s">
-        <v>256</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>257</v>
-      </c>
-      <c r="E30" s="45"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="44" t="s">
-        <v>227</v>
-      </c>
-      <c r="C31" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>269</v>
-      </c>
-      <c r="E31" s="45"/>
-      <c r="F31" s="44" t="s">
-        <v>270</v>
-      </c>
-      <c r="G31" s="44"/>
-    </row>
-    <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="44" t="s">
-        <v>228</v>
-      </c>
-      <c r="C32" s="44" t="s">
-        <v>276</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>277</v>
-      </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-    </row>
-    <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="44" t="s">
-        <v>229</v>
-      </c>
-      <c r="C33" s="44" t="s">
-        <v>304</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="E33" s="45"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-    </row>
-    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="C34" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>296</v>
-      </c>
-      <c r="E34" s="45"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="C35" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="44" t="s">
-        <v>324</v>
-      </c>
-      <c r="E35" s="45"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="44" t="s">
-        <v>234</v>
-      </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
+      <c r="D48" s="27"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D49" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3696,846 +3654,615 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:I109"/>
+  <dimension ref="B1:I106"/>
   <sheetViews>
-    <sheetView topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.7109375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="42" customWidth="1"/>
+    <col min="3" max="3" width="8" style="43" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="43" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="43"/>
+    <col min="6" max="6" width="5.85546875" style="43" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="43"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I1" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" s="30" t="s">
+      <c r="C4" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F4" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G4" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H4" s="47" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>273</v>
+      <c r="I4" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="48"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="I5" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="I7" t="s">
-        <v>213</v>
+      <c r="B6" s="6"/>
+      <c r="I6" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="I7" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="I8" t="s">
-        <v>213</v>
+      <c r="B8" s="6"/>
+      <c r="I8" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="I9" t="s">
-        <v>213</v>
+      <c r="B9" s="6"/>
+      <c r="I9" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
-        <v>261</v>
+      <c r="B10" s="6"/>
+      <c r="I10" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
-        <v>260</v>
+      <c r="B11" s="6"/>
+      <c r="I11" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="I12" t="s">
-        <v>213</v>
+      <c r="B12" s="6"/>
+      <c r="I12" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="I13" t="s">
-        <v>213</v>
+      <c r="B13" s="6"/>
+      <c r="I13" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="I14" t="s">
-        <v>213</v>
+      <c r="B14" s="6"/>
+      <c r="I14" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="I15" t="s">
-        <v>213</v>
+      <c r="B15" s="6"/>
+      <c r="I15" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="I16" t="s">
-        <v>213</v>
+      <c r="B16" s="6"/>
+      <c r="I16" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="I17" t="s">
-        <v>213</v>
+      <c r="B17" s="6"/>
+      <c r="I17" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="I18" t="s">
-        <v>213</v>
+      <c r="B18" s="6"/>
+      <c r="I18" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" t="s">
-        <v>213</v>
+      <c r="B19" s="6"/>
+      <c r="I19" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="I20" t="s">
-        <v>213</v>
+      <c r="B20" s="6"/>
+      <c r="I20" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="I21" t="s">
-        <v>213</v>
+      <c r="B21" s="6"/>
+      <c r="I21" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="I22" t="s">
-        <v>213</v>
+      <c r="B22" s="6"/>
+      <c r="I22" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="I23" t="s">
-        <v>213</v>
+      <c r="B23" s="6"/>
+      <c r="I23" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="I24" t="s">
-        <v>213</v>
+      <c r="B24" s="6"/>
+      <c r="I24" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="I25" t="s">
-        <v>213</v>
+      <c r="B25" s="6"/>
+      <c r="I25" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="I26" t="s">
-        <v>213</v>
+      <c r="B26" s="6"/>
+      <c r="I26" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="I27" t="s">
-        <v>213</v>
+      <c r="B27" s="6"/>
+      <c r="I27" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="I28" t="s">
-        <v>213</v>
+      <c r="B28" s="6"/>
+      <c r="I28" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="I29" t="s">
-        <v>213</v>
+      <c r="B29" s="6"/>
+      <c r="I29" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="34" t="s">
-        <v>258</v>
+      <c r="B30" s="6"/>
+      <c r="I30" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="34" t="s">
-        <v>259</v>
+      <c r="B31" s="6"/>
+      <c r="I31" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="34"/>
+      <c r="B32" s="6"/>
+      <c r="I32" s="43" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="34"/>
+      <c r="B33" s="6"/>
+      <c r="I33" s="43" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="34"/>
+      <c r="B34" s="6"/>
+      <c r="I34" s="43" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="34"/>
+      <c r="B35" s="6"/>
+      <c r="I35" s="43" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="34"/>
+      <c r="B36" s="6"/>
+      <c r="I36" s="43" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="34"/>
+      <c r="B37" s="6"/>
+      <c r="I37" s="43" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I38" t="s">
-        <v>213</v>
+      <c r="B38" s="6"/>
+      <c r="I38" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" t="s">
-        <v>213</v>
+      <c r="B39" s="6"/>
+      <c r="I39" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="I40" t="s">
-        <v>213</v>
+      <c r="I40" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="I41" t="s">
-        <v>213</v>
+      <c r="B41" s="6"/>
+      <c r="I41" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="I42" t="s">
-        <v>213</v>
+      <c r="B42" s="6"/>
+      <c r="I42" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="I43" t="s">
-        <v>213</v>
+      <c r="B43" s="6"/>
+      <c r="I43" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="I44" t="s">
-        <v>213</v>
+      <c r="B44" s="6"/>
+      <c r="I44" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="I45" t="s">
-        <v>213</v>
+      <c r="B45" s="6"/>
+      <c r="I45" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="I46" t="s">
-        <v>213</v>
+      <c r="B46" s="6"/>
+      <c r="I46" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="I47" t="s">
-        <v>213</v>
+      <c r="B47" s="6"/>
+      <c r="I47" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="I48" t="s">
-        <v>213</v>
+      <c r="B48" s="6"/>
+      <c r="I48" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="I49" t="s">
-        <v>213</v>
+      <c r="B49" s="6"/>
+      <c r="I49" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="I50" t="s">
-        <v>213</v>
+      <c r="B50" s="6"/>
+      <c r="I50" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I51" t="s">
-        <v>213</v>
+      <c r="B51" s="6"/>
+      <c r="I51" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="I52" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="H53" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="I53" t="s">
-        <v>213</v>
+      <c r="B52" s="6"/>
+      <c r="I52" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="6"/>
+      <c r="I53" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="I54" t="s">
-        <v>213</v>
+      <c r="B54" s="6"/>
+      <c r="I54" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I55" t="s">
-        <v>213</v>
+      <c r="B55" s="6"/>
+      <c r="I55" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="I56" t="s">
-        <v>213</v>
+      <c r="B56" s="6"/>
+      <c r="I56" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="I57" t="s">
-        <v>213</v>
+      <c r="B57" s="6"/>
+      <c r="I57" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="I58" t="s">
-        <v>213</v>
+      <c r="B58" s="6"/>
+      <c r="I58" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="I59" t="s">
-        <v>213</v>
+      <c r="B59" s="6"/>
+      <c r="I59" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="I60" t="s">
-        <v>213</v>
+      <c r="B60" s="6"/>
+      <c r="I60" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="34" t="s">
-        <v>193</v>
-      </c>
-      <c r="I61" t="s">
-        <v>213</v>
+      <c r="B61" s="6"/>
+      <c r="I61" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="I62" t="s">
-        <v>213</v>
+      <c r="B62" s="6"/>
+      <c r="I62" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="I63" t="s">
-        <v>213</v>
+      <c r="B63" s="6"/>
+      <c r="I63" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="I64" t="s">
-        <v>213</v>
+      <c r="B64" s="6"/>
+      <c r="I64" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="I65" t="s">
-        <v>213</v>
+      <c r="B65" s="6"/>
+      <c r="I65" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="I66" t="s">
-        <v>213</v>
+      <c r="B66" s="6"/>
+      <c r="I66" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="I67" t="s">
-        <v>213</v>
+      <c r="B67" s="6"/>
+      <c r="I67" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="I68" t="s">
-        <v>213</v>
+      <c r="B68" s="6"/>
+      <c r="I68" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I69" t="s">
-        <v>213</v>
+      <c r="B69" s="6"/>
+      <c r="I69" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="I70" t="s">
-        <v>213</v>
+      <c r="B70" s="6"/>
+      <c r="I70" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="I71" t="s">
-        <v>213</v>
+      <c r="B71" s="6"/>
+      <c r="I71" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="I72" t="s">
-        <v>213</v>
+      <c r="B72" s="6"/>
+      <c r="I72" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="I73" t="s">
-        <v>213</v>
+      <c r="B73" s="6"/>
+      <c r="I73" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="I74" t="s">
-        <v>213</v>
+      <c r="B74" s="6"/>
+      <c r="I74" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="I75" t="s">
-        <v>213</v>
+      <c r="B75" s="6"/>
+      <c r="I75" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" t="s">
-        <v>213</v>
+      <c r="B76" s="6"/>
+      <c r="I76" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="I77" t="s">
-        <v>213</v>
+      <c r="B77" s="6"/>
+      <c r="I77" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="I78" t="s">
-        <v>213</v>
+      <c r="B78" s="6"/>
+      <c r="I78" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="I79" t="s">
-        <v>213</v>
+      <c r="B79" s="6"/>
+      <c r="I79" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="I80" t="s">
-        <v>213</v>
+      <c r="B80" s="6"/>
+      <c r="I80" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="I81" t="s">
-        <v>213</v>
+      <c r="B81" s="6"/>
+      <c r="I81" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="I82" t="s">
-        <v>213</v>
+      <c r="B82" s="6"/>
+      <c r="I82" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="I83" t="s">
-        <v>213</v>
+      <c r="B83" s="6"/>
+      <c r="I83" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I84" t="s">
-        <v>213</v>
+      <c r="B84" s="6"/>
+      <c r="I84" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="I85" t="s">
-        <v>213</v>
+      <c r="B85" s="6"/>
+      <c r="I85" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="I86" t="s">
-        <v>213</v>
+      <c r="I86" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I87" t="s">
-        <v>213</v>
+      <c r="B87" s="49"/>
+      <c r="I87" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I88" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B89" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="H89" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="I89" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I90" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" s="35" t="s">
-        <v>250</v>
-      </c>
-      <c r="H91" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="I91" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B92" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="I92" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B93" s="35" t="s">
-        <v>244</v>
-      </c>
-      <c r="I93" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B94" s="36" t="s">
-        <v>245</v>
-      </c>
-      <c r="I94" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="I95" t="s">
-        <v>213</v>
+      <c r="B88" s="49"/>
+      <c r="I88" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I89" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="I96" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I97" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B98" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="I98" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="I99" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I100" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="101" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B101" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="H101" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="I101" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B102" s="36" t="s">
-        <v>263</v>
-      </c>
-      <c r="H102" s="27" t="s">
-        <v>264</v>
-      </c>
-      <c r="I102" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H103" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="I103" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="104" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B104" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="H104" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="I104" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I105" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I106" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="107" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B107" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="H107" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="I107" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I108" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I109" t="s">
-        <v>213</v>
-      </c>
+      <c r="B96" s="50"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="50"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="50"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="50"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="50"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="50"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="50"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="50"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Issue/Suggest list with 0.92 priorities, floppy with new test scripts.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DE96DC-A2D0-45E3-8AF2-4AE47CFF1E05}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$61</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="300">
   <si>
     <t>Issue No.</t>
   </si>
@@ -845,11 +851,6 @@
 CP,MV,RM should also be impacted</t>
   </si>
   <si>
-    <t>REN is a simple binting to ProDOS API: 
-syntax is : REN oldpath newpath
-if you want REN oldpath newNAME, it is an enhencement</t>
-  </si>
-  <si>
     <t>Beware of bad VBL emulation in Applewin
 should be flagged HT</t>
   </si>
@@ -1004,12 +1005,36 @@
   <si>
     <t>If a script is missing the bin/shell you now give a nice invalid BIN file message, but apple still locks up.</t>
   </si>
+  <si>
+    <t>For DNSINFO make a note that if you add a host with the command you can then add that host again with a different IP and it will update the IP.  Good Stuff.</t>
+  </si>
+  <si>
+    <t>Fixed, created BADSH to test.</t>
+  </si>
+  <si>
+    <t>Redirection</t>
+  </si>
+  <si>
+    <t>If you LS &gt; afile then CAT afile, you see VT100 escape codes buried in the file.  When doing redirection, TERM type should be set to a plain/stripped type so that these formatting codes do not appear in the file.  This would be the same if you were piping the output (say to a printer) you dont want VT100 codes going to a printer).</t>
+  </si>
+  <si>
+    <t>.93</t>
+  </si>
+  <si>
+    <t>May exist with VT100 codes, need to check</t>
+  </si>
+  <si>
+    <t>.95</t>
+  </si>
+  <si>
+    <t>.92</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1078,6 +1103,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1262,7 +1295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1413,6 +1446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1719,34 +1753,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -1761,7 +1795,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -1774,7 +1808,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>122</v>
@@ -1787,7 +1821,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>53</v>
@@ -1800,12 +1834,12 @@
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -1828,7 +1862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1849,7 +1883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1871,7 +1905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1893,7 +1927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2009,7 +2043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2077,7 +2111,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2101,7 +2135,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2119,8 +2153,8 @@
         <v>31</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" t="s">
-        <v>28</v>
+      <c r="G20">
+        <v>0.93</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2191,7 +2225,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2209,8 +2243,8 @@
         <v>145</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" t="s">
-        <v>28</v>
+      <c r="G24">
+        <v>0.93</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2258,7 +2292,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2278,8 +2312,8 @@
       <c r="F27" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G27" t="s">
-        <v>28</v>
+      <c r="G27">
+        <v>0.93</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -2348,13 +2382,13 @@
         <v>117</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G30">
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2371,13 +2405,13 @@
       <c r="E31" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
@@ -2393,10 +2427,10 @@
         <v>130</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G32" t="s">
-        <v>28</v>
+        <v>280</v>
+      </c>
+      <c r="G32">
+        <v>0.93</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2471,7 +2505,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>122</v>
       </c>
@@ -2507,13 +2541,13 @@
         <v>189</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G37">
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
@@ -2533,8 +2567,8 @@
       <c r="F38" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G38" t="s">
-        <v>28</v>
+      <c r="G38" s="54">
+        <v>0.92</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
@@ -2555,7 +2589,7 @@
         <v>214</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G39">
         <v>1050</v>
@@ -2582,7 +2616,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>53</v>
       </c>
@@ -2600,13 +2634,13 @@
         <v>231</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>282</v>
+      </c>
+      <c r="G41" s="54">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2626,8 +2660,8 @@
       <c r="F42" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G42" t="s">
-        <v>28</v>
+      <c r="G42">
+        <v>0.93</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -2654,7 +2688,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>122</v>
       </c>
@@ -2672,7 +2706,7 @@
         <v>220</v>
       </c>
       <c r="F44" s="48" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2693,7 +2727,7 @@
         <v>221</v>
       </c>
       <c r="F45" s="48" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G45">
         <v>1050</v>
@@ -2747,7 +2781,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2764,8 +2798,11 @@
       <c r="E48" s="3" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -2782,11 +2819,11 @@
       <c r="E49" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F49" s="48" t="s">
-        <v>252</v>
-      </c>
-      <c r="G49" s="50" t="s">
-        <v>257</v>
+      <c r="F49" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="G49">
+        <v>0.93</v>
       </c>
       <c r="H49" t="s">
         <v>160</v>
@@ -2834,13 +2871,13 @@
         <v>247</v>
       </c>
       <c r="F51" s="48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G51">
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <f t="shared" si="1"/>
         <v>144</v>
@@ -2854,6 +2891,9 @@
       <c r="E52" s="3" t="s">
         <v>242</v>
       </c>
+      <c r="G52">
+        <v>0.93</v>
+      </c>
     </row>
     <row r="53" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
@@ -2873,9 +2913,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B54" s="1">
         <f t="shared" si="1"/>
@@ -2891,16 +2931,13 @@
         <v>246</v>
       </c>
       <c r="F54" s="39" t="s">
-        <v>286</v>
-      </c>
-      <c r="G54">
-        <v>1071</v>
+        <v>285</v>
       </c>
       <c r="H54" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -2912,10 +2949,13 @@
         <v>1069</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+      <c r="G55">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>148</v>
@@ -2927,10 +2967,13 @@
         <v>1069</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+      <c r="G56">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <f t="shared" si="1"/>
         <v>149</v>
@@ -2942,10 +2985,13 @@
         <v>1069</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+      <c r="G57">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>150</v>
       </c>
@@ -2956,10 +3002,16 @@
         <v>1069</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+      <c r="G58">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B59" s="1">
         <v>151</v>
       </c>
@@ -2970,30 +3022,36 @@
         <v>1069</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G59">
         <v>1072</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B60" s="1">
         <v>152</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D60" s="2">
         <v>1069</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G60">
         <v>1071</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B61" s="1">
         <v>153</v>
       </c>
@@ -3004,14 +3062,34 @@
         <v>1069</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="G61">
         <v>1071</v>
       </c>
     </row>
+    <row r="62" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>154</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1072</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="G62">
+        <v>0.93</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G61">
+  <autoFilter ref="A7:G61" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="V"/>
@@ -3027,23 +3105,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3086,7 +3164,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
     </row>
-    <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="37" t="s">
         <v>43</v>
@@ -3137,7 +3215,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -3154,7 +3232,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -3171,7 +3249,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="37" t="s">
         <v>72</v>
@@ -3185,7 +3263,9 @@
       <c r="E8" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="37" t="s">
+        <v>297</v>
+      </c>
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
@@ -3209,7 +3289,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -3221,7 +3301,7 @@
         <v>79</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
@@ -3238,12 +3318,12 @@
         <v>82</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -3255,7 +3335,7 @@
         <v>85</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
@@ -3272,12 +3352,12 @@
         <v>89</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>45</v>
+        <v>298</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -3289,12 +3369,12 @@
         <v>92</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -3306,7 +3386,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
@@ -3328,7 +3408,7 @@
         <v>208</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G16" s="37"/>
     </row>
@@ -3344,7 +3424,7 @@
         <v>111</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
@@ -3382,7 +3462,7 @@
         <v>114</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F19" s="37" t="s">
         <v>211</v>
@@ -3401,7 +3481,7 @@
         <v>128</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>45</v>
+        <v>299</v>
       </c>
       <c r="F20" s="37" t="s">
         <v>202</v>
@@ -3420,7 +3500,7 @@
         <v>238</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
@@ -3446,7 +3526,7 @@
       </c>
       <c r="G22" s="37"/>
     </row>
-    <row r="23" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>46</v>
       </c>
@@ -3488,7 +3568,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="37" t="s">
         <v>107</v>
@@ -3500,14 +3580,14 @@
         <v>163</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F25" s="37" t="s">
         <v>164</v>
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
@@ -3519,14 +3599,14 @@
         <v>178</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F26" s="37" t="s">
         <v>209</v>
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
         <v>166</v>
@@ -3538,14 +3618,14 @@
         <v>180</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="F27" s="37" t="s">
         <v>212</v>
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="37" t="s">
         <v>167</v>
@@ -3557,7 +3637,7 @@
         <v>182</v>
       </c>
       <c r="E28" s="38" t="s">
-        <v>45</v>
+        <v>299</v>
       </c>
       <c r="F28" s="37" t="s">
         <v>164</v>
@@ -3594,11 +3674,13 @@
       <c r="D30" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="E30" s="38"/>
+      <c r="E30" s="38" t="s">
+        <v>298</v>
+      </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>170</v>
@@ -3609,7 +3691,9 @@
       <c r="D31" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="E31" s="38"/>
+      <c r="E31" s="38" t="s">
+        <v>299</v>
+      </c>
       <c r="F31" s="37" t="s">
         <v>195</v>
       </c>
@@ -3641,7 +3725,9 @@
       <c r="D33" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="E33" s="38"/>
+      <c r="E33" s="38" t="s">
+        <v>296</v>
+      </c>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
     </row>
@@ -3656,11 +3742,13 @@
       <c r="D34" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="E34" s="38"/>
+      <c r="E34" s="38" t="s">
+        <v>296</v>
+      </c>
       <c r="F34" s="37"/>
       <c r="G34" s="37"/>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
         <v>174</v>
@@ -3671,7 +3759,9 @@
       <c r="D35" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="E35" s="38"/>
+      <c r="E35" s="38" t="s">
+        <v>296</v>
+      </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
     </row>
@@ -3681,12 +3771,14 @@
         <v>175</v>
       </c>
       <c r="C36" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="D36" s="37" t="s">
         <v>258</v>
       </c>
-      <c r="D36" s="37" t="s">
-        <v>259</v>
-      </c>
-      <c r="E36" s="38"/>
+      <c r="E36" s="38" t="s">
+        <v>296</v>
+      </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
     </row>
@@ -3696,12 +3788,14 @@
         <v>176</v>
       </c>
       <c r="C37" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="D37" s="37" t="s">
-        <v>261</v>
-      </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="38" t="s">
+        <v>296</v>
+      </c>
       <c r="F37" s="37"/>
       <c r="G37" s="37"/>
     </row>
@@ -3714,9 +3808,11 @@
         <v>157</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>262</v>
-      </c>
-      <c r="E38" s="38"/>
+        <v>261</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>296</v>
+      </c>
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
     </row>
@@ -3725,24 +3821,27 @@
         <v>53</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D39" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F39" s="52" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="F39" s="52" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B40" s="4" t="s">
-        <v>265</v>
-      </c>
       <c r="C40" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>197</v>
@@ -3751,9 +3850,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>13</v>
@@ -3761,82 +3860,114 @@
       <c r="D41" s="4" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="E41" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D42" s="27" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E42" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D43" s="27" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E43" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D44" s="27" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E44" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D45" s="27" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E45" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B47" s="4" t="s">
-        <v>272</v>
-      </c>
       <c r="C47" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D47" s="27" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E47" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>273</v>
-      </c>
-      <c r="D48" s="27"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="4" t="s">
-        <v>274</v>
       </c>
       <c r="D49" s="27"/>
     </row>
@@ -3850,34 +3981,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="41"/>
-    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="41"/>
-    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="41"/>
+    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="41"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="53" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -3889,12 +4020,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I3" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
@@ -3920,7 +4051,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="45"/>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -3931,529 +4062,529 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="I6" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="I8" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="I9" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="46"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="46"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="47"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="47"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="47"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="47"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="47"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="47"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TestLog with names of new Tests that have been created.  Updated Issue list with multiple new issues found in latest build.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A097CC-019C-4DBD-90B2-DADD19A2DD8F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -12,10 +18,10 @@
     <sheet name="Commands" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$71</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$49</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="310">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1018,11 +1024,47 @@
   <si>
     <t>.95</t>
   </si>
+  <si>
+    <t>If you do REN without arguments you get a [$C0] Script Syntax Error.  This is not a script.  Maybe its issuing the wrong error code.</t>
+  </si>
+  <si>
+    <t>MV Dir1 Dir2  results in 0 Files Moved.  I tried full path names, paths with and with out beg/end /</t>
+  </si>
+  <si>
+    <t>The Quit option on more only responds to "Q" being pressed, it should also quit on lcase "q".</t>
+  </si>
+  <si>
+    <t>Now MORE doesn’t process the \f \n\n type things, I just started to write MANPAGES based on this.  Is this a bug or decide to change MORE?</t>
+  </si>
+  <si>
+    <t>TELNETD</t>
+  </si>
+  <si>
+    <t>When you load TELNETD and then do a login a message appears on main user screen about incoming connection.  This message should go to the OA-2 screen, not the OA-1 one.</t>
+  </si>
+  <si>
+    <t>If you have both a local and telnetd session going, you start getting out of mem errors and other strange behavior (like try doing a long LS -R in one session and while going do a LS in the other).</t>
+  </si>
+  <si>
+    <t>LS -R</t>
+  </si>
+  <si>
+    <t>LS -R is displaying contents and doing recursion in the order the filenames/dirs occur in prodos, this is really hard to file.  The recursion on Dirs should happen first and then the files in that DIR should be showed.</t>
+  </si>
+  <si>
+    <t>At a minimum we should remove TELNETD startup from NET.</t>
+  </si>
+  <si>
+    <t>String Tests All Fail, see new IFSTRTEST</t>
+  </si>
+  <si>
+    <t>Was editing script, did a number of mark block copy and paste, after 5-6 EDIT crashed with hMem error.  Came back later and did large Block B/E and Ctrl-D and EDIT crashed with Hmem error.  3rd Reboot, edit file and deleted multiple lines (10+) with Ctrl-W and EDIT went bat shit crazy then locked.  Went to close AWin and PC Crashed hard.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1742,22 +1784,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
@@ -2124,7 +2166,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2214,7 +2256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2281,7 +2323,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2377,7 +2419,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2629,7 +2671,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2770,7 +2812,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2791,7 +2833,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -2866,7 +2908,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <f t="shared" si="1"/>
         <v>144</v>
@@ -2926,7 +2968,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -2944,7 +2986,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>148</v>
@@ -2962,7 +3004,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <f t="shared" si="1"/>
         <v>149</v>
@@ -2980,7 +3022,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>150</v>
       </c>
@@ -3060,7 +3102,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>154</v>
       </c>
@@ -3077,18 +3119,140 @@
         <v>0.93</v>
       </c>
     </row>
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
+        <v>155</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
+        <v>156</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" s="1">
+        <v>157</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B66" s="1">
+        <v>158</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
+        <v>159</v>
+      </c>
+      <c r="C67" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>160</v>
+      </c>
+      <c r="C68" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <v>161</v>
+      </c>
+      <c r="C69" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>162</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
+        <v>163</v>
+      </c>
+      <c r="C71" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1075</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G62">
+  <autoFilter ref="A7:G71" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
-      <filters>
+      <filters blank="1">
         <filter val="V"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters blank="1">
-        <filter val="0,92"/>
-        <filter val="1071"/>
-        <filter val="1072"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3101,15 +3265,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
@@ -3231,7 +3395,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -3267,7 +3431,7 @@
       </c>
       <c r="G8" s="37"/>
     </row>
-    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>46</v>
       </c>
@@ -3390,7 +3554,7 @@
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
     </row>
-    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>46</v>
       </c>
@@ -3428,7 +3592,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>46</v>
       </c>
@@ -3504,7 +3668,7 @@
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
         <v>46</v>
       </c>
@@ -3525,7 +3689,7 @@
       </c>
       <c r="G22" s="37"/>
     </row>
-    <row r="23" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>46</v>
       </c>
@@ -3544,7 +3708,7 @@
       </c>
       <c r="G23" s="37"/>
     </row>
-    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>46</v>
       </c>
@@ -3971,7 +4135,12 @@
       <c r="D49" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G49">
+  <autoFilter ref="A1:G49" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="V"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters blank="1">
         <filter val="0,92"/>
@@ -3988,14 +4157,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>

</xml_diff>

<commit_message>
Committing Sheet and Floppy so you can run the new IFNUMTEST which is showing several IF -GE -LE -NE type errors.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16EA3FB-77CF-46AD-8640-BCAF4568A212}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$71</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$49</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="327">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1070,11 +1076,53 @@
 1&gt; ${ROOT}/VAR/LOG/TELNETD.LOG 
 2&gt; ${ROOT}/VAR/LOG/TELNETD.ERR </t>
   </si>
+  <si>
+    <t>Editing comand line, Ctrl-X deletes rest of line, Ctrl-C clear line but keep in history, hist is 256 bytes</t>
+  </si>
+  <si>
+    <t>S0049</t>
+  </si>
+  <si>
+    <t>Add the ability to parse substrings ${VAR:12:22}.  This will likely also require a LEN($VAR) command.</t>
+  </si>
+  <si>
+    <t>S0050</t>
+  </si>
+  <si>
+    <t>S0051</t>
+  </si>
+  <si>
+    <t>S0052</t>
+  </si>
+  <si>
+    <t>S0053</t>
+  </si>
+  <si>
+    <t>S0054</t>
+  </si>
+  <si>
+    <t>S0055</t>
+  </si>
+  <si>
+    <t>Add a way to ECHO "something" with no CR/LF, so that the next ECHO "else" will put on screen "somethingelse".  There are many uses like Displaying "Test IF LT: " and then after test run "Pass or Fail" on same line.  Or if processing large loop, can ECHO "."; and have dots appear for each loop run.</t>
+  </si>
+  <si>
+    <t>If you are running a long script (IFNUMTEST) and press Ctrl-S to pause output you get [$80} Unknown Error in the script, and you have to press return to continue the script.</t>
+  </si>
+  <si>
+    <t>EDIT longfile.  Down arrow 5 or 6 times, hit Ctrl-P to page down, the top 5-6 lines get blanked and cursor goes bottom.  If you Ctrl-O/P at top/bttm screen its ok</t>
+  </si>
+  <si>
+    <t>IF Numerics</t>
+  </si>
+  <si>
+    <t>Several Tests failing, see new IFNUMTEST tests 4 8 9 12 and 14</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1503,9 +1551,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1514,6 +1559,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1822,34 +1870,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -1864,7 +1912,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -1877,7 +1925,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>122</v>
@@ -1890,7 +1938,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>53</v>
@@ -1903,12 +1951,12 @@
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -1931,7 +1979,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1952,7 +2000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1974,7 +2022,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1996,7 +2044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2112,7 +2160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2180,7 +2228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2204,7 +2252,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2616,7 +2664,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
@@ -2630,7 +2678,7 @@
       <c r="D38" s="2">
         <v>1034</v>
       </c>
-      <c r="E38" s="57" t="s">
+      <c r="E38" s="56" t="s">
         <v>234</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -2685,7 +2733,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>53</v>
       </c>
@@ -2705,11 +2753,11 @@
       <c r="F41" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="G41" s="56">
+      <c r="G41" s="55">
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2850,7 +2898,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2871,7 +2919,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -2946,7 +2994,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <f t="shared" si="1"/>
         <v>144</v>
@@ -3006,7 +3054,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B55" s="1">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -3020,11 +3071,14 @@
       <c r="E55" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="G55" s="56">
+      <c r="G55" s="55">
         <v>1079</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>148</v>
@@ -3042,7 +3096,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <f t="shared" si="1"/>
         <v>149</v>
@@ -3053,14 +3107,17 @@
       <c r="D57" s="2">
         <v>1069</v>
       </c>
-      <c r="E57" s="55" t="s">
+      <c r="E57" s="54" t="s">
         <v>278</v>
       </c>
       <c r="G57">
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B58" s="1">
         <v>150</v>
       </c>
@@ -3140,7 +3197,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>154</v>
       </c>
@@ -3157,7 +3214,10 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B63" s="1">
         <v>155</v>
       </c>
@@ -3174,7 +3234,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>156</v>
       </c>
@@ -3194,7 +3254,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B65" s="1">
         <v>157</v>
       </c>
@@ -3211,7 +3274,10 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B66" s="1">
         <v>158</v>
       </c>
@@ -3228,7 +3294,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
         <v>159</v>
       </c>
@@ -3248,7 +3314,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>160</v>
       </c>
@@ -3258,14 +3324,14 @@
       <c r="D68" s="2">
         <v>1075</v>
       </c>
-      <c r="E68" s="58" t="s">
+      <c r="E68" s="57" t="s">
         <v>303</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="69" spans="2:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>161</v>
       </c>
@@ -3285,7 +3351,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B70" s="1">
         <v>162</v>
       </c>
@@ -3302,7 +3371,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="2:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>163</v>
       </c>
@@ -3312,12 +3381,54 @@
       <c r="D71" s="2">
         <v>1075</v>
       </c>
-      <c r="E71" s="55" t="s">
+      <c r="E71" s="54" t="s">
         <v>308</v>
       </c>
     </row>
+    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <v>164</v>
+      </c>
+      <c r="C72" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1079</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B73" s="1">
+        <v>165</v>
+      </c>
+      <c r="C73" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1079</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
+        <v>166</v>
+      </c>
+      <c r="C74" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1079</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G71">
+  <autoFilter ref="A7:G71" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="V"/>
@@ -3339,24 +3450,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3452,7 +3563,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -3469,7 +3580,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -3486,7 +3597,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="37" t="s">
         <v>72</v>
@@ -3528,7 +3639,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -3562,7 +3673,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -3596,7 +3707,7 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -3613,7 +3724,7 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -3708,7 +3819,7 @@
       </c>
       <c r="G19" s="37"/>
     </row>
-    <row r="20" spans="1:7" ht="52" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="37" t="s">
         <v>102</v>
@@ -3807,7 +3918,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="37" t="s">
         <v>107</v>
@@ -3864,7 +3975,7 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="37" t="s">
         <v>167</v>
@@ -3919,7 +4030,7 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>170</v>
@@ -3938,7 +4049,7 @@
       </c>
       <c r="G31" s="37"/>
     </row>
-    <row r="32" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="36"/>
       <c r="B32" s="37" t="s">
         <v>171</v>
@@ -3987,7 +4098,7 @@
       <c r="F34" s="37"/>
       <c r="G34" s="37"/>
     </row>
-    <row r="35" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
         <v>174</v>
@@ -4055,7 +4166,7 @@
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
     </row>
-    <row r="39" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>53</v>
       </c>
@@ -4078,7 +4189,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>264</v>
       </c>
@@ -4106,7 +4217,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>266</v>
       </c>
@@ -4120,7 +4231,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>267</v>
       </c>
@@ -4134,7 +4245,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
         <v>268</v>
       </c>
@@ -4148,7 +4259,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>269</v>
       </c>
@@ -4162,7 +4273,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
         <v>270</v>
       </c>
@@ -4176,7 +4287,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>271</v>
       </c>
@@ -4190,7 +4301,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>272</v>
       </c>
@@ -4207,14 +4318,66 @@
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D49" s="27"/>
+      <c r="C49" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>321</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G49">
+  <autoFilter ref="A1:G49" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="V"/>
@@ -4236,51 +4399,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="41"/>
-    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="41"/>
-    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="41"/>
+    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="41"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="58" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I3" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
@@ -4306,7 +4469,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="45"/>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -4317,529 +4480,529 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="I6" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="I8" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="I9" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="46"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="46"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="47"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="47"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="47"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="47"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="47"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="47"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Issue List with closed and new issues.  Test floppy updated with new tests and TestLog has new tests listed.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16EA3FB-77CF-46AD-8640-BCAF4568A212}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA2519E-6417-4F7D-8DC8-3082F9169171}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Commands" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$71</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$56</definedName>
   </definedNames>
   <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="337">
   <si>
     <t>Issue No.</t>
   </si>
@@ -457,12 +457,6 @@
   </si>
   <si>
     <t>Exiting shell (Ctrl-D) then relog in puts you in a nomans land for CD/PWD and then gives FreeMem error.</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.93</t>
   </si>
   <si>
     <t>A2OSX.SRC is FULL
@@ -556,9 +550,6 @@
     <t>MAN</t>
   </si>
   <si>
-    <t>Need a product specification for V1.0 and V2.0 of MAN system.</t>
-  </si>
-  <si>
     <t>Assign to PK</t>
   </si>
   <si>
@@ -683,18 +674,12 @@
   </si>
   <si>
     <t>GH #35</t>
-  </si>
-  <si>
-    <t>0,93</t>
   </si>
   <si>
     <t>SHELL will handle SYS files, calling API shutown with arg=.SYS file
 this will pass .SYS file to A2osX QC</t>
   </si>
   <si>
-    <t>0,92</t>
-  </si>
-  <si>
     <t>my son did it ! Coming soon…</t>
   </si>
   <si>
@@ -708,9 +693,6 @@
 Same for "FNT": A2osX bitmap font format </t>
   </si>
   <si>
-    <t>REN works with file dir, and volume</t>
-  </si>
-  <si>
     <t>On a Linux host, if you are doing something that productes a lot of output (ls -l /usr/bin or ps -ef) there are times of noticable pauses and they grow longer and longer.  And in Linux if you want to abort the command and get back to prompt its Ctrl-C, which aborts TELNET (its handled locally rather than passed to session).  For Telnet you should pass Ctrl-C then have another abort key or sequence (maybe Escape Ctrl-C).</t>
   </si>
   <si>
@@ -721,9 +703,6 @@
   </si>
   <si>
     <t>PAUSE should accept any keystroke to continue not just return.</t>
-  </si>
-  <si>
-    <t>Planned 0.93 or after.</t>
   </si>
   <si>
     <t>MD5 should return its result in all lowercase (as do most other MD5 utils/sites).</t>
@@ -866,9 +845,6 @@
     <t>$PWD always reset to $HOME</t>
   </si>
   <si>
-    <t>Change name to RV or MV</t>
-  </si>
-  <si>
     <t>COMP</t>
   </si>
   <si>
@@ -1019,9 +995,6 @@
     <t>If you LS &gt; afile then CAT afile, you see VT100 escape codes buried in the file.  When doing redirection, TERM type should be set to a plain/stripped type so that these formatting codes do not appear in the file.  This would be the same if you were piping the output (say to a printer) you dont want VT100 codes going to a printer).</t>
   </si>
   <si>
-    <t>.95</t>
-  </si>
-  <si>
     <t>If you do REN without arguments you get a [$C0] Script Syntax Error.  This is not a script.  Maybe its issuing the wrong error code.</t>
   </si>
   <si>
@@ -1061,9 +1034,6 @@
     <t>ECHO -N "blah blah" suppress ending CR/LF
 ECHO -N "blah blah\r" move cursor back to beginning of line
 ECHO "\e[10;33Htest" prints "test at line 10, row 33</t>
-  </si>
-  <si>
-    <t>Ehnancement</t>
   </si>
   <si>
     <t>MV -R is required to cp/mv/rm DIRs</t>
@@ -1077,9 +1047,6 @@
 2&gt; ${ROOT}/VAR/LOG/TELNETD.ERR </t>
   </si>
   <si>
-    <t>Editing comand line, Ctrl-X deletes rest of line, Ctrl-C clear line but keep in history, hist is 256 bytes</t>
-  </si>
-  <si>
     <t>S0049</t>
   </si>
   <si>
@@ -1117,6 +1084,69 @@
   </si>
   <si>
     <t>Several Tests failing, see new IFNUMTEST tests 4 8 9 12 and 14</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>Extend Exit command in scripts to support a return code.</t>
+  </si>
+  <si>
+    <t>See http://wiki.bash-hackers.org/scripting/terminalcodes</t>
+  </si>
+  <si>
+    <t>Need a product specification for V1.0 and V2.0 of MAN system. A special MAN program that does page up and down and does hyperlinks (tab) and HyperCard Like behaviors.</t>
+  </si>
+  <si>
+    <t>File Structure/Layout, what files go where, HOME, USR/BIN</t>
+  </si>
+  <si>
+    <t>Spec</t>
+  </si>
+  <si>
+    <t>Write up idea for RAM3/Cache/Bin thing at startup</t>
+  </si>
+  <si>
+    <t>ECHO -N</t>
+  </si>
+  <si>
+    <t>Change name to RV or MV.  This is also a document error, README.MD needs to be updated so say REN only works on vol names.</t>
+  </si>
+  <si>
+    <t>When you Ctrl-S save, it prompts for filename and you press return to save, after it saves your cursor is moved down one line, like you pressed down arrow.</t>
+  </si>
+  <si>
+    <t>If you Ctrl-W to delete 2 lines in a row it erases the wrong row.  If you are on row 2, and ctrl-w twice it first erases 2 and then it erases 1 instead of the new 2 (which is the old 3).  Its not always, it may have to do with if you are at the end of the line when doing deletes or have added below and moved back up in file.  I will try to get exact keystrokes to reproduce.</t>
+  </si>
+  <si>
+    <t>add support for \a bell, \t tab, \v vtab, \r CR and I would not mind a \p14:22 thing that is a short code for position cursor to line 14 col 22</t>
+  </si>
+  <si>
+    <t>VTTEST if you run it, error occurs because of ; in the VT100 code (valid code), if you MORE the file it processes the code correctly, but running the script causes error. VTTEST2 tries other codes too that do not seem to work.</t>
+  </si>
+  <si>
+    <t>I need to understand what codes work for CONSOLE.DRV so I can document for developers and script writers.</t>
+  </si>
+  <si>
+    <t>No longer locks without Arg.</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Enhancement</t>
+  </si>
+  <si>
+    <t>REN works with VOL</t>
+  </si>
+  <si>
+    <t>Editing comand line, Ctrl-X is destrcutive BS, Ctrl-C clear line but keep in history, hist is 256 bytes</t>
+  </si>
+  <si>
+    <t>EXIT Arg</t>
+  </si>
+  <si>
+    <t>When you do EXIT 20 in a script, the script then gives yuou a Line #xx:[$14] Unknown Error (14 being Hex for 20).  The script should not through the error, but rather return it to called script that can be evaluating $?.  See RCTEST, RCSUB1 and RCSUB2</t>
   </si>
 </sst>
 </file>
@@ -1402,7 +1432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1544,9 +1574,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1563,6 +1590,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1878,11 +1920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A73" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +2020,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2000,7 +2041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2022,7 +2063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -2044,7 +2085,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2068,7 +2109,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -2092,7 +2133,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>122</v>
       </c>
@@ -2116,7 +2157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -2138,7 +2179,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -2156,11 +2197,8 @@
         <v>20</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2182,7 +2220,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -2206,7 +2244,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -2228,7 +2266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2246,13 +2284,13 @@
         <v>32</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G19">
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2274,7 +2312,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -2296,7 +2334,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -2318,7 +2356,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -2336,13 +2374,13 @@
         <v>48</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2357,14 +2395,14 @@
         <v>1016</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24">
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2388,7 +2426,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2409,7 +2447,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2433,7 +2471,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2457,7 +2495,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -2481,7 +2519,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -2499,13 +2537,13 @@
         <v>117</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="G30">
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2526,7 +2564,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -2544,13 +2582,13 @@
         <v>130</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="G32">
         <v>0.93</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -2568,13 +2606,13 @@
         <v>136</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
@@ -2592,13 +2630,13 @@
         <v>140</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -2607,22 +2645,22 @@
         <v>127</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D35" s="2">
         <v>1034</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>122</v>
       </c>
@@ -2631,16 +2669,16 @@
         <v>128</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -2655,10 +2693,10 @@
         <v>1034</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G37">
         <v>1039</v>
@@ -2673,22 +2711,22 @@
         <v>130</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D38" s="2">
         <v>1034</v>
       </c>
-      <c r="E38" s="56" t="s">
-        <v>234</v>
+      <c r="E38" s="55" t="s">
+        <v>227</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G38" s="53">
+        <v>202</v>
+      </c>
+      <c r="G38" s="52">
         <v>0.92</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -2703,16 +2741,16 @@
         <v>1037</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G39">
         <v>1050</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -2721,13 +2759,13 @@
         <v>132</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D40" s="2">
         <v>1037</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G40">
         <v>1047</v>
@@ -2735,29 +2773,29 @@
     </row>
     <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D41" s="2">
         <v>1047</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="G41" s="55">
+        <v>274</v>
+      </c>
+      <c r="G41" s="54">
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2766,22 +2804,19 @@
         <v>134</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D42" s="2">
         <v>1047</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="G42">
         <v>0.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -2796,16 +2831,16 @@
         <v>1047</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F43" s="39" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="G43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>122</v>
       </c>
@@ -2820,13 +2855,13 @@
         <v>1047</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F44" s="48" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>122</v>
       </c>
@@ -2835,22 +2870,22 @@
         <v>137</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D45" s="2">
         <v>1047</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F45" s="48" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G45">
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2865,16 +2900,16 @@
         <v>1047</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F46" s="48" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="G46">
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2883,22 +2918,22 @@
         <v>139</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D47" s="2">
         <v>1047</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F47" s="48" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="G47">
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2913,13 +2948,13 @@
         <v>1047</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G48">
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -2928,25 +2963,25 @@
         <v>141</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D49" s="2">
         <v>1047</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F49" s="50" t="s">
-        <v>256</v>
+        <v>324</v>
       </c>
       <c r="G49">
         <v>0.93</v>
       </c>
       <c r="H49" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
@@ -2961,16 +2996,16 @@
         <v>1047</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F50" s="48" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="G50" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
@@ -2979,40 +3014,46 @@
         <v>143</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D51" s="2">
         <v>1047</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F51" s="48" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G51">
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B52" s="1">
         <f t="shared" si="1"/>
         <v>144</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D52" s="2">
         <v>1047</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>330</v>
       </c>
       <c r="G52">
         <v>0.93</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>46</v>
       </c>
@@ -3021,16 +3062,16 @@
         <v>145</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D53" s="2">
         <v>1047</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>46</v>
       </c>
@@ -3045,13 +3086,13 @@
         <v>1047</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F54" s="39" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="H54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -3069,9 +3110,9 @@
         <v>1069</v>
       </c>
       <c r="E55" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="G55" s="55">
+        <v>268</v>
+      </c>
+      <c r="G55" s="54">
         <v>1079</v>
       </c>
     </row>
@@ -3090,7 +3131,7 @@
         <v>1069</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="G56">
         <v>1078</v>
@@ -3107,8 +3148,8 @@
       <c r="D57" s="2">
         <v>1069</v>
       </c>
-      <c r="E57" s="54" t="s">
-        <v>278</v>
+      <c r="E57" s="53" t="s">
+        <v>270</v>
       </c>
       <c r="G57">
         <v>0.92</v>
@@ -3128,13 +3169,13 @@
         <v>1069</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="G58">
         <v>1078</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -3148,13 +3189,13 @@
         <v>1069</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="G59">
         <v>1072</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>46</v>
       </c>
@@ -3162,19 +3203,19 @@
         <v>152</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D60" s="2">
         <v>1069</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="G60">
         <v>1071</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>46</v>
       </c>
@@ -3188,27 +3229,27 @@
         <v>1069</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G61">
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>154</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D62" s="2">
         <v>1072</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G62">
         <v>0.93</v>
@@ -3222,19 +3263,19 @@
         <v>155</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D63" s="2">
         <v>1075</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="G63">
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>156</v>
       </c>
@@ -3245,13 +3286,13 @@
         <v>1075</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="G64" t="s">
-        <v>142</v>
+        <v>301</v>
+      </c>
+      <c r="G64" s="52">
+        <v>0.92</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3268,7 +3309,7 @@
         <v>1075</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="G65">
         <v>1078</v>
@@ -3288,30 +3329,33 @@
         <v>1075</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="G66">
         <v>1078</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>331</v>
+      </c>
       <c r="B67" s="1">
         <v>159</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D67" s="2">
         <v>1075</v>
       </c>
       <c r="E67" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="G67" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3319,36 +3363,36 @@
         <v>160</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D68" s="2">
         <v>1075</v>
       </c>
-      <c r="E68" s="57" t="s">
-        <v>303</v>
+      <c r="E68" s="56" t="s">
+        <v>294</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>161</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D69" s="2">
         <v>1075</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="G69" t="s">
-        <v>142</v>
+        <v>332</v>
+      </c>
+      <c r="G69">
+        <v>0.93</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3365,7 +3409,7 @@
         <v>1075</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="G70">
         <v>1078</v>
@@ -3381,11 +3425,14 @@
       <c r="D71" s="2">
         <v>1075</v>
       </c>
-      <c r="E71" s="54" t="s">
-        <v>308</v>
+      <c r="E71" s="53" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B72" s="1">
         <v>164</v>
       </c>
@@ -3396,7 +3443,7 @@
         <v>1079</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3410,37 +3457,87 @@
         <v>1079</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B74" s="1">
         <v>166</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="D74" s="2">
         <v>1079</v>
       </c>
       <c r="E74" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B75" s="1">
+        <v>167</v>
+      </c>
+      <c r="C75" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1081</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B76" s="1">
+        <v>168</v>
+      </c>
+      <c r="C76" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1081</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>326</v>
       </c>
     </row>
+    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
+        <v>169</v>
+      </c>
+      <c r="C77" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1081</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
+        <v>170</v>
+      </c>
+      <c r="C78" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1081</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G71" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="V"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters blank="1">
-        <filter val="0,92"/>
-        <filter val="1078"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A7:G74" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -3451,11 +3548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3464,7 +3560,7 @@
     <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="62" customWidth="1"/>
     <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
     <col min="8" max="16384" width="8.7109375" style="4"/>
@@ -3483,7 +3579,7 @@
       <c r="D1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="58" t="s">
         <v>116</v>
       </c>
       <c r="F1" s="34" t="s">
@@ -3493,7 +3589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="37" t="s">
         <v>42</v>
@@ -3504,14 +3600,16 @@
       <c r="D2" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="38" t="s">
-        <v>142</v>
+      <c r="E2" s="59">
+        <v>0.93</v>
       </c>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
+      <c r="A3" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="B3" s="37" t="s">
         <v>43</v>
       </c>
@@ -3519,17 +3617,17 @@
       <c r="D3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="51" t="s">
-        <v>208</v>
+      <c r="E3" s="60">
+        <v>0.92</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="37">
         <v>1075</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="102" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="37" t="s">
         <v>44</v>
@@ -3538,15 +3636,15 @@
       <c r="D4" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="59">
+        <v>0.93</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="37" t="s">
-        <v>144</v>
-      </c>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="B5" s="37" t="s">
         <v>64</v>
@@ -3557,13 +3655,13 @@
       <c r="D5" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="38" t="s">
-        <v>206</v>
+      <c r="E5" s="59">
+        <v>0.93</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -3574,13 +3672,13 @@
       <c r="D6" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>142</v>
+      <c r="E6" s="59">
+        <v>0.93</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -3593,12 +3691,14 @@
       <c r="D7" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="B8" s="37" t="s">
         <v>72</v>
       </c>
@@ -3608,17 +3708,17 @@
       <c r="D8" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="61" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="G8" s="37">
         <v>1078</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>46</v>
       </c>
@@ -3631,15 +3731,15 @@
       <c r="D9" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="38" t="s">
-        <v>208</v>
+      <c r="E9" s="59">
+        <v>0.92</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -3650,13 +3750,13 @@
       <c r="D10" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="38" t="s">
-        <v>142</v>
+      <c r="E10" s="59">
+        <v>0.93</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
     </row>
-    <row r="11" spans="1:7" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="37" t="s">
         <v>80</v>
@@ -3667,13 +3767,13 @@
       <c r="D11" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="38" t="s">
-        <v>142</v>
+      <c r="E11" s="59">
+        <v>0.93</v>
       </c>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -3684,13 +3784,13 @@
       <c r="D12" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="38" t="s">
-        <v>142</v>
+      <c r="E12" s="59">
+        <v>0.93</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
     </row>
-    <row r="13" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="36"/>
       <c r="B13" s="37" t="s">
         <v>87</v>
@@ -3701,13 +3801,13 @@
       <c r="D13" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="38" t="s">
-        <v>142</v>
+      <c r="E13" s="59">
+        <v>0.93</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -3718,13 +3818,13 @@
       <c r="D14" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="38" t="s">
-        <v>142</v>
+      <c r="E14" s="59">
+        <v>0.93</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -3735,13 +3835,13 @@
       <c r="D15" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="38" t="s">
-        <v>142</v>
+      <c r="E15" s="59">
+        <v>0.93</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
     </row>
-    <row r="16" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>46</v>
       </c>
@@ -3754,15 +3854,15 @@
       <c r="D16" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="38" t="s">
-        <v>208</v>
+      <c r="E16" s="59">
+        <v>0.92</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
       <c r="B17" s="37" t="s">
         <v>99</v>
@@ -3773,13 +3873,13 @@
       <c r="D17" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="38" t="s">
-        <v>142</v>
+      <c r="E17" s="59">
+        <v>0.93</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>46</v>
       </c>
@@ -3792,15 +3892,15 @@
       <c r="D18" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="61" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G18" s="37"/>
     </row>
-    <row r="19" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
       <c r="B19" s="37" t="s">
         <v>101</v>
@@ -3811,11 +3911,11 @@
       <c r="D19" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="38" t="s">
-        <v>142</v>
+      <c r="E19" s="59">
+        <v>0.93</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G19" s="37"/>
     </row>
@@ -3830,32 +3930,32 @@
       <c r="D20" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="38" t="s">
-        <v>208</v>
+      <c r="E20" s="59">
+        <v>0.92</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G20" s="37"/>
     </row>
-    <row r="21" spans="1:7" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
       <c r="B21" s="37" t="s">
         <v>103</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>142</v>
+        <v>231</v>
+      </c>
+      <c r="E21" s="59">
+        <v>0.93</v>
       </c>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
         <v>46</v>
       </c>
@@ -3868,15 +3968,15 @@
       <c r="D22" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="38" t="s">
-        <v>141</v>
+      <c r="E22" s="59">
+        <v>0.92</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>213</v>
+        <v>333</v>
       </c>
       <c r="G22" s="37"/>
     </row>
-    <row r="23" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>46</v>
       </c>
@@ -3889,13 +3989,13 @@
       <c r="D23" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G23" s="37"/>
     </row>
-    <row r="24" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>46</v>
       </c>
@@ -3908,124 +4008,124 @@
       <c r="D24" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="E24" s="38" t="s">
-        <v>208</v>
+      <c r="E24" s="59">
+        <v>0.92</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G24" s="37">
         <v>1039</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="37" t="s">
         <v>107</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>142</v>
+        <v>319</v>
+      </c>
+      <c r="E25" s="59">
+        <v>0.93</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>142</v>
+        <v>175</v>
+      </c>
+      <c r="E26" s="59">
+        <v>0.93</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="E27" s="38" t="s">
-        <v>142</v>
+        <v>177</v>
+      </c>
+      <c r="E27" s="59">
+        <v>0.93</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="37" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>208</v>
+        <v>179</v>
+      </c>
+      <c r="E28" s="59">
+        <v>0.92</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G28" s="37"/>
     </row>
-    <row r="29" spans="1:7" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A29" s="36"/>
       <c r="B29" s="37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>206</v>
+        <v>184</v>
+      </c>
+      <c r="E29" s="59">
+        <v>0.93</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G29" s="37"/>
     </row>
-    <row r="30" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
       <c r="B30" s="37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>296</v>
+        <v>188</v>
+      </c>
+      <c r="E30" s="59">
+        <v>0.95</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
@@ -4033,157 +4133,157 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" s="38" t="s">
-        <v>208</v>
+        <v>191</v>
+      </c>
+      <c r="E31" s="59">
+        <v>0.92</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="36"/>
       <c r="B32" s="37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>201</v>
-      </c>
-      <c r="E32" s="38"/>
+        <v>198</v>
+      </c>
+      <c r="E32" s="61"/>
       <c r="F32" s="37"/>
       <c r="G32" s="37"/>
     </row>
-    <row r="33" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A33" s="36"/>
       <c r="B33" s="37" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>142</v>
+        <v>221</v>
+      </c>
+      <c r="E33" s="59">
+        <v>0.93</v>
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
     </row>
-    <row r="34" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
       <c r="B34" s="37" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C34" s="37" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>142</v>
+        <v>212</v>
+      </c>
+      <c r="E34" s="59">
+        <v>0.93</v>
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="37"/>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C35" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>142</v>
+        <v>238</v>
+      </c>
+      <c r="E35" s="59">
+        <v>0.93</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
     </row>
-    <row r="36" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A36" s="36"/>
       <c r="B36" s="37" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>258</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>142</v>
+        <v>250</v>
+      </c>
+      <c r="E36" s="59">
+        <v>0.93</v>
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
     </row>
-    <row r="37" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="36"/>
       <c r="B37" s="37" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>260</v>
-      </c>
-      <c r="E37" s="38" t="s">
-        <v>142</v>
+        <v>252</v>
+      </c>
+      <c r="E37" s="59">
+        <v>0.93</v>
       </c>
       <c r="F37" s="37"/>
       <c r="G37" s="37"/>
     </row>
-    <row r="38" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" s="36"/>
       <c r="B38" s="37" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>261</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>142</v>
+        <v>253</v>
+      </c>
+      <c r="E38" s="59">
+        <v>0.93</v>
       </c>
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
     </row>
     <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="F39" s="52" t="s">
-        <v>284</v>
+        <v>255</v>
+      </c>
+      <c r="E39" s="59">
+        <v>0.92</v>
+      </c>
+      <c r="F39" s="51" t="s">
+        <v>276</v>
       </c>
       <c r="G39" s="4">
         <v>1078</v>
@@ -4191,205 +4291,229 @@
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>142</v>
+        <v>196</v>
+      </c>
+      <c r="E41" s="59">
+        <v>0.93</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>274</v>
-      </c>
       <c r="D42" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>208</v>
+        <v>159</v>
+      </c>
+      <c r="E42" s="59">
+        <v>0.92</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="E43" s="38" t="s">
-        <v>208</v>
+        <v>182</v>
+      </c>
+      <c r="E43" s="59">
+        <v>0.92</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E44" s="38" t="s">
-        <v>208</v>
+        <v>195</v>
+      </c>
+      <c r="E44" s="59">
+        <v>0.92</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="E45" s="38" t="s">
-        <v>208</v>
+        <v>189</v>
+      </c>
+      <c r="E45" s="59">
+        <v>0.92</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="E46" s="38" t="s">
-        <v>208</v>
+        <v>280</v>
+      </c>
+      <c r="E46" s="59">
+        <v>0.92</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="E47" s="38" t="s">
-        <v>208</v>
+        <v>193</v>
+      </c>
+      <c r="E47" s="59">
+        <v>0.92</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="E48" s="38" t="s">
-        <v>208</v>
+        <v>284</v>
+      </c>
+      <c r="E48" s="59">
+        <v>0.92</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
+        <v>331</v>
+      </c>
       <c r="B49" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="B51" s="4" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D51" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G49" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="V"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters blank="1">
-        <filter val="0,92"/>
-        <filter val="0.92"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G56" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -4425,15 +4549,15 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
+      <c r="B2" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>
@@ -4448,19 +4572,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E4" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="43" t="s">
         <v>151</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>153</v>
       </c>
       <c r="H4" s="44" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Updated suggestions with WGET/IFTTT and updating PK floppy just in case.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00628A7-CAF0-4734-BECA-DBF8DC5708D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F8D32-8BB7-4806-A386-C2B8DC9F143B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="347">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1159,6 +1159,24 @@
   </si>
   <si>
     <t>Create a TCUTIL to set the time on a thunderclock that mirrors the function of the NSCUTIL program.</t>
+  </si>
+  <si>
+    <t>S0056</t>
+  </si>
+  <si>
+    <t>WGET</t>
+  </si>
+  <si>
+    <t>Make a utility that will perfrom a wget to the internet using StdIn as URL and StdOut as returned result.  Option should include -F filename for taking input from a file (output redirection of &gt; should work).  Return codes should be set for invalid URL, DNS unresolved, empty return set or other things I make up).  Max URL length is 2048 chars.  Return results could be any length and multipart, how do we handle?</t>
+  </si>
+  <si>
+    <t>S0057</t>
+  </si>
+  <si>
+    <t>IFTTT</t>
+  </si>
+  <si>
+    <t>Write a script to build IFTTT actions to submit via WGET.  We will need to handle $EVENT, $KEYm and 3 Values ($VALUE1-$VALUE3) with the full URL being http://maker.ifttt.com/trigger/$EVENT/with/key/$KEY?value1=$VALUE1&amp;value2=VALUE2&amp;value3=VALUE3.</t>
   </si>
 </sst>
 </file>
@@ -1934,7 +1952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
@@ -3581,10 +3599,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4549,6 +4567,28 @@
       </c>
       <c r="D56" s="4" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with quick testing of open issues for 1100. Closed many with notes.  Look for highlighted (bright yellow) notes.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F8D32-8BB7-4806-A386-C2B8DC9F143B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0B347B-2B21-4DEA-BBB5-A1498F641B69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="354">
   <si>
     <t>Issue No.</t>
   </si>
@@ -397,9 +397,6 @@
   </si>
   <si>
     <t>Verified in latest.  Boot, -run, at prompt EDIT A.  Then type some stuff, then ctrl-S  PRESS ESCAPE and then type aaa and return.  Error 40</t>
-  </si>
-  <si>
-    <t>Which NIC/Driver ? -RG This is on AppleWin using NET script.  I need to test this on a real Apple, it may be the Eth driver in AppleWin is reporting it wrong to you. -PK</t>
   </si>
   <si>
     <t>HT</t>
@@ -831,10 +828,6 @@
 CP,MV,RM should also be impacted</t>
   </si>
   <si>
-    <t>Beware of bad VBL emulation in Applewin
-should be flagged HT</t>
-  </si>
-  <si>
     <t>side note : Applewin does not allow Writing to NSC
 should be flagged HT</t>
   </si>
@@ -1177,6 +1170,33 @@
   </si>
   <si>
     <t>Write a script to build IFTTT actions to submit via WGET.  We will need to handle $EVENT, $KEYm and 3 Values ($VALUE1-$VALUE3) with the full URL being http://maker.ifttt.com/trigger/$EVENT/with/key/$KEY?value1=$VALUE1&amp;value2=VALUE2&amp;value3=VALUE3.</t>
+  </si>
+  <si>
+    <t>Fixed!</t>
+  </si>
+  <si>
+    <t>Link Status on real HW reports OK, AW does not report it correctly, will make note in our Doc.  Not a bug. Closed.</t>
+  </si>
+  <si>
+    <t>Confirmed behavior on both read Hardware (Apple //e U2 card) and AW. Happens with both local hosts and internet.  Behavior not consistent.</t>
+  </si>
+  <si>
+    <t>Closing.  Thought to be related to bad media or sector order problems on media.  If reoccurs, will try format/recopy files and test again.</t>
+  </si>
+  <si>
+    <t>Can no longer duplicated problem after DEL change.</t>
+  </si>
+  <si>
+    <t>S0058</t>
+  </si>
+  <si>
+    <t>It you have made changes to a file and Quite, Edit should warn you that you have not saved and kill you a Cancel Quit, Save Changes, Quit Anyways option.</t>
+  </si>
+  <si>
+    <t>When I telnet to linux, when session starts it is already asking me for my password as Telnet has sent a CR/LF or whatever and pushed me passed the login prompt.  Yes you can just press return and get another one.</t>
+  </si>
+  <si>
+    <t>No longer get error, but return code is not right.  Test RCTEST which calls RCSUB1 and RCSUB2, RCTEST should get the return codes, it only gets 0.</t>
   </si>
 </sst>
 </file>
@@ -1601,9 +1621,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1635,6 +1652,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1950,10 +1970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,10 +2019,10 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="14"/>
@@ -2163,9 +2183,9 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
@@ -2181,7 +2201,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>121</v>
+        <v>346</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
@@ -2314,7 +2334,7 @@
         <v>32</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G19">
         <v>1039</v>
@@ -2404,7 +2424,7 @@
         <v>48</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -2425,7 +2445,7 @@
         <v>1016</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24">
@@ -2450,7 +2470,7 @@
         <v>49</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G25">
         <v>1034</v>
@@ -2495,7 +2515,7 @@
         <v>51</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G27">
         <v>0.93</v>
@@ -2543,7 +2563,7 @@
         <v>59</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G29">
         <v>1020</v>
@@ -2567,7 +2587,7 @@
         <v>117</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G30">
         <v>1069</v>
@@ -2588,7 +2608,7 @@
         <v>1027</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G31">
         <v>0.93</v>
@@ -2609,10 +2629,10 @@
         <v>1027</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G32">
         <v>0.93</v>
@@ -2627,16 +2647,16 @@
         <v>125</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D33" s="2">
         <v>1027</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G33" t="s">
         <v>28</v>
@@ -2651,16 +2671,16 @@
         <v>126</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D34" s="2">
         <v>1027</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G34" t="s">
         <v>28</v>
@@ -2675,16 +2695,16 @@
         <v>127</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D35" s="2">
         <v>1034</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="G35" t="s">
         <v>28</v>
@@ -2692,20 +2712,23 @@
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="B36" s="1">
         <f t="shared" ref="B36:B57" si="1">B35+1</f>
         <v>128</v>
       </c>
       <c r="C36" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="G36" t="s">
-        <v>28</v>
+      <c r="F36" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G36">
+        <v>0.92</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2723,10 +2746,10 @@
         <v>1034</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G37">
         <v>1039</v>
@@ -2741,18 +2764,18 @@
         <v>130</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D38" s="2">
         <v>1034</v>
       </c>
-      <c r="E38" s="55" t="s">
-        <v>227</v>
+      <c r="E38" s="54" t="s">
+        <v>226</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="G38" s="52">
+        <v>201</v>
+      </c>
+      <c r="G38" s="51">
         <v>0.92</v>
       </c>
     </row>
@@ -2771,10 +2794,10 @@
         <v>1037</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G39">
         <v>1050</v>
@@ -2789,13 +2812,13 @@
         <v>132</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D40" s="2">
         <v>1037</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G40">
         <v>1047</v>
@@ -2810,18 +2833,18 @@
         <v>133</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D41" s="2">
         <v>1047</v>
       </c>
-      <c r="E41" s="39" t="s">
-        <v>224</v>
+      <c r="E41" s="48" t="s">
+        <v>223</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="G41" s="54">
+        <v>272</v>
+      </c>
+      <c r="G41" s="53">
         <v>1079</v>
       </c>
     </row>
@@ -2834,13 +2857,13 @@
         <v>134</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D42" s="2">
         <v>1047</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G42">
         <v>0.93</v>
@@ -2861,10 +2884,10 @@
         <v>1047</v>
       </c>
       <c r="E43" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F43" s="48" t="s">
         <v>225</v>
-      </c>
-      <c r="F43" s="39" t="s">
-        <v>226</v>
       </c>
       <c r="G43" t="s">
         <v>28</v>
@@ -2872,7 +2895,7 @@
     </row>
     <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="1"/>
@@ -2885,31 +2908,31 @@
         <v>1047</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F44" s="48" t="s">
-        <v>245</v>
+        <v>212</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" si="1"/>
         <v>137</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D45" s="2">
         <v>1047</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F45" s="48" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G45">
         <v>1050</v>
@@ -2930,10 +2953,10 @@
         <v>1047</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F46" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G46">
         <v>1050</v>
@@ -2948,16 +2971,16 @@
         <v>139</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D47" s="2">
         <v>1047</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F47" s="48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G47">
         <v>1050</v>
@@ -2965,7 +2988,7 @@
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" si="1"/>
@@ -2978,7 +3001,10 @@
         <v>1047</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>348</v>
       </c>
       <c r="G48">
         <v>0.93</v>
@@ -2993,22 +3019,22 @@
         <v>141</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D49" s="2">
         <v>1047</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="F49" s="50" t="s">
-        <v>324</v>
+        <v>218</v>
+      </c>
+      <c r="F49" s="62" t="s">
+        <v>322</v>
       </c>
       <c r="G49">
         <v>0.93</v>
       </c>
       <c r="H49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3026,13 +3052,13 @@
         <v>1047</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F50" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="G50" t="s">
         <v>242</v>
-      </c>
-      <c r="G50" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -3044,16 +3070,16 @@
         <v>143</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D51" s="2">
         <v>1047</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F51" s="48" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G51">
         <v>1050</v>
@@ -3068,16 +3094,16 @@
         <v>144</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D52" s="2">
         <v>1047</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G52">
         <v>0.93</v>
@@ -3092,13 +3118,13 @@
         <v>145</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D53" s="2">
         <v>1047</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3116,13 +3142,13 @@
         <v>1047</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="F54" s="39" t="s">
-        <v>277</v>
+        <v>238</v>
+      </c>
+      <c r="F54" s="48" t="s">
+        <v>275</v>
       </c>
       <c r="H54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -3139,10 +3165,10 @@
       <c r="D55" s="2">
         <v>1069</v>
       </c>
-      <c r="E55" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="G55" s="54">
+      <c r="E55" s="48" t="s">
+        <v>266</v>
+      </c>
+      <c r="G55" s="53">
         <v>1079</v>
       </c>
     </row>
@@ -3161,13 +3187,16 @@
         <v>1069</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G56">
         <v>1078</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B57" s="1">
         <f t="shared" si="1"/>
         <v>149</v>
@@ -3178,8 +3207,11 @@
       <c r="D57" s="2">
         <v>1069</v>
       </c>
-      <c r="E57" s="53" t="s">
-        <v>270</v>
+      <c r="E57" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="F57" s="39" t="s">
+        <v>349</v>
       </c>
       <c r="G57">
         <v>0.92</v>
@@ -3199,7 +3231,7 @@
         <v>1069</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G58">
         <v>1078</v>
@@ -3219,7 +3251,7 @@
         <v>1069</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G59">
         <v>1072</v>
@@ -3233,13 +3265,13 @@
         <v>152</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D60" s="2">
         <v>1069</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G60">
         <v>1071</v>
@@ -3259,27 +3291,30 @@
         <v>1069</v>
       </c>
       <c r="E61" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="G61">
         <v>1071</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B62" s="1">
         <v>154</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D62" s="2">
         <v>1072</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G62">
         <v>0.93</v>
@@ -3293,19 +3328,22 @@
         <v>155</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D63" s="2">
         <v>1075</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G63">
         <v>1078</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B64" s="1">
         <v>156</v>
       </c>
@@ -3316,12 +3354,12 @@
         <v>1075</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="G64" s="52">
+        <v>299</v>
+      </c>
+      <c r="G64" s="51">
         <v>0.92</v>
       </c>
     </row>
@@ -3339,7 +3377,7 @@
         <v>1075</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G65">
         <v>1078</v>
@@ -3359,7 +3397,7 @@
         <v>1075</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G66">
         <v>1078</v>
@@ -3367,25 +3405,25 @@
     </row>
     <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B67" s="1">
         <v>159</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D67" s="2">
         <v>1075</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3393,16 +3431,16 @@
         <v>160</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D68" s="2">
         <v>1075</v>
       </c>
-      <c r="E68" s="56" t="s">
-        <v>294</v>
+      <c r="E68" s="55" t="s">
+        <v>292</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3410,16 +3448,16 @@
         <v>161</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D69" s="2">
         <v>1075</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G69">
         <v>0.93</v>
@@ -3439,7 +3477,7 @@
         <v>1075</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G70">
         <v>1078</v>
@@ -3455,8 +3493,8 @@
       <c r="D71" s="2">
         <v>1075</v>
       </c>
-      <c r="E71" s="53" t="s">
-        <v>299</v>
+      <c r="E71" s="52" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3473,10 +3511,13 @@
         <v>1079</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B73" s="1">
         <v>165</v>
       </c>
@@ -3486,8 +3527,8 @@
       <c r="D73" s="2">
         <v>1079</v>
       </c>
-      <c r="E73" s="53" t="s">
-        <v>313</v>
+      <c r="E73" s="52" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3498,16 +3539,19 @@
         <v>166</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D74" s="2">
         <v>1079</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B75" s="1">
         <v>167</v>
       </c>
@@ -3517,11 +3561,14 @@
       <c r="D75" s="2">
         <v>1081</v>
       </c>
-      <c r="E75" s="53" t="s">
-        <v>325</v>
+      <c r="E75" s="52" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B76" s="1">
         <v>168</v>
       </c>
@@ -3531,11 +3578,14 @@
       <c r="D76" s="2">
         <v>1081</v>
       </c>
-      <c r="E76" s="53" t="s">
-        <v>326</v>
+      <c r="E76" s="48" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B77" s="1">
         <v>169</v>
       </c>
@@ -3546,44 +3596,67 @@
         <v>1081</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G77">
         <v>1085</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B78" s="1">
         <v>170</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D78" s="2">
         <v>1081</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
+      </c>
+      <c r="F78" s="39" t="s">
+        <v>353</v>
       </c>
       <c r="G78">
         <v>1100</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B79" s="1">
         <v>171</v>
       </c>
       <c r="C79" s="27" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D79" s="2">
         <v>1085</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B80" s="1">
+        <v>171</v>
+      </c>
+      <c r="C80" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3599,10 +3672,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3611,7 +3684,7 @@
     <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="60" customWidth="1"/>
     <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
     <col min="8" max="16384" width="8.7109375" style="4"/>
@@ -3630,7 +3703,7 @@
       <c r="D1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>116</v>
       </c>
       <c r="F1" s="34" t="s">
@@ -3651,7 +3724,7 @@
       <c r="D2" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="58">
+      <c r="E2" s="57">
         <v>0.93</v>
       </c>
       <c r="F2" s="37"/>
@@ -3668,11 +3741,11 @@
       <c r="D3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="58">
         <v>0.92</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G3" s="37">
         <v>1075</v>
@@ -3687,11 +3760,11 @@
       <c r="D4" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="57">
         <v>0.93</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G4" s="37"/>
     </row>
@@ -3706,7 +3779,7 @@
       <c r="D5" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="57">
         <v>0.93</v>
       </c>
       <c r="F5" s="37"/>
@@ -3723,7 +3796,7 @@
       <c r="D6" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="57">
         <v>0.93</v>
       </c>
       <c r="F6" s="37"/>
@@ -3742,7 +3815,7 @@
       <c r="D7" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="59"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
@@ -3759,11 +3832,11 @@
       <c r="D8" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="59" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G8" s="37">
         <v>1078</v>
@@ -3782,11 +3855,11 @@
       <c r="D9" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="57">
         <v>0.92</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G9" s="37"/>
     </row>
@@ -3801,7 +3874,7 @@
       <c r="D10" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="57">
         <v>0.93</v>
       </c>
       <c r="F10" s="37"/>
@@ -3818,7 +3891,7 @@
       <c r="D11" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="57">
         <v>0.93</v>
       </c>
       <c r="F11" s="37"/>
@@ -3835,7 +3908,7 @@
       <c r="D12" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="57">
         <v>0.93</v>
       </c>
       <c r="F12" s="37"/>
@@ -3852,7 +3925,7 @@
       <c r="D13" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="57">
         <v>0.93</v>
       </c>
       <c r="F13" s="37"/>
@@ -3869,7 +3942,7 @@
       <c r="D14" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="58">
+      <c r="E14" s="57">
         <v>0.93</v>
       </c>
       <c r="F14" s="37"/>
@@ -3886,7 +3959,7 @@
       <c r="D15" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="57">
         <v>0.93</v>
       </c>
       <c r="F15" s="37"/>
@@ -3905,11 +3978,11 @@
       <c r="D16" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="57">
         <v>0.92</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G16" s="37"/>
     </row>
@@ -3924,7 +3997,7 @@
       <c r="D17" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="57">
         <v>0.93</v>
       </c>
       <c r="F17" s="37"/>
@@ -3943,11 +4016,11 @@
       <c r="D18" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="59" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G18" s="37"/>
     </row>
@@ -3962,11 +4035,11 @@
       <c r="D19" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="57">
         <v>0.93</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G19" s="37"/>
     </row>
@@ -3976,16 +4049,16 @@
         <v>102</v>
       </c>
       <c r="C20" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="58">
+      <c r="E20" s="57">
         <v>0.92</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G20" s="37"/>
     </row>
@@ -3995,12 +4068,12 @@
         <v>103</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="E21" s="58">
+        <v>230</v>
+      </c>
+      <c r="E21" s="57">
         <v>0.93</v>
       </c>
       <c r="F21" s="37"/>
@@ -4014,16 +4087,16 @@
         <v>104</v>
       </c>
       <c r="C22" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="E22" s="58">
+      <c r="E22" s="57">
         <v>0.92</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G22" s="37"/>
     </row>
@@ -4035,14 +4108,14 @@
         <v>105</v>
       </c>
       <c r="C23" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E23" s="60"/>
+      <c r="E23" s="59"/>
       <c r="F23" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G23" s="37"/>
     </row>
@@ -4054,16 +4127,16 @@
         <v>106</v>
       </c>
       <c r="C24" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="58">
+      <c r="E24" s="57">
         <v>0.92</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G24" s="37">
         <v>1039</v>
@@ -4075,16 +4148,16 @@
         <v>107</v>
       </c>
       <c r="C25" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="E25" s="57">
+        <v>0.93</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>160</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>319</v>
-      </c>
-      <c r="E25" s="58">
-        <v>0.93</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>161</v>
       </c>
       <c r="G25" s="37"/>
     </row>
@@ -4094,88 +4167,88 @@
         <v>108</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="E26" s="58">
+        <v>174</v>
+      </c>
+      <c r="E26" s="57">
         <v>0.93</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G26" s="37"/>
     </row>
     <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="D27" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="58">
+      <c r="E27" s="57">
         <v>0.93</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="D28" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="E28" s="58">
+      <c r="E28" s="57">
         <v>0.92</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G28" s="37"/>
     </row>
     <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A29" s="36"/>
       <c r="B29" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C29" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="E29" s="58">
+      <c r="E29" s="57">
         <v>0.93</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
       <c r="B30" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="D30" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="E30" s="58">
+      <c r="E30" s="57">
         <v>0.95</v>
       </c>
       <c r="F30" s="37"/>
@@ -4184,49 +4257,49 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="E31" s="57">
+        <v>0.92</v>
+      </c>
+      <c r="F31" s="37" t="s">
         <v>191</v>
-      </c>
-      <c r="E31" s="58">
-        <v>0.92</v>
-      </c>
-      <c r="F31" s="37" t="s">
-        <v>192</v>
       </c>
       <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="36"/>
       <c r="B32" s="37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="D32" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="E32" s="60"/>
+      <c r="E32" s="59"/>
       <c r="F32" s="37"/>
       <c r="G32" s="37"/>
     </row>
     <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A33" s="36"/>
       <c r="B33" s="37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C33" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="D33" s="37" t="s">
-        <v>221</v>
-      </c>
-      <c r="E33" s="58">
+      <c r="E33" s="57">
         <v>0.93</v>
       </c>
       <c r="F33" s="37"/>
@@ -4235,15 +4308,15 @@
     <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
       <c r="B34" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34" s="37" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="E34" s="58">
+        <v>211</v>
+      </c>
+      <c r="E34" s="57">
         <v>0.93</v>
       </c>
       <c r="F34" s="37"/>
@@ -4252,15 +4325,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C35" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="E35" s="58">
+        <v>237</v>
+      </c>
+      <c r="E35" s="57">
         <v>0.93</v>
       </c>
       <c r="F35" s="37"/>
@@ -4269,15 +4342,15 @@
     <row r="36" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A36" s="36"/>
       <c r="B36" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="E36" s="58">
+        <v>248</v>
+      </c>
+      <c r="E36" s="57">
         <v>0.93</v>
       </c>
       <c r="F36" s="37"/>
@@ -4286,15 +4359,15 @@
     <row r="37" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="36"/>
       <c r="B37" s="37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>252</v>
-      </c>
-      <c r="E37" s="58">
+        <v>250</v>
+      </c>
+      <c r="E37" s="57">
         <v>0.93</v>
       </c>
       <c r="F37" s="37"/>
@@ -4303,15 +4376,15 @@
     <row r="38" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" s="36"/>
       <c r="B38" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>253</v>
-      </c>
-      <c r="E38" s="58">
+        <v>251</v>
+      </c>
+      <c r="E38" s="57">
         <v>0.93</v>
       </c>
       <c r="F38" s="37"/>
@@ -4322,19 +4395,19 @@
         <v>46</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E39" s="58">
+        <v>253</v>
+      </c>
+      <c r="E39" s="57">
         <v>0.92</v>
       </c>
-      <c r="F39" s="51" t="s">
-        <v>276</v>
+      <c r="F39" s="50" t="s">
+        <v>274</v>
       </c>
       <c r="G39" s="4">
         <v>1078</v>
@@ -4342,156 +4415,156 @@
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E41" s="58">
+        <v>195</v>
+      </c>
+      <c r="E41" s="57">
         <v>0.93</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="E42" s="58">
+        <v>158</v>
+      </c>
+      <c r="E42" s="57">
         <v>0.92</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="E43" s="58">
+        <v>181</v>
+      </c>
+      <c r="E43" s="57">
         <v>0.92</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E44" s="58">
+        <v>194</v>
+      </c>
+      <c r="E44" s="57">
         <v>0.92</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="E45" s="58">
+        <v>188</v>
+      </c>
+      <c r="E45" s="57">
         <v>0.92</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>280</v>
-      </c>
-      <c r="E46" s="58">
+        <v>278</v>
+      </c>
+      <c r="E46" s="57">
         <v>0.92</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E47" s="58">
+        <v>192</v>
+      </c>
+      <c r="E47" s="57">
         <v>0.92</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>266</v>
-      </c>
       <c r="D48" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="E48" s="58">
+        <v>282</v>
+      </c>
+      <c r="E48" s="57">
         <v>0.92</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
@@ -4499,16 +4572,16 @@
         <v>46</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4516,79 +4589,90 @@
         <v>46</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>346</v>
+    </row>
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -4634,15 +4718,15 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="62" t="s">
-        <v>267</v>
-      </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
+      <c r="B2" s="61" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>
@@ -4657,19 +4741,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="43" t="s">
-        <v>157</v>
-      </c>
       <c r="E4" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="G4" s="43" t="s">
         <v>150</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>151</v>
       </c>
       <c r="H4" s="44" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Added DNSINFO bug, READ suggestion.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0B347B-2B21-4DEA-BBB5-A1498F641B69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421FF9A2-3CC9-4919-BEA4-5EBD74D493D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="362">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1197,6 +1197,30 @@
   </si>
   <si>
     <t>No longer get error, but return code is not right.  Test RCTEST which calls RCSUB1 and RCSUB2, RCTEST should get the return codes, it only gets 0.</t>
+  </si>
+  <si>
+    <t>License file added to Github, GNU GPL 2.0</t>
+  </si>
+  <si>
+    <t>S0059</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>Create standard Copyright Slug that should go as a comment at the top of all Source Files, Scripts, Documentation or other public facing files.  Follow up to S0027 (license).</t>
+  </si>
+  <si>
+    <t>-RUN, then NET.  DNSINFO host ip then DNSINFO again and it lists host and then starts scrolling non stop a whole bunch of what looks like a memory dump filled with IP addresses.</t>
+  </si>
+  <si>
+    <t>READ</t>
+  </si>
+  <si>
+    <t>S0060</t>
+  </si>
+  <si>
+    <t>Add an option to READ -L 22 that limits the length of the input to arg for -L, in this example only allow for 22 chars.</t>
   </si>
 </sst>
 </file>
@@ -1650,11 +1674,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1970,10 +1994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3027,7 +3051,7 @@
       <c r="E49" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="F49" s="62" t="s">
+      <c r="F49" s="61" t="s">
         <v>322</v>
       </c>
       <c r="G49">
@@ -3657,6 +3681,25 @@
       </c>
       <c r="E80" s="3" t="s">
         <v>352</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
+        <v>172</v>
+      </c>
+      <c r="C81" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="1">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3672,10 +3715,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4200,7 +4243,9 @@
       <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="B28" s="37" t="s">
         <v>163</v>
       </c>
@@ -4214,7 +4259,7 @@
         <v>0.92</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>160</v>
+        <v>354</v>
       </c>
       <c r="G28" s="37"/>
     </row>
@@ -4673,6 +4718,28 @@
       </c>
       <c r="D59" s="4" t="s">
         <v>351</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -4718,15 +4785,15 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="62" t="s">
         <v>265</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
New issues and suggestions.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92486D8-F92E-46E6-9C15-43159EB18AC4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$82</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$56</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="367">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1216,11 +1222,26 @@
   <si>
     <t>Add an option to READ -L 22 that limits the length of the input to arg for -L, in this example only allow for 22 chars.</t>
   </si>
+  <si>
+    <t>S0061</t>
+  </si>
+  <si>
+    <t>VEDRIVE</t>
+  </si>
+  <si>
+    <t>ADTPRO can serve up 2 images to an Apple which can connect to them through Ether or SSC.  VEDRIVE is the ether version.  Would it be possible to write our own driver that used the ADTPRO spec but written on top of our net apis to do the same.</t>
+  </si>
+  <si>
+    <t>Control-C to erase command line does not erase the right characters depending where on the line you are when you press it (I think it assumes you are always at the end and you may not be).</t>
+  </si>
+  <si>
+    <t>Cp filename1 filename2, no message and no file copied.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1980,34 +2001,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -2022,7 +2043,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -2035,7 +2056,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>121</v>
@@ -2048,7 +2069,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>53</v>
@@ -2061,12 +2082,12 @@
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -2089,7 +2110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2110,7 +2131,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2132,7 +2153,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -2154,7 +2175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2267,7 +2288,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2335,7 +2356,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2359,7 +2380,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2381,7 +2402,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -2403,7 +2424,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="217.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -2449,7 +2470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2471,7 +2492,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2516,7 +2537,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2540,7 +2561,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2612,7 +2633,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2633,7 +2654,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -2774,7 +2795,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
@@ -2798,7 +2819,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -2867,7 +2888,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2888,7 +2909,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -2912,7 +2933,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -2933,7 +2954,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>121</v>
       </c>
@@ -2981,7 +3002,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -3029,7 +3050,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -3056,7 +3077,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
@@ -3104,7 +3125,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -3236,7 +3257,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>46</v>
       </c>
@@ -3319,7 +3340,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>53</v>
       </c>
@@ -3339,7 +3360,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>46</v>
       </c>
@@ -3359,7 +3380,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>53</v>
       </c>
@@ -3382,7 +3403,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>46</v>
       </c>
@@ -3402,7 +3423,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>46</v>
       </c>
@@ -3422,7 +3443,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>329</v>
       </c>
@@ -3445,7 +3466,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>160</v>
       </c>
@@ -3462,7 +3483,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>161</v>
       </c>
@@ -3482,7 +3503,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -3502,7 +3523,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>163</v>
       </c>
@@ -3516,7 +3537,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>46</v>
       </c>
@@ -3533,7 +3554,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>53</v>
       </c>
@@ -3550,7 +3571,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>46</v>
       </c>
@@ -3567,7 +3588,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>53</v>
       </c>
@@ -3584,7 +3605,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>46</v>
       </c>
@@ -3624,7 +3645,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>53</v>
       </c>
@@ -3647,7 +3668,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -3664,7 +3685,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
         <v>171</v>
       </c>
@@ -3678,7 +3699,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B81" s="1">
         <v>172</v>
       </c>
@@ -3692,13 +3713,36 @@
         <v>358</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
         <v>173</v>
       </c>
+      <c r="C82" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B83" s="1">
+        <v>174</v>
+      </c>
+      <c r="C83" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>366</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G82">
+  <autoFilter ref="A7:G82" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -3715,24 +3759,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="60" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3830,7 +3874,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -3847,7 +3891,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -3908,7 +3952,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -3942,7 +3986,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -3976,7 +4020,7 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -3993,7 +4037,7 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -4206,7 +4250,7 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
@@ -4225,7 +4269,7 @@
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
         <v>162</v>
@@ -4244,7 +4288,7 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>46</v>
       </c>
@@ -4301,7 +4345,7 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>166</v>
@@ -4352,7 +4396,7 @@
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
     </row>
-    <row r="34" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
       <c r="B34" s="37" t="s">
         <v>169</v>
@@ -4371,7 +4415,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
         <v>170</v>
@@ -4532,7 +4576,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>259</v>
       </c>
@@ -4633,7 +4677,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>46</v>
       </c>
@@ -4658,7 +4702,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>306</v>
       </c>
@@ -4724,7 +4768,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
         <v>355</v>
       </c>
@@ -4735,7 +4779,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>360</v>
       </c>
@@ -4746,8 +4790,19 @@
         <v>361</v>
       </c>
     </row>
+    <row r="62" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G56">
+  <autoFilter ref="A1:G56" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="D"/>
@@ -4763,27 +4818,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="41"/>
-    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="41"/>
-    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="41"/>
+    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="41"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
@@ -4802,12 +4857,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I3" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
@@ -4833,7 +4888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="45"/>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -4844,529 +4899,529 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="I6" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="I8" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="I9" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="46"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="46"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="47"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="47"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="47"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="47"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="47"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="47"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Issue/Suggestion Sheet.  Updated PK floppy.  Added new MAKE HD image.  This is the staging area for combining BUILD and TEST and including MAN and HELP.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC760D8-303D-49FD-ABE8-8290126DB897}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
     <sheet name="Suggestions" sheetId="2" r:id="rId2"/>
     <sheet name="Commands" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$83</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="401">
   <si>
     <t>Issue No.</t>
   </si>
@@ -532,9 +539,6 @@
     <t>Doc.</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>We need a document that discusses the tools and processes one uses to work on the A2OSX project.  Examples include the TortoiseSVN package to contribute, MarkDownPad to edit MD and other DOC files on github.  Github tools and registration.  How to edit, compile and run a program under A2OSX.</t>
   </si>
   <si>
@@ -1190,9 +1194,6 @@
     <t>When I telnet to linux, when session starts it is already asking me for my password as Telnet has sent a CR/LF or whatever and pushed me passed the login prompt.  Yes you can just press return and get another one.</t>
   </si>
   <si>
-    <t>No longer get error, but return code is not right.  Test RCTEST which calls RCSUB1 and RCSUB2, RCTEST should get the return codes, it only gets 0.</t>
-  </si>
-  <si>
     <t>License file added to Github, GNU GPL 2.0</t>
   </si>
   <si>
@@ -1247,11 +1248,107 @@
   <si>
     <t>see impact in RCTEST</t>
   </si>
+  <si>
+    <t>S0062</t>
+  </si>
+  <si>
+    <t>Add SET -E option to continute on error in scripts (implies hiding error ptr) and not display 3 error lines and with out -E shell should print error msgs and STOP executing script.  Current behavior is it both prints errors and continues execution.</t>
+  </si>
+  <si>
+    <t>S0063</t>
+  </si>
+  <si>
+    <t>Console</t>
+  </si>
+  <si>
+    <t>Can we add the \a or bell special char so we can ECHO "\a" a bell per the VT100 standard?  Is this a big thing (lot of code or a simple apple call)?</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CD return code not set properly with success, it is set right on errors.</t>
+  </si>
+  <si>
+    <t>see CDTEST</t>
+  </si>
+  <si>
+    <t>Memory Check Sheet</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Free Ptr</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Avail</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Aux</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>$2000</t>
+  </si>
+  <si>
+    <t>$86E0</t>
+  </si>
+  <si>
+    <t>$BD00</t>
+  </si>
+  <si>
+    <t>26336</t>
+  </si>
+  <si>
+    <t>$9800</t>
+  </si>
+  <si>
+    <t>30720</t>
+  </si>
+  <si>
+    <t>$ED5C</t>
+  </si>
+  <si>
+    <t>$F459</t>
+  </si>
+  <si>
+    <t>$FFFA</t>
+  </si>
+  <si>
+    <t>02977</t>
+  </si>
+  <si>
+    <t>S0064</t>
+  </si>
+  <si>
+    <t>Tweak</t>
+  </si>
+  <si>
+    <t>Rename A2OSX.BUILD to just A2OSX or BUILD, it saves memory and shortens PATH.  Move files in BIN/DEV to BIN and remove BIN/DEV from PATH (done in INIT).  Add USR/BIN to PATH (for User Scripts and programs).</t>
+  </si>
+  <si>
+    <t>S0065</t>
+  </si>
+  <si>
+    <t>Get rid of $LIB and $DRV. Make programs that rely on those vars look at ${ROOT}LIB/ or DRV/.  This will save ENV space which is limited.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1531,7 +1628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1705,16 +1802,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2023,34 +2123,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -2065,7 +2164,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -2078,7 +2177,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>121</v>
@@ -2091,7 +2190,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>53</v>
@@ -2104,12 +2203,12 @@
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -2132,7 +2231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2153,7 +2252,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2175,7 +2274,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -2197,7 +2296,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2221,7 +2320,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -2245,7 +2344,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -2263,13 +2362,13 @@
         <v>16</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -2291,7 +2390,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -2310,7 +2409,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2332,7 +2431,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -2356,7 +2455,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -2378,7 +2477,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2396,13 +2495,13 @@
         <v>32</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G19">
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2424,7 +2523,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -2446,7 +2545,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -2468,7 +2567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -2486,13 +2585,13 @@
         <v>48</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2514,7 +2613,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2538,7 +2637,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2559,7 +2658,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2583,7 +2682,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2607,7 +2706,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -2631,7 +2730,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -2649,13 +2748,13 @@
         <v>117</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G30">
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2676,7 +2775,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -2694,13 +2793,13 @@
         <v>129</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G32">
         <v>0.93</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -2724,7 +2823,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
@@ -2742,13 +2841,13 @@
         <v>139</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -2772,7 +2871,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
@@ -2781,19 +2880,19 @@
         <v>128</v>
       </c>
       <c r="C36" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="F36" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G36">
         <v>0.92</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -2808,16 +2907,16 @@
         <v>1034</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G37">
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
@@ -2826,22 +2925,22 @@
         <v>130</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D38" s="2">
         <v>1034</v>
       </c>
       <c r="E38" s="54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G38" s="51">
         <v>0.92</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -2856,16 +2955,16 @@
         <v>1037</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G39">
         <v>1050</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -2874,19 +2973,19 @@
         <v>132</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D40" s="2">
         <v>1037</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G40">
         <v>1047</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -2901,16 +3000,16 @@
         <v>1047</v>
       </c>
       <c r="E41" s="48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G41" s="53">
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2925,13 +3024,13 @@
         <v>1047</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G42">
         <v>0.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -2946,16 +3045,16 @@
         <v>1047</v>
       </c>
       <c r="E43" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F43" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="F43" s="48" t="s">
-        <v>225</v>
-      </c>
       <c r="G43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -2970,13 +3069,13 @@
         <v>1047</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>121</v>
       </c>
@@ -2991,16 +3090,16 @@
         <v>1047</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F45" s="48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G45">
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -3015,16 +3114,16 @@
         <v>1047</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F46" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G46">
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -3033,22 +3132,22 @@
         <v>139</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D47" s="2">
         <v>1047</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F47" s="48" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G47">
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -3063,16 +3162,16 @@
         <v>1047</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G48">
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -3081,25 +3180,22 @@
         <v>141</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D49" s="2">
         <v>1047</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F49" s="61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G49">
         <v>0.93</v>
       </c>
-      <c r="H49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
@@ -3114,16 +3210,16 @@
         <v>1047</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F50" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="G50" t="s">
         <v>241</v>
       </c>
-      <c r="G50" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
@@ -3132,22 +3228,22 @@
         <v>143</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D51" s="2">
         <v>1047</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F51" s="48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G51">
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -3156,22 +3252,22 @@
         <v>144</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D52" s="2">
         <v>1047</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G52">
         <v>0.93</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>46</v>
       </c>
@@ -3180,16 +3276,16 @@
         <v>145</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D53" s="2">
         <v>1047</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>46</v>
       </c>
@@ -3204,16 +3300,13 @@
         <v>1047</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F54" s="48" t="s">
-        <v>275</v>
-      </c>
-      <c r="H54" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>46</v>
       </c>
@@ -3228,13 +3321,13 @@
         <v>1069</v>
       </c>
       <c r="E55" s="48" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G55" s="53">
         <v>1079</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>46</v>
       </c>
@@ -3249,13 +3342,13 @@
         <v>1069</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G56">
         <v>1078</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>46</v>
       </c>
@@ -3270,16 +3363,16 @@
         <v>1069</v>
       </c>
       <c r="E57" s="48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F57" s="39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G57">
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>46</v>
       </c>
@@ -3293,13 +3386,13 @@
         <v>1069</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G58">
         <v>1078</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -3313,13 +3406,13 @@
         <v>1069</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G59">
         <v>1072</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>46</v>
       </c>
@@ -3327,19 +3420,19 @@
         <v>152</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D60" s="2">
         <v>1069</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G60">
         <v>1071</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>46</v>
       </c>
@@ -3353,16 +3446,16 @@
         <v>1069</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G61">
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>53</v>
       </c>
@@ -3370,19 +3463,19 @@
         <v>154</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D62" s="2">
         <v>1072</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G62">
         <v>0.93</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>46</v>
       </c>
@@ -3390,19 +3483,19 @@
         <v>155</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D63" s="2">
         <v>1075</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G63">
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>53</v>
       </c>
@@ -3416,16 +3509,16 @@
         <v>1075</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G64" s="51">
         <v>0.92</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>46</v>
       </c>
@@ -3439,13 +3532,13 @@
         <v>1075</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G65">
         <v>1078</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>46</v>
       </c>
@@ -3459,73 +3552,73 @@
         <v>1075</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G66">
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B67" s="1">
         <v>159</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D67" s="2">
         <v>1075</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G67" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>160</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D68" s="2">
         <v>1075</v>
       </c>
       <c r="E68" s="55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>161</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D69" s="2">
         <v>1075</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G69">
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -3539,13 +3632,13 @@
         <v>1075</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G70">
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>163</v>
       </c>
@@ -3556,10 +3649,10 @@
         <v>1075</v>
       </c>
       <c r="E71" s="52" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>46</v>
       </c>
@@ -3573,10 +3666,10 @@
         <v>1079</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>53</v>
       </c>
@@ -3590,10 +3683,10 @@
         <v>1079</v>
       </c>
       <c r="E73" s="52" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>46</v>
       </c>
@@ -3601,16 +3694,16 @@
         <v>166</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D74" s="2">
         <v>1079</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>53</v>
       </c>
@@ -3624,10 +3717,10 @@
         <v>1081</v>
       </c>
       <c r="E75" s="52" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>46</v>
       </c>
@@ -3641,10 +3734,10 @@
         <v>1081</v>
       </c>
       <c r="E76" s="48" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>46</v>
       </c>
@@ -3658,39 +3751,37 @@
         <v>1081</v>
       </c>
       <c r="E77" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>327</v>
       </c>
       <c r="G77">
         <v>1085</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B78" s="1">
         <v>170</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D78" s="2">
         <v>1081</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F78" s="39" t="s">
-        <v>353</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="F78" s="48"/>
       <c r="G78">
         <v>1107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -3698,16 +3789,19 @@
         <v>171</v>
       </c>
       <c r="C79" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D79" s="2">
         <v>1085</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B80" s="1">
         <v>171</v>
       </c>
@@ -3718,10 +3812,16 @@
         <v>1100</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+        <v>351</v>
+      </c>
+      <c r="G80">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B81" s="1">
         <v>172</v>
       </c>
@@ -3732,13 +3832,16 @@
         <v>1100</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G81">
         <v>1111</v>
       </c>
     </row>
-    <row r="82" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B82" s="1">
         <v>173</v>
       </c>
@@ -3749,13 +3852,16 @@
         <v>1100</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G82">
         <v>1111</v>
       </c>
     </row>
-    <row r="83" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B83" s="1">
         <v>174</v>
       </c>
@@ -3766,24 +3872,37 @@
         <v>1100</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G83">
         <v>1111</v>
       </c>
     </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" s="1">
+        <v>175</v>
+      </c>
+      <c r="C84" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1120</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G83">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="D"/>
-        <filter val="V"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A7:G83" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -3793,24 +3912,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="60" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3853,7 +3971,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
     </row>
-    <row r="3" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>46</v>
       </c>
@@ -3908,7 +4026,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -3925,7 +4043,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -3942,7 +4060,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -3959,13 +4077,13 @@
         <v>45</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G8" s="37">
         <v>1078</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>46</v>
       </c>
@@ -3982,11 +4100,11 @@
         <v>0.92</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -4020,7 +4138,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -4054,7 +4172,7 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -4071,7 +4189,7 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -4088,7 +4206,7 @@
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
     </row>
-    <row r="16" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>46</v>
       </c>
@@ -4105,7 +4223,7 @@
         <v>0.92</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G16" s="37"/>
     </row>
@@ -4126,7 +4244,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>46</v>
       </c>
@@ -4143,7 +4261,7 @@
         <v>45</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G18" s="37"/>
     </row>
@@ -4162,7 +4280,7 @@
         <v>0.93</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G19" s="37"/>
     </row>
@@ -4181,7 +4299,7 @@
         <v>0.92</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G20" s="37"/>
     </row>
@@ -4191,10 +4309,10 @@
         <v>103</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E21" s="57">
         <v>0.93</v>
@@ -4202,7 +4320,7 @@
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
         <v>46</v>
       </c>
@@ -4219,11 +4337,11 @@
         <v>0.92</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G22" s="37"/>
     </row>
-    <row r="23" spans="1:7" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>46</v>
       </c>
@@ -4242,7 +4360,7 @@
       </c>
       <c r="G23" s="37"/>
     </row>
-    <row r="24" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>46</v>
       </c>
@@ -4259,7 +4377,7 @@
         <v>0.92</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G24" s="37">
         <v>1039</v>
@@ -4271,107 +4389,107 @@
         <v>107</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E25" s="57">
         <v>0.93</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E26" s="57">
         <v>0.93</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C27" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="37" t="s">
         <v>175</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>176</v>
       </c>
       <c r="E27" s="57">
         <v>0.93</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C28" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="37" t="s">
         <v>177</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>178</v>
       </c>
       <c r="E28" s="57">
         <v>0.92</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G28" s="37"/>
     </row>
     <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A29" s="36"/>
       <c r="B29" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C29" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="D29" s="37" t="s">
         <v>182</v>
-      </c>
-      <c r="D29" s="37" t="s">
-        <v>183</v>
       </c>
       <c r="E29" s="57">
         <v>0.93</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
       <c r="B30" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C30" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="37" t="s">
         <v>186</v>
-      </c>
-      <c r="D30" s="37" t="s">
-        <v>187</v>
       </c>
       <c r="E30" s="57">
         <v>0.95</v>
@@ -4379,35 +4497,35 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C31" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="37" t="s">
         <v>189</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>190</v>
       </c>
       <c r="E31" s="57">
         <v>0.92</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="36"/>
       <c r="B32" s="37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="37" t="s">
         <v>196</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>197</v>
       </c>
       <c r="E32" s="59"/>
       <c r="F32" s="37"/>
@@ -4416,13 +4534,13 @@
     <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A33" s="36"/>
       <c r="B33" s="37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C33" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="D33" s="37" t="s">
         <v>219</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>220</v>
       </c>
       <c r="E33" s="57">
         <v>0.93</v>
@@ -4433,13 +4551,13 @@
     <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
       <c r="B34" s="37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C34" s="37" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E34" s="57">
         <v>0.93</v>
@@ -4449,16 +4567,16 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E35" s="57">
         <v>0.93</v>
@@ -4469,13 +4587,13 @@
     <row r="36" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A36" s="36"/>
       <c r="B36" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C36" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="D36" s="37" t="s">
         <v>247</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>248</v>
       </c>
       <c r="E36" s="57">
         <v>0.93</v>
@@ -4486,13 +4604,13 @@
     <row r="37" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="36"/>
       <c r="B37" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C37" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="D37" s="37" t="s">
         <v>249</v>
-      </c>
-      <c r="D37" s="37" t="s">
-        <v>250</v>
       </c>
       <c r="E37" s="57">
         <v>0.93</v>
@@ -4503,13 +4621,13 @@
     <row r="38" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" s="36"/>
       <c r="B38" s="37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C38" s="37" t="s">
         <v>154</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E38" s="57">
         <v>0.93</v>
@@ -4517,24 +4635,24 @@
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
     </row>
-    <row r="39" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E39" s="57">
         <v>0.92</v>
       </c>
       <c r="F39" s="50" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G39" s="4">
         <v>1078</v>
@@ -4542,27 +4660,27 @@
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E41" s="57">
         <v>0.93</v>
@@ -4570,13 +4688,13 @@
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E42" s="57">
         <v>0.92</v>
@@ -4584,13 +4702,13 @@
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E43" s="57">
         <v>0.92</v>
@@ -4598,27 +4716,27 @@
     </row>
     <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E44" s="57">
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E45" s="57">
         <v>0.92</v>
@@ -4626,13 +4744,13 @@
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E46" s="57">
         <v>0.92</v>
@@ -4640,13 +4758,13 @@
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E47" s="57">
         <v>0.92</v>
@@ -4654,195 +4772,233 @@
     </row>
     <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E48" s="57">
         <v>0.92</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="D49" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D50" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>302</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>303</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>314</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>319</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>340</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>343</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D60" s="4" t="s">
+    </row>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B61" s="4" t="s">
+      <c r="D61" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="D61" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>364</v>
+    </row>
+    <row r="63" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G56">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="D"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -4852,46 +5008,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="41"/>
-    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="41"/>
-    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="41"/>
+    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="41"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
+      <c r="B2" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="62"/>
       <c r="C3" s="62"/>
       <c r="D3" s="62"/>
@@ -4900,9 +5056,9 @@
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="64" t="s">
-        <v>368</v>
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="65" t="s">
+        <v>366</v>
       </c>
       <c r="C4" s="66"/>
       <c r="D4" s="66"/>
@@ -4911,18 +5067,18 @@
       <c r="G4" s="66"/>
       <c r="H4" s="66"/>
     </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="64" t="s">
-        <v>369</v>
-      </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="65" t="s">
+        <v>367</v>
+      </c>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -4931,12 +5087,12 @@
       <c r="G6" s="62"/>
       <c r="H6" s="62"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="42" t="s">
         <v>1</v>
       </c>
@@ -4962,7 +5118,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="45" t="s">
         <v>58</v>
       </c>
@@ -4972,535 +5128,535 @@
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I9" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="46"/>
       <c r="I91" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="46"/>
       <c r="I92" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="47"/>
     </row>
-    <row r="102" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="47"/>
     </row>
-    <row r="105" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="47"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="47"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="47"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="47"/>
     </row>
   </sheetData>
@@ -5512,4 +5668,115 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E12D459-7A3B-43CD-9A95-0F7C890F4CFC}">
+  <dimension ref="A3:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>383</v>
+      </c>
+      <c r="H5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" t="s">
+        <v>380</v>
+      </c>
+      <c r="E6" t="s">
+        <v>381</v>
+      </c>
+      <c r="F6" t="s">
+        <v>382</v>
+      </c>
+      <c r="G6" t="s">
+        <v>379</v>
+      </c>
+      <c r="H6" t="s">
+        <v>380</v>
+      </c>
+      <c r="I6" t="s">
+        <v>381</v>
+      </c>
+      <c r="J6" t="s">
+        <v>382</v>
+      </c>
+      <c r="K6" t="s">
+        <v>379</v>
+      </c>
+      <c r="L6" t="s">
+        <v>380</v>
+      </c>
+      <c r="M6" t="s">
+        <v>381</v>
+      </c>
+      <c r="N6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>388</v>
+      </c>
+      <c r="F7" s="63" t="s">
+        <v>389</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>386</v>
+      </c>
+      <c r="H7" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="I7" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="J7" s="63" t="s">
+        <v>391</v>
+      </c>
+      <c r="K7" s="63" t="s">
+        <v>392</v>
+      </c>
+      <c r="L7" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="M7" s="63" t="s">
+        <v>394</v>
+      </c>
+      <c r="N7" s="63" t="s">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A2OSX.MAKE has had significant structural (directory layout) changes as well as new README and script files added.  More to come.  Updated issue/suggest list
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC760D8-303D-49FD-ABE8-8290126DB897}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3465CA62-2B07-473B-8C94-C76DA0A3A467}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
     <sheet name="Suggestions" sheetId="2" r:id="rId2"/>
     <sheet name="Commands" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Memory" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$83</definedName>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="402">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1336,13 +1336,16 @@
     <t>Tweak</t>
   </si>
   <si>
-    <t>Rename A2OSX.BUILD to just A2OSX or BUILD, it saves memory and shortens PATH.  Move files in BIN/DEV to BIN and remove BIN/DEV from PATH (done in INIT).  Add USR/BIN to PATH (for User Scripts and programs).</t>
-  </si>
-  <si>
     <t>S0065</t>
   </si>
   <si>
     <t>Get rid of $LIB and $DRV. Make programs that rely on those vars look at ${ROOT}LIB/ or DRV/.  This will save ENV space which is limited.</t>
+  </si>
+  <si>
+    <t>If are editing a new file "EDIT NEWFILE" when you go to save the first time the name field is blank, you have to enter the name again.  Update: this happens multiple times while editing the file.</t>
+  </si>
+  <si>
+    <t>Rename A2OSX.BUILD to A2DEV, it saves memory and shortens PATH.  Also A2DEV reflects that it is a development image, not a production/test/release image.  Move files in BIN/DEV to BIN and remove BIN/DEV from PATH (done in INIT).  Add USR/BIN to PATH (for User Scripts and programs).</t>
   </si>
 </sst>
 </file>
@@ -2131,10 +2134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A79" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,6 +3904,20 @@
         <v>376</v>
       </c>
     </row>
+    <row r="85" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B85" s="1">
+        <v>176</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1129</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A7:G83" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3915,8 +3932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4975,7 +4992,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>396</v>
       </c>
@@ -4983,18 +5000,18 @@
         <v>397</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>397</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated issue list for build 1139.  Updated memory page (sheet 4) for 1139 comparison.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B772D6F-89AF-4C84-B753-C3F24799292E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02494A4-09EB-41D8-9DC0-A59B44D10CC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="425">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1339,9 +1339,6 @@
     <t>Get rid of $LIB and $DRV. Make programs that rely on those vars look at ${ROOT}LIB/ or DRV/.  This will save ENV space which is limited.</t>
   </si>
   <si>
-    <t>If are editing a new file "EDIT NEWFILE" when you go to save the first time the name field is blank, you have to enter the name again.  Update: this happens multiple times while editing the file.</t>
-  </si>
-  <si>
     <t>Rename A2OSX.BUILD to A2DEV, it saves memory and shortens PATH.  Also A2DEV reflects that it is a development image, not a production/test/release image.  Move files in BIN/DEV to BIN and remove BIN/DEV from PATH (done in INIT).  Add USR/BIN to PATH (for User Scripts and programs).</t>
   </si>
   <si>
@@ -1388,6 +1385,36 @@
   </si>
   <si>
     <t>04314</t>
+  </si>
+  <si>
+    <t>MORE on anyfile fails with [$06] unknown error</t>
+  </si>
+  <si>
+    <t>$ED99</t>
+  </si>
+  <si>
+    <t>$EED9</t>
+  </si>
+  <si>
+    <t>04385</t>
+  </si>
+  <si>
+    <t>set -x</t>
+  </si>
+  <si>
+    <t>SETXTEST fails.  IFTEST fails.  Any script with SET -X in it gives [$02]:Unknown error.</t>
+  </si>
+  <si>
+    <t>Return Code</t>
+  </si>
+  <si>
+    <t>RCTEST failed, calling RCSUB2 should return 20 it returns 0.</t>
+  </si>
+  <si>
+    <t>TELNET to linux, it says connected but I never get Login prompt from host.  Telnet to a80s seems to work fine.  Tried at both fast and normal speeds.</t>
+  </si>
+  <si>
+    <t>If are editing a new file "EDIT NEWFILE" when you go to save the first time the name field is blank, you have to enter the name again.  Update: this happens multiple times while editing the file. Update 2, ha[ppens with old files too.  Cd to ETC then EDIT HOSTS make changes and ctrl-S, file name will be blank.</t>
   </si>
 </sst>
 </file>
@@ -2176,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3946,7 +3973,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
         <v>176</v>
       </c>
@@ -3957,7 +3984,63 @@
         <v>1129</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>399</v>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="1">
+        <v>177</v>
+      </c>
+      <c r="C86" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1139</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B87" s="1">
+        <v>178</v>
+      </c>
+      <c r="C87" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1139</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B88" s="1">
+        <v>179</v>
+      </c>
+      <c r="C88" s="27" t="s">
+        <v>421</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1139</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B89" s="1">
+        <v>180</v>
+      </c>
+      <c r="C89" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1139</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -5042,7 +5125,7 @@
         <v>396</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
@@ -5731,10 +5814,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E12D459-7A3B-43CD-9A95-0F7C890F4CFC}">
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5839,40 +5922,40 @@
         <v>1127</v>
       </c>
       <c r="C8" s="63" t="s">
+        <v>400</v>
+      </c>
+      <c r="D8" s="63" t="s">
         <v>401</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>402</v>
       </c>
       <c r="E8" s="63" t="s">
         <v>387</v>
       </c>
       <c r="F8" s="63" t="s">
+        <v>402</v>
+      </c>
+      <c r="G8" s="63" t="s">
         <v>403</v>
       </c>
-      <c r="G8" s="63" t="s">
+      <c r="H8" s="63" t="s">
         <v>404</v>
       </c>
-      <c r="H8" s="63" t="s">
+      <c r="I8" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J8" s="63" t="s">
         <v>405</v>
       </c>
-      <c r="I8" s="63" t="s">
-        <v>405</v>
-      </c>
-      <c r="J8" s="63" t="s">
+      <c r="K8" s="63" t="s">
         <v>406</v>
       </c>
-      <c r="K8" s="63" t="s">
+      <c r="L8" s="63" t="s">
         <v>407</v>
-      </c>
-      <c r="L8" s="63" t="s">
-        <v>408</v>
       </c>
       <c r="M8" s="63" t="s">
         <v>393</v>
       </c>
       <c r="N8" s="63" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5880,40 +5963,81 @@
         <v>1137</v>
       </c>
       <c r="C9" s="63" t="s">
+        <v>409</v>
+      </c>
+      <c r="D9" s="63" t="s">
         <v>410</v>
-      </c>
-      <c r="D9" s="63" t="s">
-        <v>411</v>
       </c>
       <c r="E9" s="63" t="s">
         <v>387</v>
       </c>
       <c r="F9" s="63" t="s">
+        <v>411</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H9" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I9" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J9" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K9" s="63" t="s">
         <v>412</v>
       </c>
-      <c r="G9" s="63" t="s">
-        <v>404</v>
-      </c>
-      <c r="H9" s="63" t="s">
-        <v>405</v>
-      </c>
-      <c r="I9" s="63" t="s">
-        <v>405</v>
-      </c>
-      <c r="J9" s="63" t="s">
-        <v>406</v>
-      </c>
-      <c r="K9" s="63" t="s">
+      <c r="L9" s="63" t="s">
         <v>413</v>
-      </c>
-      <c r="L9" s="63" t="s">
-        <v>414</v>
       </c>
       <c r="M9" s="63" t="s">
         <v>393</v>
       </c>
       <c r="N9" s="63" t="s">
-        <v>415</v>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1139</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>409</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>410</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F10" s="63" t="s">
+        <v>411</v>
+      </c>
+      <c r="G10" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H10" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I10" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J10" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K10" s="63" t="s">
+        <v>416</v>
+      </c>
+      <c r="L10" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="M10" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N10" s="63" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with mem usages of latest build
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CA52DD-E8F3-4197-99E5-E9FE9B4965A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="468">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1413,11 +1419,140 @@
   <si>
     <t>cannot reproduce on 1142</t>
   </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>$81E0</t>
+  </si>
+  <si>
+    <t>25074</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>$1FF7</t>
+  </si>
+  <si>
+    <t>24297</t>
+  </si>
+  <si>
+    <t>$EB5F</t>
+  </si>
+  <si>
+    <t>$EC4F</t>
+  </si>
+  <si>
+    <t>05035</t>
+  </si>
+  <si>
+    <t>NET</t>
+  </si>
+  <si>
+    <t>$4E00</t>
+  </si>
+  <si>
+    <t>11785</t>
+  </si>
+  <si>
+    <t>$EEE5</t>
+  </si>
+  <si>
+    <t>04373</t>
+  </si>
+  <si>
+    <t>25065</t>
+  </si>
+  <si>
+    <t>Uther</t>
+  </si>
+  <si>
+    <t>$EEE2</t>
+  </si>
+  <si>
+    <t>04376</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>dhcp</t>
+  </si>
+  <si>
+    <t>$1FFA</t>
+  </si>
+  <si>
+    <t>25062</t>
+  </si>
+  <si>
+    <t>$A200</t>
+  </si>
+  <si>
+    <t>$EB86</t>
+  </si>
+  <si>
+    <t>$EC46</t>
+  </si>
+  <si>
+    <t>34913</t>
+  </si>
+  <si>
+    <t>05044</t>
+  </si>
+  <si>
+    <t>$7D00</t>
+  </si>
+  <si>
+    <t>23814</t>
+  </si>
+  <si>
+    <t>$EEd9</t>
+  </si>
+  <si>
+    <t>04382</t>
+  </si>
+  <si>
+    <t>uther</t>
+  </si>
+  <si>
+    <t>$59E0</t>
+  </si>
+  <si>
+    <t>14822</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>$4000</t>
+  </si>
+  <si>
+    <t>$5500</t>
+  </si>
+  <si>
+    <t>05376</t>
+  </si>
+  <si>
+    <t>$8BE0</t>
+  </si>
+  <si>
+    <t>19424</t>
+  </si>
+  <si>
+    <t>$FEDE</t>
+  </si>
+  <si>
+    <t>00284</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1697,7 +1832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1874,6 +2009,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2192,34 +2329,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -2234,7 +2371,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -2247,7 +2384,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>121</v>
@@ -2260,7 +2397,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>53</v>
@@ -2273,12 +2410,12 @@
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -2301,7 +2438,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2322,7 +2459,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2344,7 +2481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -2366,7 +2503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2479,7 +2616,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2547,7 +2684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2571,7 +2708,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -2593,7 +2730,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -2615,7 +2752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="217.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -2661,7 +2798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2683,7 +2820,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2728,7 +2865,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2752,7 +2889,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2824,7 +2961,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2845,7 +2982,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -2986,7 +3123,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
@@ -3010,7 +3147,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3079,7 +3216,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -3100,7 +3237,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -3124,7 +3261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -3145,7 +3282,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>121</v>
       </c>
@@ -3193,7 +3330,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -3241,7 +3378,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -3265,7 +3402,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
@@ -3313,7 +3450,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -3442,7 +3579,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>46</v>
       </c>
@@ -3525,7 +3662,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>53</v>
       </c>
@@ -3545,7 +3682,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>46</v>
       </c>
@@ -3565,7 +3702,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>53</v>
       </c>
@@ -3588,7 +3725,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>46</v>
       </c>
@@ -3608,7 +3745,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>46</v>
       </c>
@@ -3628,7 +3765,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>328</v>
       </c>
@@ -3651,7 +3788,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>160</v>
       </c>
@@ -3668,7 +3805,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>161</v>
       </c>
@@ -3688,7 +3825,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -3708,7 +3845,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>163</v>
       </c>
@@ -3722,7 +3859,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>46</v>
       </c>
@@ -3739,7 +3876,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>53</v>
       </c>
@@ -3756,7 +3893,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>46</v>
       </c>
@@ -3773,7 +3910,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>53</v>
       </c>
@@ -3790,7 +3927,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>46</v>
       </c>
@@ -3851,7 +3988,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -3868,7 +4005,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>53</v>
       </c>
@@ -3888,7 +4025,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>46</v>
       </c>
@@ -3971,7 +4108,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
         <v>176</v>
       </c>
@@ -3988,7 +4125,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
         <v>177</v>
       </c>
@@ -4005,7 +4142,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
         <v>178</v>
       </c>
@@ -4022,7 +4159,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
         <v>179</v>
       </c>
@@ -4036,7 +4173,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
         <v>180</v>
       </c>
@@ -4051,7 +4188,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G89">
+  <autoFilter ref="A7:G89" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -4068,23 +4205,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="60" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4182,7 +4319,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -4199,7 +4336,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -4216,7 +4353,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -4260,7 +4397,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -4294,7 +4431,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -4328,7 +4465,7 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -4345,7 +4482,7 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -4558,7 +4695,7 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
@@ -4577,7 +4714,7 @@
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
         <v>161</v>
@@ -4596,7 +4733,7 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>46</v>
       </c>
@@ -4653,7 +4790,7 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>165</v>
@@ -4723,7 +4860,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
         <v>169</v>
@@ -4884,7 +5021,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>258</v>
       </c>
@@ -4985,7 +5122,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>46</v>
       </c>
@@ -5010,7 +5147,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>305</v>
       </c>
@@ -5142,7 +5279,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>397</v>
       </c>
@@ -5154,7 +5291,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63"/>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -5164,46 +5301,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="41"/>
-    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="41"/>
-    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="41"/>
+    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="41"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="66" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="62"/>
       <c r="C3" s="62"/>
       <c r="D3" s="62"/>
@@ -5212,29 +5349,29 @@
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="65" t="s">
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="67" t="s">
         <v>366</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-    </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="65" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+    </row>
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="67" t="s">
         <v>367</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-    </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -5243,12 +5380,12 @@
       <c r="G6" s="62"/>
       <c r="H6" s="62"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="42" t="s">
         <v>1</v>
       </c>
@@ -5274,7 +5411,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="45" t="s">
         <v>58</v>
       </c>
@@ -5290,529 +5427,529 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="46"/>
       <c r="I91" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="46"/>
       <c r="I92" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="47"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="47"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="47"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="47"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="47"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="47"/>
     </row>
   </sheetData>
@@ -5827,14 +5964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -6052,6 +6189,414 @@
       </c>
       <c r="N10" s="63" t="s">
         <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>409</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>427</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>428</v>
+      </c>
+      <c r="G11" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H11" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I11" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J11" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K11" s="63" t="s">
+        <v>416</v>
+      </c>
+      <c r="L11" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="M11" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N11" s="63" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>429</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>409</v>
+      </c>
+      <c r="D12" s="63" t="s">
+        <v>410</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F12" s="63" t="s">
+        <v>411</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H12" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I12" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J12" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K12" s="63" t="s">
+        <v>416</v>
+      </c>
+      <c r="L12" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="M12" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N12" s="63" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1144</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>430</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>410</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F13" s="63" t="s">
+        <v>431</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H13" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I13" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J13" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K13" s="63" t="s">
+        <v>432</v>
+      </c>
+      <c r="L13" s="63" t="s">
+        <v>433</v>
+      </c>
+      <c r="M13" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N13" s="63" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>435</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>430</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>436</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F14" s="63" t="s">
+        <v>437</v>
+      </c>
+      <c r="G14" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H14" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I14" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J14" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K14" s="63" t="s">
+        <v>432</v>
+      </c>
+      <c r="L14" s="63" t="s">
+        <v>438</v>
+      </c>
+      <c r="M14" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N14" s="63" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1145</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>430</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>427</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F15" s="63" t="s">
+        <v>440</v>
+      </c>
+      <c r="G15" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H15" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I15" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J15" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K15" s="63" t="s">
+        <v>432</v>
+      </c>
+      <c r="L15" s="63" t="s">
+        <v>433</v>
+      </c>
+      <c r="M15" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N15" s="63" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" s="64">
+        <v>7900</v>
+      </c>
+      <c r="F16">
+        <v>22793</v>
+      </c>
+      <c r="L16" s="63" t="s">
+        <v>442</v>
+      </c>
+      <c r="N16" s="63" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>444</v>
+      </c>
+      <c r="D17" s="65">
+        <v>56</v>
+      </c>
+      <c r="F17">
+        <v>14057</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>445</v>
+      </c>
+      <c r="F18">
+        <v>14057</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1153</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>427</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F19" s="63" t="s">
+        <v>447</v>
+      </c>
+      <c r="G19" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H19" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I19" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J19" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K19" s="63" t="s">
+        <v>449</v>
+      </c>
+      <c r="L19" s="63" t="s">
+        <v>450</v>
+      </c>
+      <c r="M19" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N19" s="63" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>457</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>453</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F20" s="63" t="s">
+        <v>454</v>
+      </c>
+      <c r="G20" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H20" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I20" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J20" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K20" s="63" t="s">
+        <v>449</v>
+      </c>
+      <c r="L20" s="63" t="s">
+        <v>455</v>
+      </c>
+      <c r="M20" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N20" s="63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>444</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>458</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F21" s="63" t="s">
+        <v>459</v>
+      </c>
+      <c r="G21" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H21" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I21" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J21" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K21" s="63" t="s">
+        <v>449</v>
+      </c>
+      <c r="L21" s="63" t="s">
+        <v>455</v>
+      </c>
+      <c r="M21" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N21" s="63" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>460</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>461</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>462</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F22" s="63" t="s">
+        <v>463</v>
+      </c>
+      <c r="G22" s="63" t="s">
+        <v>461</v>
+      </c>
+      <c r="H22" s="63" t="s">
+        <v>464</v>
+      </c>
+      <c r="I22" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J22" s="63" t="s">
+        <v>465</v>
+      </c>
+      <c r="K22" s="63" t="s">
+        <v>449</v>
+      </c>
+      <c r="L22" s="63" t="s">
+        <v>466</v>
+      </c>
+      <c r="M22" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N22" s="63" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Issue List for 1160, many issues added.  mem chart updated.  Test files moved to Github and being added here.  Most of them still need to be updated to support being added back through scasm3.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CA52DD-E8F3-4197-99E5-E9FE9B4965A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9183FC17-A33E-4244-8131-AE564281671E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="486">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1544,6 +1544,60 @@
   </si>
   <si>
     <t>00284</t>
+  </si>
+  <si>
+    <t>$1FE6</t>
+  </si>
+  <si>
+    <t>25082</t>
+  </si>
+  <si>
+    <t>$EC50</t>
+  </si>
+  <si>
+    <t>$EDBD</t>
+  </si>
+  <si>
+    <t>04669</t>
+  </si>
+  <si>
+    <t>1 tty</t>
+  </si>
+  <si>
+    <t>$87E0</t>
+  </si>
+  <si>
+    <t>26618</t>
+  </si>
+  <si>
+    <t>$7CE0</t>
+  </si>
+  <si>
+    <t>23802</t>
+  </si>
+  <si>
+    <t>When you more a file (more ../etc/init), if you are using the option of pressing return for one more line, when you get to the end of the file, return just gives you more and more blank lines instead of ending more because you are at the end of the file.</t>
+  </si>
+  <si>
+    <t>At the end of TESTS/BUILDTEST (line 68) there is a dashed line ended with \n, which should on screen be a dashed line and then blank line, instead you get 2 dashed lines.  If you look at code, you can remove \n and the comment mark in line 69 and it displays right, but this second dashed line should not happen.</t>
+  </si>
+  <si>
+    <t>NETWORKING</t>
+  </si>
+  <si>
+    <t>DHCP Never Leases and address.  If you do fixed IP address, DNS resolution does not appear to work and ping does not get any responses to local or remote networks.  TELNET locks after Ctrl-T and does not connect to any sources.</t>
+  </si>
+  <si>
+    <t>In a script, the CD command has no effect.  See TESTS/TESTS file which gets placed in root and should change you to usr/share/tests.  It does nothing.  Even if you do . TESTS.  I tried adding PWD after the CD command in the script, pwd shows that it the working dir changed, but script exits it goes back to wear it was.</t>
+  </si>
+  <si>
+    <t>RETURN CODE</t>
+  </si>
+  <si>
+    <t>RCTEST fails, you get bogus results.  Also in CDTEST, after each CD command you get some randowm number returned instead of 0 for no error (even though it worked).  Something is clearly off here.</t>
+  </si>
+  <si>
+    <t>More Line numbering on long files works if you press space for next page, but repeats the same number over and over if you press return (though it does display contents right, except it will keep going passed end see 181).</t>
   </si>
 </sst>
 </file>
@@ -2338,10 +2392,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4185,6 +4239,90 @@
       </c>
       <c r="E89" s="3" t="s">
         <v>423</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B90" s="1">
+        <v>181</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B91" s="1">
+        <v>182</v>
+      </c>
+      <c r="C91" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B92" s="1">
+        <v>183</v>
+      </c>
+      <c r="C92" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B93" s="1">
+        <v>184</v>
+      </c>
+      <c r="C93" s="27" t="s">
+        <v>480</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B94" s="1">
+        <v>185</v>
+      </c>
+      <c r="C94" s="27" t="s">
+        <v>483</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B95" s="1">
+        <v>186</v>
+      </c>
+      <c r="C95" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -5965,10 +6103,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A3:N22"/>
+  <dimension ref="A3:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6599,6 +6737,129 @@
         <v>467</v>
       </c>
     </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1154</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>427</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F23" s="63" t="s">
+        <v>469</v>
+      </c>
+      <c r="G23" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H23" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I23" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J23" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K23" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L23" s="63" t="s">
+        <v>471</v>
+      </c>
+      <c r="M23" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N23" s="63" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>473</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>474</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>475</v>
+      </c>
+      <c r="G24" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H24" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I24" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J24" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K24" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L24" s="63" t="s">
+        <v>471</v>
+      </c>
+      <c r="M24" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N24" s="63" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1160</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>476</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F25" s="63" t="s">
+        <v>477</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I25" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J25" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K25" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L25" s="63" t="s">
+        <v>471</v>
+      </c>
+      <c r="M25" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N25" s="63" t="s">
+        <v>472</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Mem Sheet with multiple net settings
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119E436F-78EA-4413-BAC5-04535EFF5BFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,8 +31,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Patrick</author>
+  </authors>
+  <commentList>
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{8FF86A30-C51C-452C-89AB-8368255F29CF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+manually did networkd libtcpip &amp;</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="500">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1600,15 +1640,51 @@
   <si>
     <t>Bug in TERM scroll UP</t>
   </si>
+  <si>
+    <t>netd</t>
+  </si>
+  <si>
+    <t>$3300</t>
+  </si>
+  <si>
+    <t>04890</t>
+  </si>
+  <si>
+    <t>$F061</t>
+  </si>
+  <si>
+    <t>03993</t>
+  </si>
+  <si>
+    <t>telnetd</t>
+  </si>
+  <si>
+    <t>$2DE0</t>
+  </si>
+  <si>
+    <t>03578</t>
+  </si>
+  <si>
+    <t>drv uther</t>
+  </si>
+  <si>
+    <t>networkd</t>
+  </si>
+  <si>
+    <t>$4510</t>
+  </si>
+  <si>
+    <t>09514</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1688,6 +1764,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2064,7 +2153,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2397,34 +2486,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -2439,7 +2528,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -2452,7 +2541,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>121</v>
@@ -2483,7 +2572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -2506,7 +2595,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2527,7 +2616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2684,7 +2773,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2752,7 +2841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2776,7 +2865,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -3029,7 +3118,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
@@ -3518,7 +3607,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -3893,7 +3982,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -4193,7 +4282,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
         <v>177</v>
       </c>
@@ -4272,7 +4361,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
         <v>182</v>
       </c>
@@ -4292,7 +4381,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
         <v>183</v>
       </c>
@@ -4312,7 +4401,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="67"/>
       <c r="B93" s="68">
         <v>184</v>
@@ -4331,7 +4420,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
         <v>185</v>
       </c>
@@ -4348,7 +4437,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
         <v>186</v>
       </c>
@@ -4366,7 +4455,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G89">
+  <autoFilter ref="A7:G89" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -4383,23 +4472,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="60" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4497,7 +4586,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -4514,7 +4603,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -4531,7 +4620,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -4575,7 +4664,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -4609,7 +4698,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -4643,7 +4732,7 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -4660,7 +4749,7 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -4873,7 +4962,7 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
@@ -4892,7 +4981,7 @@
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
         <v>161</v>
@@ -4911,7 +5000,7 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>46</v>
       </c>
@@ -4968,7 +5057,7 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>165</v>
@@ -5038,7 +5127,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
         <v>169</v>
@@ -5199,7 +5288,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>258</v>
       </c>
@@ -5300,7 +5389,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>46</v>
       </c>
@@ -5325,7 +5414,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>305</v>
       </c>
@@ -5457,7 +5546,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>397</v>
       </c>
@@ -5469,7 +5558,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63"/>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -5479,27 +5568,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="41"/>
-    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="41"/>
-    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="41"/>
+    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="41"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
@@ -5518,7 +5607,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="62"/>
       <c r="C3" s="62"/>
       <c r="D3" s="62"/>
@@ -5527,7 +5616,7 @@
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="72" t="s">
         <v>366</v>
       </c>
@@ -5538,7 +5627,7 @@
       <c r="G4" s="73"/>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
         <v>367</v>
       </c>
@@ -5549,7 +5638,7 @@
       <c r="G5" s="74"/>
       <c r="H5" s="74"/>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -5558,12 +5647,12 @@
       <c r="G6" s="62"/>
       <c r="H6" s="62"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="42" t="s">
         <v>1</v>
       </c>
@@ -5589,7 +5678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="45" t="s">
         <v>58</v>
       </c>
@@ -5605,529 +5694,529 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="46"/>
       <c r="I91" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="46"/>
       <c r="I92" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="47"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="47"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="47"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="47"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="47"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="47"/>
     </row>
   </sheetData>
@@ -6142,14 +6231,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -6900,8 +6992,214 @@
         <v>472</v>
       </c>
     </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1167</v>
+      </c>
+      <c r="C26" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>476</v>
+      </c>
+      <c r="E26" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F26" s="63" t="s">
+        <v>477</v>
+      </c>
+      <c r="G26" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H26" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I26" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J26" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K26" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L26" s="63" t="s">
+        <v>471</v>
+      </c>
+      <c r="M26" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N26" s="63" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>496</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>476</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F27" s="63" t="s">
+        <v>477</v>
+      </c>
+      <c r="G27" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H27" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I27" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J27" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K27" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L27" s="63" t="s">
+        <v>491</v>
+      </c>
+      <c r="M27" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N27" s="63" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>497</v>
+      </c>
+      <c r="C28" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>498</v>
+      </c>
+      <c r="E28" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F28" s="63" t="s">
+        <v>499</v>
+      </c>
+      <c r="G28" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H28" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I28" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J28" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K28" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L28" s="63" t="s">
+        <v>491</v>
+      </c>
+      <c r="M28" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N28" s="63" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>488</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>489</v>
+      </c>
+      <c r="E29" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F29" s="63" t="s">
+        <v>490</v>
+      </c>
+      <c r="G29" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H29" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I29" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J29" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K29" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L29" s="63" t="s">
+        <v>491</v>
+      </c>
+      <c r="M29" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N29" s="63" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>493</v>
+      </c>
+      <c r="C30" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D30" s="63" t="s">
+        <v>494</v>
+      </c>
+      <c r="E30" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F30" s="63" t="s">
+        <v>495</v>
+      </c>
+      <c r="G30" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H30" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="I30" s="63" t="s">
+        <v>448</v>
+      </c>
+      <c r="J30" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="K30" s="63" t="s">
+        <v>470</v>
+      </c>
+      <c r="L30" s="63" t="s">
+        <v>491</v>
+      </c>
+      <c r="M30" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N30" s="63" t="s">
+        <v>492</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated mem chart for 1173
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119E436F-78EA-4413-BAC5-04535EFF5BFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC92749-1016-4A2E-A88C-B4F239F6A6DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,12 +61,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{4625514B-D423-42AF-966A-ECB36E627AAC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+manually did networkd libtcpip &amp;</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="513">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1675,6 +1699,45 @@
   </si>
   <si>
     <t>09514</t>
+  </si>
+  <si>
+    <t>$1FE4</t>
+  </si>
+  <si>
+    <t>$EC7F</t>
+  </si>
+  <si>
+    <t>$EE2D</t>
+  </si>
+  <si>
+    <t>04557</t>
+  </si>
+  <si>
+    <t>$F0D1</t>
+  </si>
+  <si>
+    <t>03881</t>
+  </si>
+  <si>
+    <t>$7B00</t>
+  </si>
+  <si>
+    <t>23324</t>
+  </si>
+  <si>
+    <t>13596</t>
+  </si>
+  <si>
+    <t>$4360</t>
+  </si>
+  <si>
+    <t>09084</t>
+  </si>
+  <si>
+    <t>$40B0</t>
+  </si>
+  <si>
+    <t>08396</t>
   </si>
 </sst>
 </file>
@@ -6232,10 +6295,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A3:N30"/>
+  <dimension ref="A3:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7197,6 +7260,211 @@
         <v>492</v>
       </c>
     </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1173</v>
+      </c>
+      <c r="C31" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>506</v>
+      </c>
+      <c r="E31" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F31" s="63" t="s">
+        <v>507</v>
+      </c>
+      <c r="G31" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H31" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I31" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J31" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K31" s="63" t="s">
+        <v>501</v>
+      </c>
+      <c r="L31" s="63" t="s">
+        <v>502</v>
+      </c>
+      <c r="M31" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N31" s="63" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>488</v>
+      </c>
+      <c r="C32" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>462</v>
+      </c>
+      <c r="E32" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F32" s="63" t="s">
+        <v>508</v>
+      </c>
+      <c r="G32" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H32" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I32" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J32" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K32" s="63" t="s">
+        <v>501</v>
+      </c>
+      <c r="L32" s="63" t="s">
+        <v>504</v>
+      </c>
+      <c r="M32" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N32" s="63" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>496</v>
+      </c>
+      <c r="C33" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>506</v>
+      </c>
+      <c r="E33" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F33" s="63" t="s">
+        <v>507</v>
+      </c>
+      <c r="G33" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H33" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I33" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J33" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K33" s="63" t="s">
+        <v>501</v>
+      </c>
+      <c r="L33" s="63" t="s">
+        <v>504</v>
+      </c>
+      <c r="M33" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N33" s="63" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>497</v>
+      </c>
+      <c r="C34" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="D34" s="63" t="s">
+        <v>509</v>
+      </c>
+      <c r="E34" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F34" s="63" t="s">
+        <v>510</v>
+      </c>
+      <c r="G34" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H34" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I34" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J34" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K34" s="63" t="s">
+        <v>501</v>
+      </c>
+      <c r="L34" s="63" t="s">
+        <v>504</v>
+      </c>
+      <c r="M34" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N34" s="63" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>493</v>
+      </c>
+      <c r="C35" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="D35" s="63" t="s">
+        <v>511</v>
+      </c>
+      <c r="E35" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F35" s="63" t="s">
+        <v>512</v>
+      </c>
+      <c r="G35" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H35" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I35" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="J35" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K35" s="63" t="s">
+        <v>501</v>
+      </c>
+      <c r="L35" s="63" t="s">
+        <v>504</v>
+      </c>
+      <c r="M35" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N35" s="63" t="s">
+        <v>505</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated mem sheet for build 1177, highlighted the manual vs. NETD loading of network
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E369F9C5-CB7E-4A38-B727-C69C983A1E54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Patrick</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +61,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+manually did networkd libtcpip &amp;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{DFC45764-65D1-4338-A5B1-FC654D41C384}">
       <text>
         <r>
           <rPr>
@@ -84,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="526">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1733,13 +1763,52 @@
   <si>
     <t>08396</t>
   </si>
+  <si>
+    <t>$8700</t>
+  </si>
+  <si>
+    <t>26396</t>
+  </si>
+  <si>
+    <t>$A980</t>
+  </si>
+  <si>
+    <t>36833</t>
+  </si>
+  <si>
+    <t>$ECF7</t>
+  </si>
+  <si>
+    <t>$EE23</t>
+  </si>
+  <si>
+    <t>04567</t>
+  </si>
+  <si>
+    <t>$6200</t>
+  </si>
+  <si>
+    <t>16924</t>
+  </si>
+  <si>
+    <t>$F0C7</t>
+  </si>
+  <si>
+    <t>03891</t>
+  </si>
+  <si>
+    <t>$5160</t>
+  </si>
+  <si>
+    <t>12668</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1836,7 +1905,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1876,6 +1945,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2033,7 +2114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2210,7 +2291,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2236,6 +2317,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2543,34 +2632,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -2585,7 +2674,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -2598,7 +2687,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>121</v>
@@ -2629,7 +2718,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -2652,7 +2741,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2673,7 +2762,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2830,7 +2919,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2898,7 +2987,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -2922,7 +3011,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -3664,7 +3753,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -4039,7 +4128,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -4339,7 +4428,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
         <v>177</v>
       </c>
@@ -4438,7 +4527,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
         <v>183</v>
       </c>
@@ -4458,7 +4547,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="67"/>
       <c r="B93" s="68">
         <v>184</v>
@@ -4477,7 +4566,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
         <v>185</v>
       </c>
@@ -4494,7 +4583,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
         <v>186</v>
       </c>
@@ -4512,7 +4601,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G89">
+  <autoFilter ref="A7:G89" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -4529,23 +4618,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="60" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4643,7 +4732,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -4660,7 +4749,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -4677,7 +4766,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -4721,7 +4810,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -4755,7 +4844,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -4789,7 +4878,7 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -4806,7 +4895,7 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -5019,7 +5108,7 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
@@ -5038,7 +5127,7 @@
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
         <v>161</v>
@@ -5057,7 +5146,7 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>46</v>
       </c>
@@ -5114,7 +5203,7 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>165</v>
@@ -5184,7 +5273,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
         <v>169</v>
@@ -5345,7 +5434,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>258</v>
       </c>
@@ -5446,7 +5535,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>46</v>
       </c>
@@ -5471,7 +5560,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>305</v>
       </c>
@@ -5603,7 +5692,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>397</v>
       </c>
@@ -5615,7 +5704,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63"/>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -5625,27 +5714,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="41"/>
-    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="41"/>
-    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="41"/>
+    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="41"/>
+    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
@@ -5664,7 +5753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="62"/>
       <c r="C3" s="62"/>
       <c r="D3" s="62"/>
@@ -5673,7 +5762,7 @@
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="72" t="s">
         <v>366</v>
       </c>
@@ -5684,7 +5773,7 @@
       <c r="G4" s="73"/>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
         <v>367</v>
       </c>
@@ -5695,7 +5784,7 @@
       <c r="G5" s="74"/>
       <c r="H5" s="74"/>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -5704,12 +5793,12 @@
       <c r="G6" s="62"/>
       <c r="H6" s="62"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="42" t="s">
         <v>1</v>
       </c>
@@ -5735,7 +5824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="45" t="s">
         <v>58</v>
       </c>
@@ -5751,529 +5840,529 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="46"/>
       <c r="I91" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="46"/>
       <c r="I92" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="47"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="47"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="47"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="47"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="47"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="47"/>
     </row>
   </sheetData>
@@ -6288,24 +6377,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>382</v>
       </c>
@@ -6316,7 +6405,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>378</v>
       </c>
@@ -6354,7 +6443,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1117</v>
       </c>
@@ -6395,7 +6484,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1127</v>
       </c>
@@ -6436,7 +6525,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1137</v>
       </c>
@@ -6477,7 +6566,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1139</v>
       </c>
@@ -6518,7 +6607,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1141</v>
       </c>
@@ -6562,7 +6651,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>429</v>
       </c>
@@ -6603,7 +6692,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1144</v>
       </c>
@@ -6644,7 +6733,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>435</v>
       </c>
@@ -6685,7 +6774,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1145</v>
       </c>
@@ -6726,7 +6815,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>441</v>
       </c>
@@ -6743,7 +6832,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>444</v>
       </c>
@@ -6754,7 +6843,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>445</v>
       </c>
@@ -6762,7 +6851,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1153</v>
       </c>
@@ -6803,7 +6892,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>457</v>
       </c>
@@ -6844,7 +6933,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>444</v>
       </c>
@@ -6885,7 +6974,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>460</v>
       </c>
@@ -6926,7 +7015,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1154</v>
       </c>
@@ -6967,7 +7056,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>473</v>
       </c>
@@ -7008,7 +7097,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1160</v>
       </c>
@@ -7049,7 +7138,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1167</v>
       </c>
@@ -7090,7 +7179,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>496</v>
       </c>
@@ -7131,7 +7220,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>497</v>
       </c>
@@ -7172,7 +7261,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>488</v>
       </c>
@@ -7213,7 +7302,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>493</v>
       </c>
@@ -7254,7 +7343,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1173</v>
       </c>
@@ -7295,7 +7384,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>488</v>
       </c>
@@ -7336,7 +7425,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>496</v>
       </c>
@@ -7377,7 +7466,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>497</v>
       </c>
@@ -7418,7 +7507,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>493</v>
       </c>
@@ -7458,6 +7547,184 @@
       <c r="N35" s="63" t="s">
         <v>505</v>
       </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1177</v>
+      </c>
+      <c r="C36" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="D36" s="63" t="s">
+        <v>513</v>
+      </c>
+      <c r="E36" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F36" s="63" t="s">
+        <v>514</v>
+      </c>
+      <c r="G36" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H36" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="I36" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J36" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K36" s="63" t="s">
+        <v>517</v>
+      </c>
+      <c r="L36" s="63" t="s">
+        <v>518</v>
+      </c>
+      <c r="M36" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N36" s="63" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="77" t="s">
+        <v>488</v>
+      </c>
+      <c r="C37" s="78" t="s">
+        <v>500</v>
+      </c>
+      <c r="D37" s="78" t="s">
+        <v>520</v>
+      </c>
+      <c r="E37" s="78" t="s">
+        <v>387</v>
+      </c>
+      <c r="F37" s="78" t="s">
+        <v>521</v>
+      </c>
+      <c r="G37" s="78" t="s">
+        <v>403</v>
+      </c>
+      <c r="H37" s="78" t="s">
+        <v>404</v>
+      </c>
+      <c r="I37" s="78" t="s">
+        <v>515</v>
+      </c>
+      <c r="J37" s="78" t="s">
+        <v>516</v>
+      </c>
+      <c r="K37" s="78" t="s">
+        <v>517</v>
+      </c>
+      <c r="L37" s="78" t="s">
+        <v>522</v>
+      </c>
+      <c r="M37" s="78" t="s">
+        <v>393</v>
+      </c>
+      <c r="N37" s="78" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="75" t="s">
+        <v>496</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>500</v>
+      </c>
+      <c r="D38" s="76" t="s">
+        <v>513</v>
+      </c>
+      <c r="E38" s="76" t="s">
+        <v>387</v>
+      </c>
+      <c r="F38" s="76" t="s">
+        <v>514</v>
+      </c>
+      <c r="G38" s="76" t="s">
+        <v>403</v>
+      </c>
+      <c r="H38" s="76" t="s">
+        <v>404</v>
+      </c>
+      <c r="I38" s="76" t="s">
+        <v>515</v>
+      </c>
+      <c r="J38" s="76" t="s">
+        <v>516</v>
+      </c>
+      <c r="K38" s="76" t="s">
+        <v>517</v>
+      </c>
+      <c r="L38" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="M38" s="76" t="s">
+        <v>393</v>
+      </c>
+      <c r="N38" s="76" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="75" t="s">
+        <v>497</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>500</v>
+      </c>
+      <c r="D39" s="76" t="s">
+        <v>524</v>
+      </c>
+      <c r="E39" s="76" t="s">
+        <v>387</v>
+      </c>
+      <c r="F39" s="76" t="s">
+        <v>525</v>
+      </c>
+      <c r="G39" s="76" t="s">
+        <v>403</v>
+      </c>
+      <c r="H39" s="76" t="s">
+        <v>404</v>
+      </c>
+      <c r="I39" s="76" t="s">
+        <v>515</v>
+      </c>
+      <c r="J39" s="76" t="s">
+        <v>516</v>
+      </c>
+      <c r="K39" s="76" t="s">
+        <v>517</v>
+      </c>
+      <c r="L39" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="M39" s="76" t="s">
+        <v>393</v>
+      </c>
+      <c r="N39" s="76" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="63"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated mem page for Build 1182
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\AppleWin\A2osX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E369F9C5-CB7E-4A38-B727-C69C983A1E54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="10875" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="181029" calcMode="manual"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,12 +31,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Patrick</author>
+    <author>Patrick Kloepfer</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="B28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="B34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{DFC45764-65D1-4338-A5B1-FC654D41C384}">
+    <comment ref="B39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -109,12 +109,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B45" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick Kloepfer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+loaded after NETD not manual net load</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="544">
   <si>
     <t>Issue No.</t>
   </si>
@@ -1802,15 +1826,69 @@
   <si>
     <t>12668</t>
   </si>
+  <si>
+    <t>Add an option for shell scripts like SET -X, called SET -C that will disable Control-C from exiting this Script or ANY script it calls.</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>$1FFB</t>
+  </si>
+  <si>
+    <t>26373</t>
+  </si>
+  <si>
+    <t>$ECED</t>
+  </si>
+  <si>
+    <t>$EE19</t>
+  </si>
+  <si>
+    <t>04577</t>
+  </si>
+  <si>
+    <t>16901</t>
+  </si>
+  <si>
+    <t>$F0BD</t>
+  </si>
+  <si>
+    <t>03901</t>
+  </si>
+  <si>
+    <t>$56E0</t>
+  </si>
+  <si>
+    <t>14053</t>
+  </si>
+  <si>
+    <t>12645</t>
+  </si>
+  <si>
+    <t>Kill telnetd</t>
+  </si>
+  <si>
+    <t>Kill networkd</t>
+  </si>
+  <si>
+    <t>$6400</t>
+  </si>
+  <si>
+    <t>17621</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1903,6 +1981,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2306,6 +2397,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2317,14 +2416,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2639,12 +2730,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A95" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96:F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,7 +3104,7 @@
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1">
         <f>B19+1</f>
@@ -4600,8 +4691,22 @@
         <v>1163</v>
       </c>
     </row>
+    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B96" s="1">
+        <v>187</v>
+      </c>
+      <c r="C96" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G89" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A7:G89">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -4618,7 +4723,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -5704,7 +5809,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:G63"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -5714,7 +5819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5740,15 +5845,15 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="75" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>
@@ -5763,26 +5868,26 @@
       <c r="H3" s="62"/>
     </row>
     <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="76" t="s">
         <v>366</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="76" t="s">
         <v>367</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="62"/>
@@ -6377,16 +6482,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A3:N40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7590,141 +7695,458 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="77" t="s">
+      <c r="B37" s="73" t="s">
         <v>488</v>
       </c>
-      <c r="C37" s="78" t="s">
+      <c r="C37" s="74" t="s">
         <v>500</v>
       </c>
-      <c r="D37" s="78" t="s">
+      <c r="D37" s="74" t="s">
         <v>520</v>
       </c>
-      <c r="E37" s="78" t="s">
+      <c r="E37" s="74" t="s">
         <v>387</v>
       </c>
-      <c r="F37" s="78" t="s">
+      <c r="F37" s="74" t="s">
         <v>521</v>
       </c>
-      <c r="G37" s="78" t="s">
+      <c r="G37" s="74" t="s">
         <v>403</v>
       </c>
-      <c r="H37" s="78" t="s">
+      <c r="H37" s="74" t="s">
         <v>404</v>
       </c>
-      <c r="I37" s="78" t="s">
+      <c r="I37" s="74" t="s">
         <v>515</v>
       </c>
-      <c r="J37" s="78" t="s">
+      <c r="J37" s="74" t="s">
         <v>516</v>
       </c>
-      <c r="K37" s="78" t="s">
+      <c r="K37" s="74" t="s">
         <v>517</v>
       </c>
-      <c r="L37" s="78" t="s">
+      <c r="L37" s="74" t="s">
         <v>522</v>
       </c>
-      <c r="M37" s="78" t="s">
+      <c r="M37" s="74" t="s">
         <v>393</v>
       </c>
-      <c r="N37" s="78" t="s">
+      <c r="N37" s="74" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="71" t="s">
         <v>496</v>
       </c>
-      <c r="C38" s="76" t="s">
+      <c r="C38" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="D38" s="76" t="s">
+      <c r="D38" s="72" t="s">
         <v>513</v>
       </c>
-      <c r="E38" s="76" t="s">
+      <c r="E38" s="72" t="s">
         <v>387</v>
       </c>
-      <c r="F38" s="76" t="s">
+      <c r="F38" s="72" t="s">
         <v>514</v>
       </c>
-      <c r="G38" s="76" t="s">
+      <c r="G38" s="72" t="s">
         <v>403</v>
       </c>
-      <c r="H38" s="76" t="s">
+      <c r="H38" s="72" t="s">
         <v>404</v>
       </c>
-      <c r="I38" s="76" t="s">
+      <c r="I38" s="72" t="s">
         <v>515</v>
       </c>
-      <c r="J38" s="76" t="s">
+      <c r="J38" s="72" t="s">
         <v>516</v>
       </c>
-      <c r="K38" s="76" t="s">
+      <c r="K38" s="72" t="s">
         <v>517</v>
       </c>
-      <c r="L38" s="76" t="s">
+      <c r="L38" s="72" t="s">
         <v>522</v>
       </c>
-      <c r="M38" s="76" t="s">
+      <c r="M38" s="72" t="s">
         <v>393</v>
       </c>
-      <c r="N38" s="76" t="s">
+      <c r="N38" s="72" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="71" t="s">
         <v>497</v>
       </c>
-      <c r="C39" s="76" t="s">
+      <c r="C39" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="D39" s="76" t="s">
+      <c r="D39" s="72" t="s">
         <v>524</v>
       </c>
-      <c r="E39" s="76" t="s">
+      <c r="E39" s="72" t="s">
         <v>387</v>
       </c>
-      <c r="F39" s="76" t="s">
+      <c r="F39" s="72" t="s">
         <v>525</v>
       </c>
-      <c r="G39" s="76" t="s">
+      <c r="G39" s="72" t="s">
         <v>403</v>
       </c>
-      <c r="H39" s="76" t="s">
+      <c r="H39" s="72" t="s">
         <v>404</v>
       </c>
-      <c r="I39" s="76" t="s">
+      <c r="I39" s="72" t="s">
         <v>515</v>
       </c>
-      <c r="J39" s="76" t="s">
+      <c r="J39" s="72" t="s">
         <v>516</v>
       </c>
-      <c r="K39" s="76" t="s">
+      <c r="K39" s="72" t="s">
         <v>517</v>
       </c>
-      <c r="L39" s="76" t="s">
+      <c r="L39" s="72" t="s">
         <v>522</v>
       </c>
-      <c r="M39" s="76" t="s">
+      <c r="M39" s="72" t="s">
         <v>393</v>
       </c>
-      <c r="N39" s="76" t="s">
+      <c r="N39" s="72" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="63"/>
-      <c r="K40" s="63"/>
-      <c r="L40" s="63"/>
-      <c r="M40" s="63"/>
-      <c r="N40" s="63"/>
+      <c r="A40">
+        <v>1182</v>
+      </c>
+      <c r="B40" t="s">
+        <v>528</v>
+      </c>
+      <c r="C40" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D40" s="63" t="s">
+        <v>513</v>
+      </c>
+      <c r="E40" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F40" s="63" t="s">
+        <v>530</v>
+      </c>
+      <c r="G40" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H40" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I40" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J40" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K40" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L40" s="63" t="s">
+        <v>532</v>
+      </c>
+      <c r="M40" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N40" s="63" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>527</v>
+      </c>
+      <c r="C41" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D41" s="63" t="s">
+        <v>513</v>
+      </c>
+      <c r="E41" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F41" s="63" t="s">
+        <v>530</v>
+      </c>
+      <c r="G41" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H41" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I41" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J41" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K41" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L41" s="63" t="s">
+        <v>532</v>
+      </c>
+      <c r="M41" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N41" s="63" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>488</v>
+      </c>
+      <c r="C42" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D42" s="63" t="s">
+        <v>520</v>
+      </c>
+      <c r="E42" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F42" s="63" t="s">
+        <v>534</v>
+      </c>
+      <c r="G42" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H42" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I42" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J42" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K42" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L42" s="63" t="s">
+        <v>535</v>
+      </c>
+      <c r="M42" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N42" s="63" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>496</v>
+      </c>
+      <c r="C43" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D43" s="63" t="s">
+        <v>513</v>
+      </c>
+      <c r="E43" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F43" s="63" t="s">
+        <v>530</v>
+      </c>
+      <c r="G43" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H43" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I43" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J43" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K43" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L43" s="63" t="s">
+        <v>535</v>
+      </c>
+      <c r="M43" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N43" s="63" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>497</v>
+      </c>
+      <c r="C44" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D44" s="63" t="s">
+        <v>524</v>
+      </c>
+      <c r="E44" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F44" s="63" t="s">
+        <v>539</v>
+      </c>
+      <c r="G44" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H44" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I44" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J44" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K44" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L44" s="63" t="s">
+        <v>535</v>
+      </c>
+      <c r="M44" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N44" s="63" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>493</v>
+      </c>
+      <c r="C45" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D45" s="63" t="s">
+        <v>537</v>
+      </c>
+      <c r="E45" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F45" s="63" t="s">
+        <v>538</v>
+      </c>
+      <c r="G45" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H45" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I45" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J45" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K45" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L45" s="63" t="s">
+        <v>535</v>
+      </c>
+      <c r="M45" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N45" s="63" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>540</v>
+      </c>
+      <c r="C46" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D46" s="63" t="s">
+        <v>520</v>
+      </c>
+      <c r="E46" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F46" s="63" t="s">
+        <v>534</v>
+      </c>
+      <c r="G46" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H46" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I46" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J46" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K46" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L46" s="63" t="s">
+        <v>535</v>
+      </c>
+      <c r="M46" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N46" s="63" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>541</v>
+      </c>
+      <c r="C47" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D47" s="63" t="s">
+        <v>542</v>
+      </c>
+      <c r="E47" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="F47" s="63" t="s">
+        <v>543</v>
+      </c>
+      <c r="G47" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="H47" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I47" s="63" t="s">
+        <v>515</v>
+      </c>
+      <c r="J47" s="63" t="s">
+        <v>516</v>
+      </c>
+      <c r="K47" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="L47" s="63" t="s">
+        <v>535</v>
+      </c>
+      <c r="M47" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="N47" s="63" t="s">
+        <v>536</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kernel 0.92, /DEV/NULL fix
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10880"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -18,10 +13,10 @@
     <sheet name="Memory" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$102</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="145621" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +32,7 @@
     <author>Patrick Kloepfer</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0" shapeId="0">
+    <comment ref="B34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0">
+    <comment ref="B39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="1" shapeId="0">
+    <comment ref="B45" authorId="1">
       <text>
         <r>
           <rPr>
@@ -117,7 +112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patrick Kloepfer:</t>
         </r>
@@ -126,7 +121,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 loaded after NETD not manual net load</t>
@@ -1920,11 +1915,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2017,19 +2012,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -2461,7 +2443,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2473,18 +2455,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2505,6 +2475,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2811,7 +2793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2819,25 +2801,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="27" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
@@ -2852,7 +2835,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>55</v>
@@ -2865,7 +2848,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>121</v>
@@ -2878,7 +2861,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>53</v>
@@ -2891,12 +2874,12 @@
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
@@ -2919,7 +2902,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2940,7 +2923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2962,7 +2945,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -2984,7 +2967,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -3008,7 +2991,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -3032,7 +3015,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -3056,7 +3039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -3078,7 +3061,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -3097,7 +3080,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -3119,7 +3102,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -3143,7 +3126,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -3165,7 +3148,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -3189,7 +3172,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3213,7 +3196,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -3235,7 +3218,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="217.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -3257,7 +3240,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -3281,7 +3264,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -3303,7 +3286,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -3327,7 +3310,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -3348,7 +3331,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -3372,7 +3355,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -3396,7 +3379,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -3420,7 +3403,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -3444,7 +3427,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>46</v>
       </c>
@@ -3468,7 +3451,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -3492,7 +3475,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -3516,7 +3499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
@@ -3540,7 +3523,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -3564,7 +3547,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
@@ -3585,7 +3568,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -3609,7 +3592,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -3633,7 +3616,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3657,7 +3640,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -3678,7 +3661,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -3702,7 +3685,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -3723,7 +3706,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -3747,7 +3730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>121</v>
       </c>
@@ -3768,7 +3751,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>121</v>
       </c>
@@ -3792,7 +3775,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -3816,7 +3799,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -3840,7 +3823,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -3864,7 +3847,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -3888,7 +3871,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
@@ -3912,7 +3895,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
@@ -3936,7 +3919,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -3960,7 +3943,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>46</v>
       </c>
@@ -3978,7 +3961,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>46</v>
       </c>
@@ -3999,7 +3982,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>46</v>
       </c>
@@ -4020,7 +4003,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>46</v>
       </c>
@@ -4041,7 +4024,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>46</v>
       </c>
@@ -4065,7 +4048,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>46</v>
       </c>
@@ -4085,7 +4068,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -4105,7 +4088,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>46</v>
       </c>
@@ -4125,7 +4108,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>46</v>
       </c>
@@ -4148,7 +4131,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>53</v>
       </c>
@@ -4168,7 +4151,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>46</v>
       </c>
@@ -4188,7 +4171,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>53</v>
       </c>
@@ -4211,7 +4194,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>46</v>
       </c>
@@ -4231,7 +4214,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>46</v>
       </c>
@@ -4251,7 +4234,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>326</v>
       </c>
@@ -4274,7 +4257,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>46</v>
       </c>
@@ -4294,7 +4277,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B69" s="1">
         <v>161</v>
       </c>
@@ -4314,7 +4297,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -4334,7 +4317,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B71" s="1">
         <v>163</v>
       </c>
@@ -4348,7 +4331,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>46</v>
       </c>
@@ -4365,7 +4348,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>53</v>
       </c>
@@ -4382,7 +4365,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>46</v>
       </c>
@@ -4399,7 +4382,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>53</v>
       </c>
@@ -4419,7 +4402,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>46</v>
       </c>
@@ -4436,7 +4419,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>46</v>
       </c>
@@ -4459,7 +4442,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>46</v>
       </c>
@@ -4480,7 +4463,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -4497,7 +4480,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>46</v>
       </c>
@@ -4520,7 +4503,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>46</v>
       </c>
@@ -4540,7 +4523,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>46</v>
       </c>
@@ -4560,7 +4543,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>46</v>
       </c>
@@ -4583,7 +4566,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>46</v>
       </c>
@@ -4603,7 +4586,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>53</v>
       </c>
@@ -4622,8 +4605,11 @@
       <c r="F85" s="39" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>46</v>
       </c>
@@ -4646,7 +4632,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>46</v>
       </c>
@@ -4669,7 +4655,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B88" s="1">
         <v>179</v>
       </c>
@@ -4682,8 +4668,11 @@
       <c r="E88" s="3" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>46</v>
       </c>
@@ -4703,7 +4692,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>46</v>
       </c>
@@ -4726,7 +4715,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -4749,7 +4738,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>46</v>
       </c>
@@ -4772,30 +4761,30 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A93" s="75" t="s">
+    <row r="93" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="B93" s="76">
+      <c r="B93" s="72">
         <v>184</v>
       </c>
-      <c r="C93" s="77" t="s">
+      <c r="C93" s="73" t="s">
         <v>476</v>
       </c>
-      <c r="D93" s="78">
+      <c r="D93" s="74">
         <v>1160</v>
       </c>
-      <c r="E93" s="79" t="s">
+      <c r="E93" s="75" t="s">
         <v>477</v>
       </c>
-      <c r="F93" s="80" t="s">
+      <c r="F93" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="G93" s="81">
+      <c r="G93" s="77">
         <v>1163</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>46</v>
       </c>
@@ -4818,7 +4807,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>46</v>
       </c>
@@ -4834,14 +4823,14 @@
       <c r="E95" s="66" t="s">
         <v>481</v>
       </c>
-      <c r="F95" s="80" t="s">
+      <c r="F95" s="76" t="s">
         <v>54</v>
       </c>
       <c r="G95">
         <v>1163</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B96" s="1">
         <v>187</v>
       </c>
@@ -4854,8 +4843,11 @@
       <c r="F96" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B97" s="1">
         <v>188</v>
       </c>
@@ -4869,7 +4861,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>46</v>
       </c>
@@ -4889,7 +4881,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B99" s="1">
         <v>190</v>
       </c>
@@ -4903,7 +4895,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B100" s="1">
         <v>191</v>
       </c>
@@ -4917,7 +4909,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="B101" s="1">
         <v>192</v>
       </c>
@@ -4931,7 +4923,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B102" s="1">
         <v>193</v>
       </c>
@@ -4944,9 +4936,19 @@
       <c r="E102" s="3" t="s">
         <v>555</v>
       </c>
+      <c r="G102">
+        <v>1186</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G96"/>
+  <autoFilter ref="A7:G102">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="D"/>
+        <filter val="V"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -4963,16 +4965,16 @@
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="60" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.7109375" style="4"/>
+    <col min="1" max="1" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="52.26953125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" style="60" customWidth="1"/>
+    <col min="6" max="6" width="38.1796875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.81640625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -5070,7 +5072,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
         <v>66</v>
@@ -5087,7 +5089,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
@@ -5104,7 +5106,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -5148,7 +5150,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37" t="s">
         <v>77</v>
@@ -5182,7 +5184,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="37" t="s">
         <v>83</v>
@@ -5216,7 +5218,7 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="37" t="s">
         <v>90</v>
@@ -5233,7 +5235,7 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="36"/>
       <c r="B15" s="37" t="s">
         <v>93</v>
@@ -5446,7 +5448,7 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="36"/>
       <c r="B26" s="37" t="s">
         <v>108</v>
@@ -5465,7 +5467,7 @@
       </c>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A27" s="36"/>
       <c r="B27" s="37" t="s">
         <v>161</v>
@@ -5484,7 +5486,7 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>46</v>
       </c>
@@ -5541,7 +5543,7 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>165</v>
@@ -5611,7 +5613,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
       <c r="B35" s="37" t="s">
         <v>169</v>
@@ -5772,7 +5774,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>257</v>
       </c>
@@ -5873,7 +5875,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>46</v>
       </c>
@@ -5898,7 +5900,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>303</v>
       </c>
@@ -6059,39 +6061,39 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="40" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" style="40" customWidth="1"/>
     <col min="3" max="3" width="8" style="41" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="41"/>
-    <col min="6" max="6" width="5.85546875" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="41"/>
-    <col min="8" max="8" width="52.140625" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="41"/>
+    <col min="4" max="4" width="5.1796875" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="41"/>
+    <col min="6" max="6" width="5.81640625" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="41"/>
+    <col min="8" max="8" width="52.1796875" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="I1" s="41" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="78" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
       <c r="I2" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="62"/>
       <c r="C3" s="62"/>
       <c r="D3" s="62"/>
@@ -6100,29 +6102,29 @@
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
     </row>
-    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="72" t="s">
+    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="79" t="s">
         <v>363</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-    </row>
-    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="72" t="s">
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+    </row>
+    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="79" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+    </row>
+    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -6131,12 +6133,12 @@
       <c r="G6" s="62"/>
       <c r="H6" s="62"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="I7" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="42" t="s">
         <v>1</v>
       </c>
@@ -6162,7 +6164,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="45" t="s">
         <v>58</v>
       </c>
@@ -6178,529 +6180,529 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="I11" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="I12" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="I13" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="I14" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
       <c r="I18" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
       <c r="I19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
       <c r="I20" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
       <c r="I21" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
       <c r="I22" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
       <c r="I23" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="I24" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
       <c r="I25" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
       <c r="I26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
       <c r="I27" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
       <c r="I28" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="6"/>
       <c r="I29" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
       <c r="I30" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="6"/>
       <c r="I31" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="6"/>
       <c r="I32" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
       <c r="I33" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="6"/>
       <c r="I34" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
       <c r="I35" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="6"/>
       <c r="I36" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="6"/>
       <c r="I37" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="6"/>
       <c r="I38" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" s="6"/>
       <c r="I39" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="6"/>
       <c r="I40" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" s="6"/>
       <c r="I41" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
       <c r="I42" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B43" s="6"/>
       <c r="I43" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I44" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" s="6"/>
       <c r="I45" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" s="6"/>
       <c r="I46" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="6"/>
       <c r="I47" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" s="6"/>
       <c r="I48" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="6"/>
       <c r="I49" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" s="6"/>
       <c r="I50" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" s="6"/>
       <c r="I51" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="6"/>
       <c r="I52" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="6"/>
       <c r="I53" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="6"/>
       <c r="I54" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" s="6"/>
       <c r="I55" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="6"/>
       <c r="I56" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="6"/>
       <c r="I57" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" s="6"/>
       <c r="I58" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="6"/>
       <c r="I59" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="6"/>
       <c r="I60" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="6"/>
       <c r="I61" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="6"/>
       <c r="I62" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="6"/>
       <c r="I63" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" s="6"/>
       <c r="I64" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B65" s="6"/>
       <c r="I65" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B66" s="6"/>
       <c r="I66" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67" s="6"/>
       <c r="I67" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" s="6"/>
       <c r="I68" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B69" s="6"/>
       <c r="I69" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70" s="6"/>
       <c r="I70" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B71" s="6"/>
       <c r="I71" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B72" s="6"/>
       <c r="I72" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73" s="6"/>
       <c r="I73" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" s="6"/>
       <c r="I74" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" s="6"/>
       <c r="I75" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B76" s="6"/>
       <c r="I76" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" s="6"/>
       <c r="I77" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" s="6"/>
       <c r="I78" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B79" s="6"/>
       <c r="I79" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" s="6"/>
       <c r="I80" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B81" s="6"/>
       <c r="I81" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82" s="6"/>
       <c r="I82" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B83" s="6"/>
       <c r="I83" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84" s="6"/>
       <c r="I84" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B85" s="6"/>
       <c r="I85" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B86" s="6"/>
       <c r="I86" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B87" s="6"/>
       <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B88" s="6"/>
       <c r="I88" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B89" s="6"/>
       <c r="I89" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I90" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B91" s="46"/>
       <c r="I91" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B92" s="46"/>
       <c r="I92" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I93" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100" s="47"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101" s="47"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" s="47"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104" s="47"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105" s="47"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107" s="47"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B108" s="47"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110" s="47"/>
     </row>
   </sheetData>
@@ -6722,9 +6724,9 @@
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update with notes for 1203
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2181F006-25E4-426A-BC2A-6EE24803E4BB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10880"/>
+    <workbookView xWindow="555" yWindow="1290" windowWidth="14580" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +32,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Patrick</author>
     <author>Patrick Kloepfer</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="1">
+    <comment ref="B45" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +134,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="1">
+    <comment ref="B53" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick Kloepfer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+loaded after NETD not manual net load</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B61" authorId="1" shapeId="0" xr:uid="{D349E2A6-487F-4F50-B3CE-FEE69E393416}">
       <text>
         <r>
           <rPr>
@@ -157,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="634">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2156,13 +2186,40 @@
   <si>
     <t>PK to check all commands for -H and update Commands page of this doc (DONE!).  PK to attempt to add -H option to CAT and others following code in MORE.</t>
   </si>
+  <si>
+    <t>$EBA4</t>
+  </si>
+  <si>
+    <t>$ECD0</t>
+  </si>
+  <si>
+    <t>04906</t>
+  </si>
+  <si>
+    <t>$6100</t>
+  </si>
+  <si>
+    <t>16645</t>
+  </si>
+  <si>
+    <t>$EF74</t>
+  </si>
+  <si>
+    <t>04230</t>
+  </si>
+  <si>
+    <t>CD ../etc returns FreeMem:$E4=Bad,/A2OSX.BUILD/BIN/SHELL and then lock of AW.  Run TESTS in root which includes a CD command will lock system.  CD .. Same result.  Only CD by itself will avoid a lock.  Since CD does not work at all, running other tests becomes difficult.  Pushdpopdtest failed because it includes CD.</t>
+  </si>
+  <si>
+    <t>READTEST showing failures (test of READ command).  After input of "Patrick" echo of read var says "PatrickE" Run again, input "Pat" echo back of "PatPickE" Run again, input "Remy" return "RemyPckE"  notice the pattern of ending P and E.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2567,7 +2624,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -3039,35 +3096,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="36" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="37" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="37" customWidth="1"/>
     <col min="3" max="3" width="14" style="38" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="36" customWidth="1"/>
     <col min="5" max="5" width="44" style="39" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="39" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" style="40" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="40"/>
+    <col min="6" max="6" width="34.28515625" style="39" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="40" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>62</v>
       </c>
@@ -3082,7 +3139,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="45"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47" t="s">
         <v>55</v>
@@ -3095,7 +3152,7 @@
       <c r="F3" s="49"/>
       <c r="G3" s="50"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="46"/>
       <c r="B4" s="47" t="s">
         <v>121</v>
@@ -3108,7 +3165,7 @@
       <c r="F4" s="49"/>
       <c r="G4" s="50"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="51"/>
       <c r="B5" s="52" t="s">
         <v>53</v>
@@ -3121,12 +3178,12 @@
       <c r="F5" s="54"/>
       <c r="G5" s="55"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
         <v>3</v>
       </c>
@@ -3149,7 +3206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -3170,7 +3227,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>46</v>
       </c>
@@ -3192,7 +3249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>55</v>
       </c>
@@ -3214,7 +3271,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>46</v>
       </c>
@@ -3327,7 +3384,7 @@
       </c>
       <c r="F15" s="38"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>46</v>
       </c>
@@ -3395,7 +3452,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>46</v>
       </c>
@@ -3419,7 +3476,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>46</v>
       </c>
@@ -3443,7 +3500,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
         <v>55</v>
       </c>
@@ -3465,7 +3522,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="217.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
         <v>46</v>
       </c>
@@ -3511,7 +3568,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>53</v>
       </c>
@@ -3533,7 +3590,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
         <v>46</v>
       </c>
@@ -3578,7 +3635,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
         <v>53</v>
       </c>
@@ -3602,7 +3659,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>46</v>
       </c>
@@ -3932,7 +3989,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
         <v>53</v>
       </c>
@@ -3953,7 +4010,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="36" t="s">
         <v>55</v>
       </c>
@@ -4046,7 +4103,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
         <v>46</v>
       </c>
@@ -4094,7 +4151,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
         <v>53</v>
       </c>
@@ -4118,7 +4175,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
         <v>46</v>
       </c>
@@ -4166,7 +4223,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="36" t="s">
         <v>46</v>
       </c>
@@ -4295,7 +4352,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>46</v>
       </c>
@@ -4378,7 +4435,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
         <v>53</v>
       </c>
@@ -4398,7 +4455,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="36" t="s">
         <v>46</v>
       </c>
@@ -4418,7 +4475,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="36" t="s">
         <v>53</v>
       </c>
@@ -4441,7 +4498,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="36" t="s">
         <v>46</v>
       </c>
@@ -4461,7 +4518,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="36" t="s">
         <v>46</v>
       </c>
@@ -4481,7 +4538,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="36" t="s">
         <v>325</v>
       </c>
@@ -4504,7 +4561,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="36" t="s">
         <v>46</v>
       </c>
@@ -4524,7 +4581,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B69" s="37">
         <v>161</v>
       </c>
@@ -4544,7 +4601,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="36" t="s">
         <v>46</v>
       </c>
@@ -4564,7 +4621,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B71" s="37">
         <v>163</v>
       </c>
@@ -4578,7 +4635,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="36" t="s">
         <v>46</v>
       </c>
@@ -4595,7 +4652,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="36" t="s">
         <v>53</v>
       </c>
@@ -4612,7 +4669,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="36" t="s">
         <v>46</v>
       </c>
@@ -4629,7 +4686,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="36" t="s">
         <v>53</v>
       </c>
@@ -4649,7 +4706,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="36" t="s">
         <v>46</v>
       </c>
@@ -4710,7 +4767,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="36" t="s">
         <v>53</v>
       </c>
@@ -4727,7 +4784,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
         <v>46</v>
       </c>
@@ -4833,7 +4890,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="36" t="s">
         <v>53</v>
       </c>
@@ -4856,7 +4913,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="36" t="s">
         <v>46</v>
       </c>
@@ -5083,7 +5140,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B96" s="37">
         <v>187</v>
       </c>
@@ -5100,7 +5157,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="36" t="s">
         <v>46</v>
       </c>
@@ -5140,7 +5197,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B99" s="37">
         <v>190</v>
       </c>
@@ -5154,7 +5211,10 @@
         <v>620</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A100" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="B100" s="37">
         <v>191</v>
       </c>
@@ -5171,7 +5231,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B101" s="37">
         <v>192</v>
       </c>
@@ -5191,7 +5251,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="36" t="s">
         <v>46</v>
       </c>
@@ -5214,7 +5274,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B103" s="37">
         <v>194</v>
       </c>
@@ -5228,7 +5288,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B104" s="37">
         <v>195</v>
       </c>
@@ -5245,7 +5305,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B105" s="37">
         <v>196</v>
       </c>
@@ -5262,7 +5322,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B106" s="37">
         <v>197</v>
       </c>
@@ -5276,7 +5336,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B107" s="37">
         <v>198</v>
       </c>
@@ -5290,7 +5350,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="B108" s="37">
         <v>199</v>
       </c>
@@ -5307,7 +5367,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B109" s="37">
         <v>200</v>
       </c>
@@ -5321,8 +5381,36 @@
         <v>614</v>
       </c>
     </row>
+    <row r="110" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B110" s="37">
+        <v>201</v>
+      </c>
+      <c r="C110" s="38" t="s">
+        <v>369</v>
+      </c>
+      <c r="D110" s="36">
+        <v>1203</v>
+      </c>
+      <c r="E110" s="39" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B111" s="37">
+        <v>202</v>
+      </c>
+      <c r="C111" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="D111" s="36">
+        <v>1203</v>
+      </c>
+      <c r="E111" s="39" t="s">
+        <v>633</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G109">
+  <autoFilter ref="A7:G109" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -5339,23 +5427,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -5453,7 +5541,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>66</v>
@@ -5470,7 +5558,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>46</v>
       </c>
@@ -5487,7 +5575,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>46</v>
       </c>
@@ -5531,7 +5619,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>77</v>
@@ -5565,7 +5653,7 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>83</v>
@@ -5599,7 +5687,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>90</v>
@@ -5616,7 +5704,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>93</v>
@@ -5829,7 +5917,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
         <v>108</v>
@@ -5848,7 +5936,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
         <v>160</v>
@@ -5867,7 +5955,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>46</v>
       </c>
@@ -5924,7 +6012,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
         <v>164</v>
@@ -5994,7 +6082,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
         <v>168</v>
@@ -6155,7 +6243,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>256</v>
       </c>
@@ -6256,7 +6344,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>46</v>
       </c>
@@ -6281,7 +6369,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>302</v>
       </c>
@@ -6425,7 +6513,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63"/>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -6435,27 +6523,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I110"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="13" customWidth="1"/>
     <col min="3" max="3" width="8" style="81" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="14"/>
-    <col min="6" max="6" width="5.81640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="81"/>
-    <col min="8" max="8" width="52.1796875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="14"/>
+    <col min="4" max="4" width="5.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="14"/>
+    <col min="6" max="6" width="5.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="81"/>
+    <col min="8" max="8" width="52.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="14" t="s">
         <v>28</v>
       </c>
@@ -6474,7 +6562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="27"/>
       <c r="C3" s="3"/>
       <c r="D3" s="27"/>
@@ -6483,7 +6571,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="84" t="s">
         <v>361</v>
       </c>
@@ -6494,7 +6582,7 @@
       <c r="G4" s="85"/>
       <c r="H4" s="85"/>
     </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="84" t="s">
         <v>362</v>
       </c>
@@ -6505,7 +6593,7 @@
       <c r="G5" s="86"/>
       <c r="H5" s="86"/>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27"/>
       <c r="C6" s="3"/>
       <c r="D6" s="27"/>
@@ -6514,12 +6602,12 @@
       <c r="G6" s="3"/>
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
@@ -6545,7 +6633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
@@ -6560,7 +6648,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>598</v>
       </c>
@@ -6571,7 +6659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>596</v>
       </c>
@@ -6582,7 +6670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>597</v>
       </c>
@@ -6593,7 +6681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>331</v>
       </c>
@@ -6604,7 +6692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>587</v>
       </c>
@@ -6615,7 +6703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -6626,7 +6714,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>202</v>
       </c>
@@ -6637,7 +6725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -6648,7 +6736,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -6662,7 +6750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>588</v>
       </c>
@@ -6673,7 +6761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>600</v>
       </c>
@@ -6684,7 +6772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>453</v>
       </c>
@@ -6695,7 +6783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>595</v>
       </c>
@@ -6709,7 +6797,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>601</v>
       </c>
@@ -6720,7 +6808,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
         <v>578</v>
       </c>
@@ -6731,7 +6819,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
@@ -6742,7 +6830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>603</v>
       </c>
@@ -6756,7 +6844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>586</v>
       </c>
@@ -6767,7 +6855,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>589</v>
       </c>
@@ -6781,7 +6869,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>604</v>
       </c>
@@ -6795,7 +6883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>39</v>
       </c>
@@ -6806,7 +6894,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>590</v>
       </c>
@@ -6820,7 +6908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>591</v>
       </c>
@@ -6834,7 +6922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>21</v>
       </c>
@@ -6845,7 +6933,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>592</v>
       </c>
@@ -6859,7 +6947,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>599</v>
       </c>
@@ -6873,7 +6961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>593</v>
       </c>
@@ -6887,7 +6975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>22</v>
       </c>
@@ -6898,7 +6986,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>23</v>
       </c>
@@ -6909,7 +6997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>594</v>
       </c>
@@ -6923,7 +7011,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>602</v>
       </c>
@@ -6937,7 +7025,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>152</v>
       </c>
@@ -6948,7 +7036,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>24</v>
       </c>
@@ -6959,7 +7047,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>30</v>
       </c>
@@ -6970,7 +7058,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>25</v>
       </c>
@@ -6981,7 +7069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>230</v>
       </c>
@@ -6992,7 +7080,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>58</v>
       </c>
@@ -7003,7 +7091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>26</v>
       </c>
@@ -7017,7 +7105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>287</v>
       </c>
@@ -7031,296 +7119,296 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="I49" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="I50" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="I51" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="I52" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="I53" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="I54" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="I55" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="I56" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="I57" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="I58" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="I59" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="I60" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="I61" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="I62" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="I63" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="I64" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="I65" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="I66" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="I67" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="I68" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="I69" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="I70" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="I71" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="I72" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="I73" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="I74" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
       <c r="I75" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="I76" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="I77" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="I78" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="I79" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="I80" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="I81" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="I82" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="I83" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
       <c r="I84" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="I85" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
       <c r="I86" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
       <c r="I87" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
       <c r="I88" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
       <c r="I89" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="19"/>
       <c r="I91" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="19"/>
       <c r="I92" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="20"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="20"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="20"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="20"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="20"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="20"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="20"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="20"/>
     </row>
   </sheetData>
@@ -7338,24 +7426,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>377</v>
       </c>
@@ -7366,7 +7454,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>373</v>
       </c>
@@ -7404,7 +7492,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1117</v>
       </c>
@@ -7445,7 +7533,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1127</v>
       </c>
@@ -7486,7 +7574,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1137</v>
       </c>
@@ -7527,7 +7615,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1139</v>
       </c>
@@ -7568,7 +7656,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1141</v>
       </c>
@@ -7612,7 +7700,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>422</v>
       </c>
@@ -7653,7 +7741,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1144</v>
       </c>
@@ -7694,7 +7782,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>428</v>
       </c>
@@ -7735,7 +7823,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1145</v>
       </c>
@@ -7776,7 +7864,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>434</v>
       </c>
@@ -7793,7 +7881,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>437</v>
       </c>
@@ -7804,7 +7892,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>438</v>
       </c>
@@ -7812,7 +7900,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1153</v>
       </c>
@@ -7853,7 +7941,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>450</v>
       </c>
@@ -7894,7 +7982,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>437</v>
       </c>
@@ -7935,7 +8023,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>453</v>
       </c>
@@ -7976,7 +8064,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1154</v>
       </c>
@@ -8017,7 +8105,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>466</v>
       </c>
@@ -8058,7 +8146,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1160</v>
       </c>
@@ -8099,7 +8187,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1167</v>
       </c>
@@ -8140,7 +8228,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>487</v>
       </c>
@@ -8181,7 +8269,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>488</v>
       </c>
@@ -8222,7 +8310,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>479</v>
       </c>
@@ -8263,7 +8351,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>484</v>
       </c>
@@ -8304,7 +8392,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1173</v>
       </c>
@@ -8345,7 +8433,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>479</v>
       </c>
@@ -8386,7 +8474,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>487</v>
       </c>
@@ -8427,7 +8515,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>488</v>
       </c>
@@ -8468,7 +8556,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>484</v>
       </c>
@@ -8509,7 +8597,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1177</v>
       </c>
@@ -8550,7 +8638,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="33" t="s">
         <v>479</v>
       </c>
@@ -8591,7 +8679,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="31" t="s">
         <v>487</v>
       </c>
@@ -8632,7 +8720,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="31" t="s">
         <v>488</v>
       </c>
@@ -8673,7 +8761,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1182</v>
       </c>
@@ -8717,7 +8805,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>518</v>
       </c>
@@ -8758,7 +8846,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>479</v>
       </c>
@@ -8799,7 +8887,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>487</v>
       </c>
@@ -8840,7 +8928,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>488</v>
       </c>
@@ -8881,7 +8969,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>484</v>
       </c>
@@ -8922,7 +9010,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>531</v>
       </c>
@@ -8963,7 +9051,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>532</v>
       </c>
@@ -9004,7 +9092,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1190</v>
       </c>
@@ -9048,7 +9136,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>518</v>
       </c>
@@ -9089,7 +9177,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>479</v>
       </c>
@@ -9130,7 +9218,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>487</v>
       </c>
@@ -9171,7 +9259,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>488</v>
       </c>
@@ -9212,7 +9300,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>484</v>
       </c>
@@ -9253,7 +9341,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>531</v>
       </c>
@@ -9294,7 +9382,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>532</v>
       </c>
@@ -9333,6 +9421,157 @@
       </c>
       <c r="N55" s="28" t="s">
         <v>573</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1203</v>
+      </c>
+      <c r="B56" t="s">
+        <v>519</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="E56" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="F56" s="28" t="s">
+        <v>566</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>506</v>
+      </c>
+      <c r="I56" s="28" t="s">
+        <v>506</v>
+      </c>
+      <c r="J56" s="28" t="s">
+        <v>507</v>
+      </c>
+      <c r="K56" s="28" t="s">
+        <v>625</v>
+      </c>
+      <c r="L56" s="28" t="s">
+        <v>626</v>
+      </c>
+      <c r="M56" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="N56" s="28" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>518</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>566</v>
+      </c>
+      <c r="G57" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="H57" s="28" t="s">
+        <v>506</v>
+      </c>
+      <c r="I57" s="28" t="s">
+        <v>506</v>
+      </c>
+      <c r="J57" s="28" t="s">
+        <v>507</v>
+      </c>
+      <c r="K57" s="28" t="s">
+        <v>625</v>
+      </c>
+      <c r="L57" s="28" t="s">
+        <v>626</v>
+      </c>
+      <c r="M57" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="N57" s="28" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>479</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="G58" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="H58" s="28" t="s">
+        <v>506</v>
+      </c>
+      <c r="I58" s="28" t="s">
+        <v>506</v>
+      </c>
+      <c r="J58" s="28" t="s">
+        <v>507</v>
+      </c>
+      <c r="K58" s="28" t="s">
+        <v>625</v>
+      </c>
+      <c r="L58" s="28" t="s">
+        <v>630</v>
+      </c>
+      <c r="M58" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="N58" s="28" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MAKE and many TESTS as well as the Issue List with items reported recently.  The syntax errors are causing the most problems as they are breaking almost all the new tests.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19252B53-84FD-4B01-840D-175A4E5F5915}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1290" windowWidth="14580" windowHeight="10880"/>
+    <workbookView xWindow="975" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +32,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Patrick</author>
     <author>Patrick Kloepfer</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="1">
+    <comment ref="B45" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="1">
+    <comment ref="B53" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -152,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B61" authorId="1">
+    <comment ref="B61" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="640">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2207,13 +2213,31 @@
   <si>
     <t>READTEST showing failures (test of READ command).  After input of "Patrick" echo of read var says "PatrickE" Run again, input "Pat" echo back of "PatPickE" Run again, input "Remy" return "RemyPckE"  notice the pattern of ending P and E.</t>
   </si>
+  <si>
+    <t>Boot BUILD.  CD to /PKA2OSX/TESTS and then run RCTEST.  The test ends with some LIB/GUI garbage on screen that is nowhere in script and the script does not even complete, it terminates after the RCSUB1 step.  You get a PATH not found and FreeMem error.  If you immediately run the command again, you do not get the same trash on the screen, but the test still terminates early after running RCSUB1.</t>
+  </si>
+  <si>
+    <t>SHELL Redirection</t>
+  </si>
+  <si>
+    <t>Redirection does not seem to be working.  Check /MAKE/USR/SHARE/TESTS/MAKECHAR</t>
+  </si>
+  <si>
+    <t>I updated RCTEST in /MAKE/USR/SHARE/TESTS and tried running this version.  It stops on the line LS /RAM4 2&gt; /DEV/NULL saying "NO Device".  This does not occur in the PKA2OSX version and the only real difference between the scripts is the old version has a SET -X at top.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELL </t>
+  </si>
+  <si>
+    <t>In MAKE..TESTS is a new TESTMENU.  When you select choice 1 the command CORETEST (another script) gives you a syntax error.  If you type CORETEST at prompt it runs.  However, at the READ test, you enter Y, you get another Expression Syntax Error.   Update: Select choice 6 and you still get the CORETEST syntax error.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2618,7 +2642,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -3090,35 +3114,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="36" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="37" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="37" customWidth="1"/>
     <col min="3" max="3" width="14" style="38" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="36" customWidth="1"/>
     <col min="5" max="5" width="44" style="39" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="39" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" style="40" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="40"/>
+    <col min="6" max="6" width="34.28515625" style="39" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="40" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>62</v>
       </c>
@@ -3133,7 +3157,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="45"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47" t="s">
         <v>55</v>
@@ -3146,7 +3170,7 @@
       <c r="F3" s="49"/>
       <c r="G3" s="50"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="46"/>
       <c r="B4" s="47" t="s">
         <v>121</v>
@@ -3177,7 +3201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
         <v>3</v>
       </c>
@@ -3200,7 +3224,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -3221,7 +3245,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>46</v>
       </c>
@@ -3378,7 +3402,7 @@
       </c>
       <c r="F15" s="38"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>46</v>
       </c>
@@ -3446,7 +3470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>46</v>
       </c>
@@ -4217,7 +4241,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="36" t="s">
         <v>46</v>
       </c>
@@ -4595,7 +4619,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="36" t="s">
         <v>46</v>
       </c>
@@ -4907,7 +4931,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="36" t="s">
         <v>46</v>
       </c>
@@ -5395,7 +5419,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B111" s="37">
         <v>202</v>
       </c>
@@ -5409,8 +5433,64 @@
         <v>633</v>
       </c>
     </row>
+    <row r="112" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="B112" s="37">
+        <v>203</v>
+      </c>
+      <c r="C112" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D112" s="36">
+        <v>1222</v>
+      </c>
+      <c r="E112" s="39" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B113" s="37">
+        <v>204</v>
+      </c>
+      <c r="C113" s="38" t="s">
+        <v>635</v>
+      </c>
+      <c r="D113" s="36">
+        <v>1222</v>
+      </c>
+      <c r="E113" s="39" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B114" s="37">
+        <v>205</v>
+      </c>
+      <c r="C114" s="38" t="s">
+        <v>635</v>
+      </c>
+      <c r="D114" s="36">
+        <v>1222</v>
+      </c>
+      <c r="E114" s="39" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B115" s="37">
+        <v>206</v>
+      </c>
+      <c r="C115" s="38" t="s">
+        <v>638</v>
+      </c>
+      <c r="D115" s="36">
+        <v>1222</v>
+      </c>
+      <c r="E115" s="39" t="s">
+        <v>639</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G109">
+  <autoFilter ref="A7:G109" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -5427,23 +5507,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -5541,7 +5621,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>66</v>
@@ -5558,7 +5638,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>46</v>
       </c>
@@ -5575,7 +5655,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>46</v>
       </c>
@@ -5619,7 +5699,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>77</v>
@@ -5653,7 +5733,7 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>83</v>
@@ -5687,7 +5767,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>90</v>
@@ -5704,7 +5784,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>93</v>
@@ -5917,7 +5997,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
         <v>108</v>
@@ -5936,7 +6016,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
         <v>160</v>
@@ -5955,7 +6035,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>46</v>
       </c>
@@ -6012,7 +6092,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
         <v>164</v>
@@ -6082,7 +6162,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
         <v>168</v>
@@ -6243,7 +6323,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>256</v>
       </c>
@@ -6344,7 +6424,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>46</v>
       </c>
@@ -6369,7 +6449,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>302</v>
       </c>
@@ -6501,7 +6581,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>392</v>
       </c>
@@ -6513,7 +6593,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63"/>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -6523,27 +6603,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I110"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="13" customWidth="1"/>
     <col min="3" max="3" width="8" style="81" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="14"/>
-    <col min="6" max="6" width="5.81640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="81"/>
-    <col min="8" max="8" width="52.1796875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="14"/>
+    <col min="4" max="4" width="5.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="14"/>
+    <col min="6" max="6" width="5.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="81"/>
+    <col min="8" max="8" width="52.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="14" t="s">
         <v>28</v>
       </c>
@@ -6562,7 +6642,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="27"/>
       <c r="C3" s="3"/>
       <c r="D3" s="27"/>
@@ -6571,7 +6651,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="84" t="s">
         <v>361</v>
       </c>
@@ -6582,7 +6662,7 @@
       <c r="G4" s="85"/>
       <c r="H4" s="85"/>
     </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="84" t="s">
         <v>362</v>
       </c>
@@ -6593,7 +6673,7 @@
       <c r="G5" s="86"/>
       <c r="H5" s="86"/>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27"/>
       <c r="C6" s="3"/>
       <c r="D6" s="27"/>
@@ -6602,12 +6682,12 @@
       <c r="G6" s="3"/>
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
@@ -6633,7 +6713,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
@@ -6648,7 +6728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>598</v>
       </c>
@@ -6659,7 +6739,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>596</v>
       </c>
@@ -6670,7 +6750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>597</v>
       </c>
@@ -6681,7 +6761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>331</v>
       </c>
@@ -6692,7 +6772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>587</v>
       </c>
@@ -6703,7 +6783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -6714,7 +6794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>202</v>
       </c>
@@ -6725,7 +6805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -6736,7 +6816,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -6750,7 +6830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>588</v>
       </c>
@@ -6761,7 +6841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>600</v>
       </c>
@@ -6772,7 +6852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>453</v>
       </c>
@@ -6783,7 +6863,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>595</v>
       </c>
@@ -6797,7 +6877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>601</v>
       </c>
@@ -6808,7 +6888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
         <v>578</v>
       </c>
@@ -6819,7 +6899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
@@ -6830,7 +6910,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>603</v>
       </c>
@@ -6844,7 +6924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>586</v>
       </c>
@@ -6855,7 +6935,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>589</v>
       </c>
@@ -6869,7 +6949,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>604</v>
       </c>
@@ -6883,7 +6963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>39</v>
       </c>
@@ -6894,7 +6974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>590</v>
       </c>
@@ -6908,7 +6988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>591</v>
       </c>
@@ -6922,7 +7002,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>21</v>
       </c>
@@ -6933,7 +7013,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>592</v>
       </c>
@@ -6947,7 +7027,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>599</v>
       </c>
@@ -6961,7 +7041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>593</v>
       </c>
@@ -6975,7 +7055,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>22</v>
       </c>
@@ -6986,7 +7066,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>23</v>
       </c>
@@ -6997,7 +7077,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>594</v>
       </c>
@@ -7011,7 +7091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>602</v>
       </c>
@@ -7025,7 +7105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>152</v>
       </c>
@@ -7036,7 +7116,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>24</v>
       </c>
@@ -7047,7 +7127,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>30</v>
       </c>
@@ -7058,7 +7138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>25</v>
       </c>
@@ -7069,7 +7149,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>230</v>
       </c>
@@ -7080,7 +7160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>58</v>
       </c>
@@ -7091,7 +7171,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>26</v>
       </c>
@@ -7105,7 +7185,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>287</v>
       </c>
@@ -7119,296 +7199,296 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="I49" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="I50" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="I51" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="I52" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="I53" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="I54" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="I55" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="I56" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="I57" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="I58" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="I59" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="I60" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="I61" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="I62" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="I63" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="I64" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="I65" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="I66" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="I67" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="I68" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="I69" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="I70" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="I71" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="I72" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="I73" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="I74" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
       <c r="I75" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="I76" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="I77" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="I78" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="I79" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="I80" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="I81" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="I82" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="I83" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
       <c r="I84" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="I85" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
       <c r="I86" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
       <c r="I87" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
       <c r="I88" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
       <c r="I89" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="19"/>
       <c r="I91" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="19"/>
       <c r="I92" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="20"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="20"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="20"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="20"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="20"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="20"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="20"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="20"/>
     </row>
   </sheetData>
@@ -7426,24 +7506,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:N63"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>377</v>
       </c>
@@ -7454,7 +7534,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>373</v>
       </c>
@@ -7492,7 +7572,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1117</v>
       </c>
@@ -7533,7 +7613,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1127</v>
       </c>
@@ -7574,7 +7654,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1137</v>
       </c>
@@ -7615,7 +7695,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1139</v>
       </c>
@@ -7656,7 +7736,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1141</v>
       </c>
@@ -7700,7 +7780,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>422</v>
       </c>
@@ -7741,7 +7821,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1144</v>
       </c>
@@ -7782,7 +7862,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>428</v>
       </c>
@@ -7823,7 +7903,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1145</v>
       </c>
@@ -7864,7 +7944,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>434</v>
       </c>
@@ -7881,7 +7961,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>437</v>
       </c>
@@ -7892,7 +7972,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>438</v>
       </c>
@@ -7900,7 +7980,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1153</v>
       </c>
@@ -7941,7 +8021,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>450</v>
       </c>
@@ -7982,7 +8062,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>437</v>
       </c>
@@ -8023,7 +8103,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>453</v>
       </c>
@@ -8064,7 +8144,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1154</v>
       </c>
@@ -8105,7 +8185,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>466</v>
       </c>
@@ -8146,7 +8226,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1160</v>
       </c>
@@ -8187,7 +8267,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1167</v>
       </c>
@@ -8228,7 +8308,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>487</v>
       </c>
@@ -8269,7 +8349,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>488</v>
       </c>
@@ -8310,7 +8390,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>479</v>
       </c>
@@ -8351,7 +8431,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>484</v>
       </c>
@@ -8392,7 +8472,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1173</v>
       </c>
@@ -8433,7 +8513,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>479</v>
       </c>
@@ -8474,7 +8554,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>487</v>
       </c>
@@ -8515,7 +8595,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>488</v>
       </c>
@@ -8556,7 +8636,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>484</v>
       </c>
@@ -8597,7 +8677,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1177</v>
       </c>
@@ -8638,7 +8718,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="33" t="s">
         <v>479</v>
       </c>
@@ -8679,7 +8759,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="31" t="s">
         <v>487</v>
       </c>
@@ -8720,7 +8800,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="31" t="s">
         <v>488</v>
       </c>
@@ -8761,7 +8841,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1182</v>
       </c>
@@ -8805,7 +8885,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>518</v>
       </c>
@@ -8846,7 +8926,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>479</v>
       </c>
@@ -8887,7 +8967,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>487</v>
       </c>
@@ -8928,7 +9008,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>488</v>
       </c>
@@ -8969,7 +9049,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>484</v>
       </c>
@@ -9010,7 +9090,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>531</v>
       </c>
@@ -9051,7 +9131,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>532</v>
       </c>
@@ -9092,7 +9172,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1190</v>
       </c>
@@ -9136,7 +9216,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>518</v>
       </c>
@@ -9177,7 +9257,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>479</v>
       </c>
@@ -9218,7 +9298,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>487</v>
       </c>
@@ -9259,7 +9339,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>488</v>
       </c>
@@ -9300,7 +9380,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>484</v>
       </c>
@@ -9341,7 +9421,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>531</v>
       </c>
@@ -9382,7 +9462,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>532</v>
       </c>
@@ -9423,7 +9503,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1203</v>
       </c>
@@ -9467,7 +9547,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>518</v>
       </c>
@@ -9508,7 +9588,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>479</v>
       </c>
@@ -9549,27 +9629,27 @@
         <v>631</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>532</v>
       </c>

</xml_diff>

<commit_message>
Updated most of the TEST scripts to support new #!BIN/SH directive.  Also updated issue list.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19252B53-84FD-4B01-840D-175A4E5F5915}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D9B3C7-95F5-4361-ABC8-BFD8790F39D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="650">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2230,6 +2230,36 @@
   </si>
   <si>
     <t>In MAKE..TESTS is a new TESTMENU.  When you select choice 1 the command CORETEST (another script) gives you a syntax error.  If you type CORETEST at prompt it runs.  However, at the READ test, you enter Y, you get another Expression Syntax Error.   Update: Select choice 6 and you still get the CORETEST syntax error.</t>
+  </si>
+  <si>
+    <t>LOCKUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start AW with 8meg RAM3 support.  Boot Build.  MD /RAM3/A  … MD /RAM3/D  then CD .. to go to .BUILD, then CP -R * /RAM3/A and again for  B C D. </t>
+  </si>
+  <si>
+    <t>LS -L / or LS / displays results then locks machine.  LS on directories or files works fine.</t>
+  </si>
+  <si>
+    <t>Add -Q or quiet option that does not display filenames as they are copied.  Maybe a -q (can you have an upper and lower case option) that instead just displays a single dot "." for each file copied that way you can display ….... As copying goes.</t>
+  </si>
+  <si>
+    <t>Slows down.  In TESTS check COPYTORAM3.  If you do these same set of commands manually all the copies go flying by screen, but with script adter the copies start going slower and slower.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RM -R </t>
+  </si>
+  <si>
+    <t>Eventually crashes PRODOS HARD.   Do . Tests then run COPYTORAM3  then CD /RAM3 then RM -R A then RM-R B etc.  BOOM.</t>
+  </si>
+  <si>
+    <t>Look at listing as it goes by on a long RM batch and you will see times where right after a DIR removed with [OK] the next message appears on the same line instead of a new one.</t>
+  </si>
+  <si>
+    <t>On a long one, if it does it crash, near the end, the text starts to be gibberish, but the RM -R may complete.  When this does happen, the garbage text is always the same.</t>
+  </si>
+  <si>
+    <t>goto TESTS and run IFNUMTEST, notice the word ECHO that appears in top left of screen.  NO idea where this is coming from.  Also run IFSTRTEST, the echo commands are almost the same in both, but here the spaces are missing, the top line doesn’t center the same.</t>
   </si>
 </sst>
 </file>
@@ -3123,10 +3153,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5447,7 +5477,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="113" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B113" s="37">
         <v>204</v>
       </c>
@@ -5461,7 +5491,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="114" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B114" s="37">
         <v>205</v>
       </c>
@@ -5475,7 +5505,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="115" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B115" s="37">
         <v>206</v>
       </c>
@@ -5487,6 +5517,73 @@
       </c>
       <c r="E115" s="39" t="s">
         <v>639</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C116" s="38" t="s">
+        <v>640</v>
+      </c>
+      <c r="E116" s="39" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C117" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E117" s="39" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="C118" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="39" t="s">
+        <v>643</v>
+      </c>
+      <c r="F118" s="39" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="C119" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="39" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C120" s="38" t="s">
+        <v>645</v>
+      </c>
+      <c r="E120" s="39" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C121" s="38" t="s">
+        <v>645</v>
+      </c>
+      <c r="E121" s="39" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C122" s="38" t="s">
+        <v>645</v>
+      </c>
+      <c r="E122" s="39" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="C123" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E123" s="39" t="s">
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New ECHO issue plus closed other issues.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3B6B56-F27A-4531-BF84-9A6BC27ABDA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0A2C73-FA98-4726-AD54-E29841A1E7F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="570" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26355" yWindow="150" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Memory" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$127</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
   <calcPr calcId="181029" calcMode="manual"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="656">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2273,6 +2273,12 @@
   </si>
   <si>
     <t>Requestor was an idiot.</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>ECHO by itself directed to a file "ECHO &gt;&gt; afile" does not add a blank line to the file.</t>
   </si>
 </sst>
 </file>
@@ -3129,10 +3135,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G123"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3230,7 +3237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>46</v>
       </c>
@@ -3251,7 +3258,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>46</v>
       </c>
@@ -3273,7 +3280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>55</v>
       </c>
@@ -3295,7 +3302,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>46</v>
       </c>
@@ -3319,7 +3326,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>46</v>
       </c>
@@ -3343,7 +3350,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>46</v>
       </c>
@@ -3367,7 +3374,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>55</v>
       </c>
@@ -3389,7 +3396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>46</v>
       </c>
@@ -3408,7 +3415,7 @@
       </c>
       <c r="F15" s="29"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>46</v>
       </c>
@@ -3430,7 +3437,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>46</v>
       </c>
@@ -3454,7 +3461,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>55</v>
       </c>
@@ -3476,7 +3483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>46</v>
       </c>
@@ -3500,7 +3507,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>46</v>
       </c>
@@ -3524,7 +3531,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>55</v>
       </c>
@@ -3546,7 +3553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>46</v>
       </c>
@@ -3568,7 +3575,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>46</v>
       </c>
@@ -3614,7 +3621,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>46</v>
       </c>
@@ -3638,7 +3645,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>46</v>
       </c>
@@ -3683,7 +3690,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>46</v>
       </c>
@@ -3707,7 +3714,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>46</v>
       </c>
@@ -3731,7 +3738,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>46</v>
       </c>
@@ -3755,7 +3762,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>46</v>
       </c>
@@ -3779,7 +3786,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>46</v>
       </c>
@@ -3803,7 +3810,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>46</v>
       </c>
@@ -3827,7 +3834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>46</v>
       </c>
@@ -3851,7 +3858,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>46</v>
       </c>
@@ -3875,7 +3882,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>46</v>
       </c>
@@ -3896,7 +3903,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>46</v>
       </c>
@@ -3920,7 +3927,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>46</v>
       </c>
@@ -3944,7 +3951,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>46</v>
       </c>
@@ -3968,7 +3975,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>46</v>
       </c>
@@ -3989,7 +3996,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>46</v>
       </c>
@@ -4034,7 +4041,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>55</v>
       </c>
@@ -4103,7 +4110,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
         <v>46</v>
       </c>
@@ -4127,7 +4134,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
         <v>46</v>
       </c>
@@ -4151,7 +4158,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
         <v>46</v>
       </c>
@@ -4199,7 +4206,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
         <v>46</v>
       </c>
@@ -4223,7 +4230,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>46</v>
       </c>
@@ -4247,7 +4254,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>46</v>
       </c>
@@ -4271,7 +4278,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
         <v>46</v>
       </c>
@@ -4289,7 +4296,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>46</v>
       </c>
@@ -4310,7 +4317,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
         <v>46</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="27" t="s">
         <v>46</v>
       </c>
@@ -4352,7 +4359,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
         <v>46</v>
       </c>
@@ -4376,7 +4383,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
         <v>46</v>
       </c>
@@ -4396,7 +4403,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27" t="s">
         <v>46</v>
       </c>
@@ -4416,7 +4423,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
         <v>46</v>
       </c>
@@ -4436,7 +4443,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
         <v>46</v>
       </c>
@@ -4459,7 +4466,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
         <v>46</v>
       </c>
@@ -4482,7 +4489,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
         <v>46</v>
       </c>
@@ -4525,7 +4532,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27" t="s">
         <v>46</v>
       </c>
@@ -4545,7 +4552,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
         <v>46</v>
       </c>
@@ -4588,7 +4595,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>46</v>
       </c>
@@ -4609,6 +4616,9 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="27" t="s">
+        <v>654</v>
+      </c>
       <c r="B69" s="28">
         <v>161</v>
       </c>
@@ -4625,10 +4635,10 @@
         <v>326</v>
       </c>
       <c r="G69" s="31">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27" t="s">
         <v>46</v>
       </c>
@@ -4662,7 +4672,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
         <v>46</v>
       </c>
@@ -4696,7 +4706,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
         <v>46</v>
       </c>
@@ -4733,7 +4743,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="27" t="s">
         <v>46</v>
       </c>
@@ -4750,7 +4760,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="27" t="s">
         <v>46</v>
       </c>
@@ -4773,7 +4783,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
         <v>46</v>
       </c>
@@ -4810,7 +4820,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
         <v>46</v>
       </c>
@@ -4833,7 +4843,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
         <v>46</v>
       </c>
@@ -4853,7 +4863,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
         <v>46</v>
       </c>
@@ -4873,7 +4883,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
         <v>46</v>
       </c>
@@ -4896,7 +4906,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="27" t="s">
         <v>46</v>
       </c>
@@ -4916,7 +4926,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="27" t="s">
         <v>46</v>
       </c>
@@ -4939,7 +4949,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
         <v>46</v>
       </c>
@@ -4962,7 +4972,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
         <v>46</v>
       </c>
@@ -4985,7 +4995,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="27" t="s">
         <v>46</v>
       </c>
@@ -5008,7 +5018,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
         <v>46</v>
       </c>
@@ -5028,7 +5038,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="27" t="s">
         <v>46</v>
       </c>
@@ -5051,7 +5061,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="27" t="s">
         <v>46</v>
       </c>
@@ -5074,7 +5084,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="27" t="s">
         <v>46</v>
       </c>
@@ -5097,7 +5107,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="62" t="s">
         <v>46</v>
       </c>
@@ -5120,7 +5130,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="27" t="s">
         <v>46</v>
       </c>
@@ -5143,7 +5153,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="27" t="s">
         <v>46</v>
       </c>
@@ -5166,7 +5176,10 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B96" s="28">
         <v>187</v>
       </c>
@@ -5183,7 +5196,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="27" t="s">
         <v>46</v>
       </c>
@@ -5203,7 +5216,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="27" t="s">
         <v>46</v>
       </c>
@@ -5237,7 +5250,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="27" t="s">
         <v>46</v>
       </c>
@@ -5277,7 +5290,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="27" t="s">
         <v>46</v>
       </c>
@@ -5300,7 +5313,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="27" t="s">
         <v>46</v>
       </c>
@@ -5320,7 +5333,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="27" t="s">
         <v>46</v>
       </c>
@@ -5341,6 +5354,9 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="27" t="s">
+        <v>654</v>
+      </c>
       <c r="B105" s="28">
         <v>196</v>
       </c>
@@ -5371,7 +5387,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="27" t="s">
         <v>46</v>
       </c>
@@ -5431,7 +5447,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="27" t="s">
         <v>46</v>
       </c>
@@ -5454,7 +5470,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="27" t="s">
         <v>46</v>
       </c>
@@ -5474,7 +5490,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="27" t="s">
         <v>46</v>
       </c>
@@ -5491,7 +5507,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="27" t="s">
         <v>46</v>
       </c>
@@ -5508,7 +5524,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="27" t="s">
         <v>46</v>
       </c>
@@ -5525,7 +5541,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="27" t="s">
         <v>46</v>
       </c>
@@ -5542,9 +5558,12 @@
         <v>635</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="B116" s="28">
+        <v>207</v>
       </c>
       <c r="C116" s="29" t="s">
         <v>636</v>
@@ -5553,9 +5572,12 @@
         <v>637</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="B117" s="28">
+        <v>208</v>
       </c>
       <c r="C117" s="29" t="s">
         <v>39</v>
@@ -5567,9 +5589,12 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="B118" s="28">
+        <v>209</v>
       </c>
       <c r="C118" s="29" t="s">
         <v>9</v>
@@ -5581,9 +5606,12 @@
         <v>653</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="B119" s="28">
+        <v>210</v>
       </c>
       <c r="C119" s="29" t="s">
         <v>9</v>
@@ -5592,9 +5620,12 @@
         <v>640</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="B120" s="28">
+        <v>211</v>
       </c>
       <c r="C120" s="29" t="s">
         <v>641</v>
@@ -5604,6 +5635,9 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B121" s="28">
+        <v>212</v>
+      </c>
       <c r="C121" s="29" t="s">
         <v>641</v>
       </c>
@@ -5611,9 +5645,12 @@
         <v>643</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="B122" s="28">
+        <v>213</v>
       </c>
       <c r="C122" s="29" t="s">
         <v>641</v>
@@ -5622,9 +5659,12 @@
         <v>644</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="B123" s="28">
+        <v>214</v>
       </c>
       <c r="C123" s="29" t="s">
         <v>76</v>
@@ -5639,8 +5679,43 @@
         <v>1245</v>
       </c>
     </row>
+    <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B124" s="28">
+        <v>215</v>
+      </c>
+      <c r="C124" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E124" s="30" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="28">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="28">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="28">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G123" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A7:G127" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="D"/>
+        <filter val="E"/>
+        <filter val="HT"/>
+        <filter val="V"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
I am done stuck with the IF/Syntax Problems.  Committing updates and my MAKE
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B40DFC-AB21-48EE-9A22-9C0A1908E1B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A507DC-8C7E-4BDA-80A9-56191BC90121}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26355" yWindow="150" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="675" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="663">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2288,6 +2288,18 @@
   </si>
   <si>
     <t>Does not seem to generate expected results, perhaps need proper syntax.  Tried httpget 10.0.0.159 to local server and tried httpget www.chowse.com and did display was bad.</t>
+  </si>
+  <si>
+    <t>In TESTS, CAT CATCHARS (without the -A) puts something into the next commandline buffer resulting in next thing being a bad command.</t>
+  </si>
+  <si>
+    <t>Comment out the EXIT 0 in your TSH script then run it, behavior is not right</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>I am getting Expression Syntax Errors everywhere.  I cannot get Ifs to work.  I cant do IF -Z or -N and Echo statements are the ones throwing errors, nothing makes sense.  GO RUN Updated IFSTRTEST in MAKE…TESTS.  Testing again non-existent Vars causes problems, which was whole point of -Z -N, how should this work, I am going in circles.</t>
   </si>
 </sst>
 </file>
@@ -3145,10 +3157,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,6 +5742,41 @@
       </c>
       <c r="E127" s="30" t="s">
         <v>658</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B128" s="28">
+        <v>219</v>
+      </c>
+      <c r="C128" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="E128" s="30" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B129" s="28">
+        <v>220</v>
+      </c>
+      <c r="C129" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B130" s="28">
+        <v>221</v>
+      </c>
+      <c r="E130" s="30" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="28" t="s">
+        <v>661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make so Remy can see SH changes.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A507DC-8C7E-4BDA-80A9-56191BC90121}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86FA005-A456-445A-8B21-590BB6C8A0FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="675" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="645" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="665">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2296,10 +2296,16 @@
     <t>Comment out the EXIT 0 in your TSH script then run it, behavior is not right</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>I am getting Expression Syntax Errors everywhere.  I cannot get Ifs to work.  I cant do IF -Z or -N and Echo statements are the ones throwing errors, nothing makes sense.  GO RUN Updated IFSTRTEST in MAKE…TESTS.  Testing again non-existent Vars causes problems, which was whole point of -Z -N, how should this work, I am going in circles.</t>
+  </si>
+  <si>
+    <t>Whatever change you made in 1275 and still in 1277 broke ADMINMENU and CORETEST and other things.  I will push my MAKE.  if you boot MAKE, or with your normal drives loaded.   at : prompt  do PREFIX /MAKE and then -STABLE to run old B1272  and then after login you can ADMIN and see menu works fine.  Boot normal way and then . ADMIN and then ADMINMENU and see that only option 1 works and youa re trapped in menu (seletion option 1 and control-C at pause)</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>Run READIF test in TESTS.  If you answer Y/N/1/2 or anything to the question, the script performs normally (PASS/FAIL based on your answers) but if you just press Return (empty response) then errors are generated as if the VAR Z doesn't exists (READ never sets it) as oppose to it just being empty.  Script wise this could be caught with -Z -N but wonder if READ should not return something.</t>
   </si>
 </sst>
 </file>
@@ -3157,10 +3163,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5763,7 +5769,7 @@
         <v>276</v>
       </c>
       <c r="E129" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="130" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -5774,9 +5780,26 @@
         <v>660</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="28" t="s">
-        <v>661</v>
+    <row r="131" spans="2:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="B131" s="28">
+        <v>222</v>
+      </c>
+      <c r="C131" s="29" t="s">
+        <v>663</v>
+      </c>
+      <c r="E131" s="30" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B132" s="28">
+        <v>223</v>
+      </c>
+      <c r="C132" s="29" t="s">
+        <v>663</v>
+      </c>
+      <c r="E132" s="30" t="s">
+        <v>664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tests and Issue List
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86FA005-A456-445A-8B21-590BB6C8A0FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5BEB9B-5D4B-485F-BAF6-8B508F592FEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="645" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2299,13 +2299,13 @@
     <t>I am getting Expression Syntax Errors everywhere.  I cannot get Ifs to work.  I cant do IF -Z or -N and Echo statements are the ones throwing errors, nothing makes sense.  GO RUN Updated IFSTRTEST in MAKE…TESTS.  Testing again non-existent Vars causes problems, which was whole point of -Z -N, how should this work, I am going in circles.</t>
   </si>
   <si>
-    <t>Whatever change you made in 1275 and still in 1277 broke ADMINMENU and CORETEST and other things.  I will push my MAKE.  if you boot MAKE, or with your normal drives loaded.   at : prompt  do PREFIX /MAKE and then -STABLE to run old B1272  and then after login you can ADMIN and see menu works fine.  Boot normal way and then . ADMIN and then ADMINMENU and see that only option 1 works and youa re trapped in menu (seletion option 1 and control-C at pause)</t>
-  </si>
-  <si>
     <t>SH</t>
   </si>
   <si>
     <t>Run READIF test in TESTS.  If you answer Y/N/1/2 or anything to the question, the script performs normally (PASS/FAIL based on your answers) but if you just press Return (empty response) then errors are generated as if the VAR Z doesn't exists (READ never sets it) as oppose to it just being empty.  Script wise this could be caught with -Z -N but wonder if READ should not return something.</t>
+  </si>
+  <si>
+    <t>Whatever change you made in 1275 and still in 1277 broke ADMINMENU and CORETEST and other things.  I will push my MAKE.  if you boot MAKE, or with your normal drives loaded.   at : prompt  do PREFIX /MAKE and then -STABLE to run old B1272  and then after login you can ADMIN and see menu works fine.  Boot normal way and then . ADMIN and then ADMINMENU and see that only option 1 works and youa re trapped in menu (seletion option 1 and control-C at pause).  Update: run ENVTEST, note that entering 20 does nothing, but other values (40,60,80,100) work.  All values work in previous build.</t>
   </si>
 </sst>
 </file>
@@ -3163,10 +3163,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5780,15 +5780,15 @@
         <v>660</v>
       </c>
     </row>
-    <row r="131" spans="2:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:5" ht="210" x14ac:dyDescent="0.25">
       <c r="B131" s="28">
         <v>222</v>
       </c>
       <c r="C131" s="29" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E131" s="30" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="132" spans="2:5" ht="135" x14ac:dyDescent="0.25">
@@ -5796,10 +5796,15 @@
         <v>223</v>
       </c>
       <c r="C132" s="29" t="s">
+        <v>662</v>
+      </c>
+      <c r="E132" s="30" t="s">
         <v>663</v>
       </c>
-      <c r="E132" s="30" t="s">
-        <v>664</v>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="28">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tests and XLS issues list.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5BEB9B-5D4B-485F-BAF6-8B508F592FEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE135A2-09C5-42EE-92E2-6D9CB5ADF5D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="645" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21915" yWindow="285" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="667">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2306,6 +2306,12 @@
   </si>
   <si>
     <t>Whatever change you made in 1275 and still in 1277 broke ADMINMENU and CORETEST and other things.  I will push my MAKE.  if you boot MAKE, or with your normal drives loaded.   at : prompt  do PREFIX /MAKE and then -STABLE to run old B1272  and then after login you can ADMIN and see menu works fine.  Boot normal way and then . ADMIN and then ADMINMENU and see that only option 1 works and youa re trapped in menu (seletion option 1 and control-C at pause).  Update: run ENVTEST, note that entering 20 does nothing, but other values (40,60,80,100) work.  All values work in previous build.</t>
+  </si>
+  <si>
+    <t>Appears to be fixed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no way to compare 2 strings to sort them i.e. a &gt; or &lt; or .GT option for strings.  </t>
   </si>
 </sst>
 </file>
@@ -3165,8 +3171,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5662,6 +5668,9 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A121" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B121" s="28">
         <v>212</v>
       </c>
@@ -5671,6 +5680,9 @@
       <c r="E121" s="30" t="s">
         <v>643</v>
       </c>
+      <c r="F121" s="30" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="122" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="27" t="s">
@@ -5707,6 +5719,9 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B124" s="28">
         <v>215</v>
       </c>
@@ -5716,8 +5731,14 @@
       <c r="E124" s="30" t="s">
         <v>655</v>
       </c>
+      <c r="F124" s="30" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B125" s="28">
         <v>216</v>
       </c>
@@ -5726,6 +5747,9 @@
       </c>
       <c r="E125" s="30" t="s">
         <v>656</v>
+      </c>
+      <c r="F125" s="30" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5751,6 +5775,9 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A128" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="B128" s="28">
         <v>219</v>
       </c>
@@ -5761,7 +5788,10 @@
         <v>659</v>
       </c>
     </row>
-    <row r="129" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A129" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B129" s="28">
         <v>220</v>
       </c>
@@ -5771,16 +5801,28 @@
       <c r="E129" s="30" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="130" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F129" s="30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B130" s="28">
         <v>221</v>
       </c>
       <c r="E130" s="30" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="131" spans="2:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="F130" s="30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A131" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B131" s="28">
         <v>222</v>
       </c>
@@ -5790,8 +5832,11 @@
       <c r="E131" s="30" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="132" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="F131" s="30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B132" s="28">
         <v>223</v>
       </c>
@@ -5802,9 +5847,15 @@
         <v>663</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B133" s="28">
         <v>224</v>
+      </c>
+      <c r="C133" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="E133" s="30" t="s">
+        <v>666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated XLS list.  Also updated draft of Notes for Developers.md so you can see preview.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE135A2-09C5-42EE-92E2-6D9CB5ADF5D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD2D54D-E81D-43BD-B502-90019AD5804B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21915" yWindow="285" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="673">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2312,6 +2312,24 @@
   </si>
   <si>
     <t xml:space="preserve">There is no way to compare 2 strings to sort them i.e. a &gt; or &lt; or .GT option for strings.  </t>
+  </si>
+  <si>
+    <t>SH CD</t>
+  </si>
+  <si>
+    <t>CD .\\  at prompt crashes A2osX.</t>
+  </si>
+  <si>
+    <t>RAM3</t>
+  </si>
+  <si>
+    <t>COPYTORAM3 script crashes A2osx during 3rd copy.</t>
+  </si>
+  <si>
+    <t>FOR F IN `LS TL*` ; echo $F ; NEXT    locks TTY after displaying results (in ROOT homedir)</t>
+  </si>
+  <si>
+    <t>Same as above but change echo $F to CAT $F and you get an invalid path error and lock of TTY.  I think one of these two (227 or 228) actually lead to a disconnect in ProDos, which I have been seeing more and more.  At some point you do something and then every thing you type at prompt gets a Invalid Path error (unless it is internel command).</t>
   </si>
 </sst>
 </file>
@@ -3169,10 +3187,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5856,6 +5874,50 @@
       </c>
       <c r="E133" s="30" t="s">
         <v>666</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B134" s="28">
+        <v>225</v>
+      </c>
+      <c r="C134" s="29" t="s">
+        <v>667</v>
+      </c>
+      <c r="E134" s="30" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B135" s="28">
+        <v>226</v>
+      </c>
+      <c r="C135" s="29" t="s">
+        <v>669</v>
+      </c>
+      <c r="E135" s="30" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B136" s="28">
+        <v>227</v>
+      </c>
+      <c r="C136" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E136" s="30" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B137" s="28">
+        <v>228</v>
+      </c>
+      <c r="C137" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E137" s="30" t="s">
+        <v>672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MAKE with many changes in TEST.  1 issue added to list, updates to many TEST scripts.  BUILDTEST now does 68 tests across 10-12 scripts.  2 tests deleted as they have been merged into other tests.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD2D54D-E81D-43BD-B502-90019AD5804B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C8E40-E17A-40EE-A0F0-ACF70AE43E76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21915" yWindow="285" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="674">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2330,6 +2330,9 @@
   </si>
   <si>
     <t>Same as above but change echo $F to CAT $F and you get an invalid path error and lock of TTY.  I think one of these two (227 or 228) actually lead to a disconnect in ProDos, which I have been seeing more and more.  At some point you do something and then every thing you type at prompt gets a Invalid Path error (unless it is internel command).</t>
+  </si>
+  <si>
+    <t>There is no way to tell if a VAR is a string or a number.  -Z/-N tells you if they are null, but if you do a READ VARa, and want to check if the result is a number from 1 to 10, you can't check with -GT option if user typed ABC, it gives error.</t>
   </si>
 </sst>
 </file>
@@ -3187,10 +3190,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5918,6 +5921,17 @@
       </c>
       <c r="E137" s="30" t="s">
         <v>672</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B138" s="28">
+        <v>229</v>
+      </c>
+      <c r="C138" s="29" t="s">
+        <v>662</v>
+      </c>
+      <c r="E138" s="30" t="s">
+        <v>673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated issue list, updated tests and make with updated tests.  Removed some test files that have been combined into other tests.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C8E40-E17A-40EE-A0F0-ACF70AE43E76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEDC1DE-5052-48AB-AA52-7E43E1EEE9C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21915" yWindow="285" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23850" yWindow="15" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="676">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2333,6 +2333,12 @@
   </si>
   <si>
     <t>There is no way to tell if a VAR is a string or a number.  -Z/-N tells you if they are null, but if you do a READ VARa, and want to check if the result is a number from 1 to 10, you can't check with -GT option if user typed ABC, it gives error.</t>
+  </si>
+  <si>
+    <t>VT100 Codes</t>
+  </si>
+  <si>
+    <t>The Clear to Begin of Line Code does not clear the first 3 characters of the line it was supposed to clear.  See new VTTEST Test 7.  The VT100 code that is broken is \e[1K</t>
   </si>
 </sst>
 </file>
@@ -3190,10 +3196,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G138"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5932,6 +5938,17 @@
       </c>
       <c r="E138" s="30" t="s">
         <v>673</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B139" s="28">
+        <v>230</v>
+      </c>
+      <c r="C139" s="29" t="s">
+        <v>674</v>
+      </c>
+      <c r="E139" s="30" t="s">
+        <v>675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructured README file and created new sub files for News, Screen Shots and Technical Spec.  README will be updated again to refer to these other files before release.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12AC9C7-6AA3-4488-BD1E-273886FC1712}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23850" yWindow="20" windowWidth="19560" windowHeight="10880"/>
+    <workbookView xWindow="-23850" yWindow="15" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$139</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +32,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Patrick</author>
     <author>Patrick Kloepfer</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="1">
+    <comment ref="B45" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="1">
+    <comment ref="B53" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -152,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B61" authorId="1">
+    <comment ref="B61" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="685">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2349,18 +2355,30 @@
     <t>added &lt; &amp; &gt; for string compare</t>
   </si>
   <si>
-    <t>???? Cannot reproduce</t>
-  </si>
-  <si>
     <t>NOFIX</t>
+  </si>
+  <si>
+    <t>Add -F option that like -C lists all files in column but provides the full path name of each file.</t>
+  </si>
+  <si>
+    <t>This is different then 196, its more broke now.  196 was that more didn’t display a USAGE msg, it just gave you back prompt.  Now you get stuck in more input hell.</t>
+  </si>
+  <si>
+    <t>Closing, can't reproduce in current build.</t>
+  </si>
+  <si>
+    <t>Now failing at copy 4 in build 1298.</t>
+  </si>
+  <si>
+    <t>Fixed, confirmed with VTTEST.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2741,7 +2759,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -3201,35 +3219,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I132" sqref="I132"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="28" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="28" customWidth="1"/>
     <col min="3" max="3" width="14" style="29" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="27" customWidth="1"/>
     <col min="5" max="5" width="44" style="30" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" style="31" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="31"/>
+    <col min="6" max="6" width="34.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="31" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>62</v>
       </c>
@@ -3244,7 +3262,7 @@
       <c r="F2" s="35"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="38" t="s">
         <v>55</v>
@@ -3257,7 +3275,7 @@
       <c r="F3" s="40"/>
       <c r="G3" s="41"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="38" t="s">
         <v>121</v>
@@ -3270,7 +3288,7 @@
       <c r="F4" s="40"/>
       <c r="G4" s="41"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="43" t="s">
         <v>53</v>
@@ -3283,12 +3301,12 @@
       <c r="F5" s="45"/>
       <c r="G5" s="46"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>3</v>
       </c>
@@ -3311,7 +3329,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>46</v>
       </c>
@@ -3332,7 +3350,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>46</v>
       </c>
@@ -3354,7 +3372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>55</v>
       </c>
@@ -3376,7 +3394,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>46</v>
       </c>
@@ -3489,7 +3507,7 @@
       </c>
       <c r="F15" s="29"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>46</v>
       </c>
@@ -3557,7 +3575,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>46</v>
       </c>
@@ -3673,7 +3691,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>53</v>
       </c>
@@ -3740,7 +3758,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>53</v>
       </c>
@@ -4094,7 +4112,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>53</v>
       </c>
@@ -4139,7 +4157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>121</v>
       </c>
@@ -4160,7 +4178,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>121</v>
       </c>
@@ -4256,7 +4274,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
         <v>53</v>
       </c>
@@ -4328,7 +4346,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>46</v>
       </c>
@@ -4583,7 +4601,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
         <v>53</v>
       </c>
@@ -4646,7 +4664,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>325</v>
       </c>
@@ -4689,7 +4707,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
         <v>654</v>
       </c>
@@ -4712,7 +4730,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27" t="s">
         <v>46</v>
       </c>
@@ -4732,7 +4750,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B71" s="28">
         <v>163</v>
       </c>
@@ -4763,7 +4781,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
         <v>53</v>
       </c>
@@ -4797,7 +4815,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
         <v>53</v>
       </c>
@@ -4877,7 +4895,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
         <v>53</v>
       </c>
@@ -5023,7 +5041,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
         <v>46</v>
       </c>
@@ -5310,7 +5328,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B99" s="28">
         <v>190</v>
       </c>
@@ -5344,7 +5362,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B101" s="28">
         <v>192</v>
       </c>
@@ -5427,7 +5445,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="27" t="s">
         <v>654</v>
       </c>
@@ -5447,7 +5465,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B106" s="28">
         <v>197</v>
       </c>
@@ -5484,7 +5502,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="B108" s="28">
         <v>199</v>
       </c>
@@ -5501,7 +5519,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="27" t="s">
         <v>53</v>
       </c>
@@ -5708,7 +5726,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="27" t="s">
         <v>46</v>
       </c>
@@ -5793,7 +5811,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B126" s="28">
         <v>217</v>
       </c>
@@ -5803,8 +5821,11 @@
       <c r="E126" s="30" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="F126" s="30" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B127" s="28">
         <v>218</v>
       </c>
@@ -5815,7 +5836,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="27" t="s">
         <v>53</v>
       </c>
@@ -5829,7 +5850,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="27" t="s">
         <v>46</v>
       </c>
@@ -5877,7 +5898,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="B132" s="28">
         <v>223</v>
       </c>
@@ -5891,10 +5912,10 @@
         <v>676</v>
       </c>
       <c r="G132" s="31" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B133" s="28">
         <v>224</v>
       </c>
@@ -5908,7 +5929,10 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B134" s="28">
         <v>225</v>
       </c>
@@ -5919,10 +5943,10 @@
         <v>668</v>
       </c>
       <c r="F134" s="30" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="28">
         <v>226</v>
       </c>
@@ -5932,8 +5956,14 @@
       <c r="E135" s="30" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F135" s="30" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B136" s="28">
         <v>227</v>
       </c>
@@ -5943,11 +5973,14 @@
       <c r="E136" s="30" t="s">
         <v>671</v>
       </c>
+      <c r="F136" s="30" t="s">
+        <v>273</v>
+      </c>
       <c r="G136" s="31">
         <v>1298</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B137" s="28">
         <v>228</v>
       </c>
@@ -5964,7 +5997,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B138" s="28">
         <v>229</v>
       </c>
@@ -5981,7 +6014,10 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A139" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B139" s="28">
         <v>230</v>
       </c>
@@ -5991,12 +6027,26 @@
       <c r="E139" s="30" t="s">
         <v>675</v>
       </c>
+      <c r="F139" s="30" t="s">
+        <v>684</v>
+      </c>
       <c r="G139" s="31">
         <v>1298</v>
       </c>
     </row>
+    <row r="140" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B140" s="28">
+        <v>231</v>
+      </c>
+      <c r="C140" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E140" s="30" t="s">
+        <v>680</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G139">
+  <autoFilter ref="A7:G139" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -6015,23 +6065,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6129,7 +6179,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>66</v>
@@ -6146,7 +6196,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>46</v>
       </c>
@@ -6163,7 +6213,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -6207,7 +6257,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>77</v>
@@ -6241,7 +6291,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>83</v>
@@ -6275,7 +6325,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>90</v>
@@ -6292,7 +6342,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>93</v>
@@ -6505,7 +6555,7 @@
       </c>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
         <v>108</v>
@@ -6524,7 +6574,7 @@
       </c>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="10" t="s">
         <v>160</v>
@@ -6543,7 +6593,7 @@
       </c>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>46</v>
       </c>
@@ -6600,7 +6650,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="10" t="s">
         <v>164</v>
@@ -6670,7 +6720,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
         <v>168</v>
@@ -6831,7 +6881,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>256</v>
       </c>
@@ -6932,7 +6982,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -6957,7 +7007,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>302</v>
       </c>
@@ -7089,7 +7139,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>392</v>
       </c>
@@ -7101,7 +7151,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63"/>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -7111,27 +7161,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I93"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="12" customWidth="1"/>
     <col min="3" max="3" width="8" style="69" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="12"/>
-    <col min="6" max="6" width="5.81640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="69"/>
-    <col min="8" max="8" width="52.1796875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="12"/>
+    <col min="4" max="4" width="5.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="12"/>
+    <col min="6" max="6" width="5.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="69"/>
+    <col min="8" max="8" width="52.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="12" t="s">
         <v>28</v>
       </c>
@@ -7150,7 +7200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -7158,7 +7208,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="72" t="s">
         <v>361</v>
       </c>
@@ -7169,7 +7219,7 @@
       <c r="G4" s="73"/>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
         <v>362</v>
       </c>
@@ -7180,7 +7230,7 @@
       <c r="G5" s="74"/>
       <c r="H5" s="74"/>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
@@ -7188,12 +7238,12 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>1</v>
       </c>
@@ -7219,7 +7269,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
@@ -7234,7 +7284,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>594</v>
       </c>
@@ -7245,7 +7295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>592</v>
       </c>
@@ -7256,7 +7306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>593</v>
       </c>
@@ -7267,7 +7317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>331</v>
       </c>
@@ -7278,7 +7328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>583</v>
       </c>
@@ -7289,7 +7339,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
@@ -7300,7 +7350,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>202</v>
       </c>
@@ -7311,7 +7361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -7322,7 +7372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
@@ -7336,7 +7386,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>584</v>
       </c>
@@ -7347,7 +7397,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>596</v>
       </c>
@@ -7358,7 +7408,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>453</v>
       </c>
@@ -7369,7 +7419,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>591</v>
       </c>
@@ -7383,7 +7433,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>597</v>
       </c>
@@ -7394,7 +7444,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>575</v>
       </c>
@@ -7405,7 +7455,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
@@ -7416,7 +7466,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>599</v>
       </c>
@@ -7430,7 +7480,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>582</v>
       </c>
@@ -7441,7 +7491,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>585</v>
       </c>
@@ -7455,7 +7505,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>600</v>
       </c>
@@ -7469,7 +7519,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
@@ -7480,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>586</v>
       </c>
@@ -7494,7 +7544,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>587</v>
       </c>
@@ -7508,7 +7558,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
@@ -7519,7 +7569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>588</v>
       </c>
@@ -7533,7 +7583,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>595</v>
       </c>
@@ -7547,7 +7597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>589</v>
       </c>
@@ -7561,7 +7611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
@@ -7572,7 +7622,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>23</v>
       </c>
@@ -7583,7 +7633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>590</v>
       </c>
@@ -7597,7 +7647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>598</v>
       </c>
@@ -7611,7 +7661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>152</v>
       </c>
@@ -7622,7 +7672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>24</v>
       </c>
@@ -7633,7 +7683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
@@ -7644,7 +7694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>25</v>
       </c>
@@ -7655,7 +7705,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>230</v>
       </c>
@@ -7666,7 +7716,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>58</v>
       </c>
@@ -7677,7 +7727,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
@@ -7691,7 +7741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>287</v>
       </c>
@@ -7705,270 +7755,270 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="I49" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="I50" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="I51" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="I52" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="I53" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="I54" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="I55" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="I56" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="I57" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="I58" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="I59" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="I60" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="I61" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="I62" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="I63" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="I64" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="I65" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="I66" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="I67" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="I68" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="I69" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="I70" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="I71" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="I72" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="I73" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="I74" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="I75" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="I76" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="I77" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="I78" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="I79" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="I80" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="I81" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="I82" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="I83" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="I84" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="I85" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="I86" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="I87" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="I88" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="I89" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="I91" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="I92" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="12" t="s">
         <v>28</v>
       </c>
@@ -7988,24 +8038,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:N63"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>377</v>
       </c>
@@ -8016,7 +8066,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>373</v>
       </c>
@@ -8054,7 +8104,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1117</v>
       </c>
@@ -8095,7 +8145,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1127</v>
       </c>
@@ -8136,7 +8186,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1137</v>
       </c>
@@ -8177,7 +8227,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1139</v>
       </c>
@@ -8218,7 +8268,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1141</v>
       </c>
@@ -8262,7 +8312,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>422</v>
       </c>
@@ -8303,7 +8353,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1144</v>
       </c>
@@ -8344,7 +8394,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>428</v>
       </c>
@@ -8385,7 +8435,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1145</v>
       </c>
@@ -8426,7 +8476,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>434</v>
       </c>
@@ -8443,7 +8493,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>437</v>
       </c>
@@ -8454,7 +8504,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>438</v>
       </c>
@@ -8462,7 +8512,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1153</v>
       </c>
@@ -8503,7 +8553,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>450</v>
       </c>
@@ -8544,7 +8594,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>437</v>
       </c>
@@ -8585,7 +8635,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>453</v>
       </c>
@@ -8626,7 +8676,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1154</v>
       </c>
@@ -8667,7 +8717,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>466</v>
       </c>
@@ -8708,7 +8758,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1160</v>
       </c>
@@ -8749,7 +8799,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1167</v>
       </c>
@@ -8790,7 +8840,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>487</v>
       </c>
@@ -8831,7 +8881,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>488</v>
       </c>
@@ -8872,7 +8922,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>479</v>
       </c>
@@ -8913,7 +8963,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>484</v>
       </c>
@@ -8954,7 +9004,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1173</v>
       </c>
@@ -8995,7 +9045,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>479</v>
       </c>
@@ -9036,7 +9086,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>487</v>
       </c>
@@ -9077,7 +9127,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>488</v>
       </c>
@@ -9118,7 +9168,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>484</v>
       </c>
@@ -9159,7 +9209,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1177</v>
       </c>
@@ -9200,7 +9250,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
         <v>479</v>
       </c>
@@ -9241,7 +9291,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
         <v>487</v>
       </c>
@@ -9282,7 +9332,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
         <v>488</v>
       </c>
@@ -9323,7 +9373,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1182</v>
       </c>
@@ -9367,7 +9417,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>518</v>
       </c>
@@ -9408,7 +9458,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>479</v>
       </c>
@@ -9449,7 +9499,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>487</v>
       </c>
@@ -9490,7 +9540,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>488</v>
       </c>
@@ -9531,7 +9581,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>484</v>
       </c>
@@ -9572,7 +9622,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>531</v>
       </c>
@@ -9613,7 +9663,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>532</v>
       </c>
@@ -9654,7 +9704,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1190</v>
       </c>
@@ -9698,7 +9748,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>518</v>
       </c>
@@ -9739,7 +9789,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>479</v>
       </c>
@@ -9780,7 +9830,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>487</v>
       </c>
@@ -9821,7 +9871,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>488</v>
       </c>
@@ -9862,7 +9912,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>484</v>
       </c>
@@ -9903,7 +9953,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>531</v>
       </c>
@@ -9944,7 +9994,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>532</v>
       </c>
@@ -9985,7 +10035,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1203</v>
       </c>
@@ -10029,7 +10079,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>518</v>
       </c>
@@ -10070,7 +10120,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>479</v>
       </c>
@@ -10111,27 +10161,27 @@
         <v>627</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>532</v>
       </c>

</xml_diff>

<commit_message>
Updated MAKE and XLS.  MAKE needed to test latest issue, see XLS.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53075BE1-52E0-4F09-A167-972C7610676A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23850" yWindow="20" windowWidth="19560" windowHeight="10880"/>
+    <workbookView xWindow="-24645" yWindow="510" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Issues!$A$7:$G$142</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Suggestions!$A$1:$G$63</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +32,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Patrick</author>
     <author>Patrick Kloepfer</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="1">
+    <comment ref="B45" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="1">
+    <comment ref="B53" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -152,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B61" authorId="1">
+    <comment ref="B61" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="692">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2381,13 +2387,19 @@
   <si>
     <t>The slots are tagged only if driver's  detection found HW and loaded properly, except Z80 &amp; Block Devices tagged at KERNEL INIT</t>
   </si>
+  <si>
+    <t>Editing of command line when lines grows to more then 80 chars is off.</t>
+  </si>
+  <si>
+    <t>Memory corruption or something.  Using latest MAKE mounted.  Boot BUILD.  RM ../ETC/PASSWD to be sure you do not have one.  Then ADMIN.  Option 6 (usermenu) then L to List users.  It will prompt you to make PASSWD, say yes then notice that User list display is all corrupted,    BUT exit out (pressing return X for exit 0 to exit, etc.) until back at $ prompt of root.  Do ADMIN again, and list users, it is clean and fine.  Corruption happens to mem only executing create of file commands then display.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2768,7 +2780,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -3228,35 +3240,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="28" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="28" customWidth="1"/>
     <col min="3" max="3" width="14" style="29" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="27" customWidth="1"/>
     <col min="5" max="5" width="44" style="30" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" style="31" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="31"/>
+    <col min="6" max="6" width="34.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="31" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>62</v>
       </c>
@@ -3271,7 +3283,7 @@
       <c r="F2" s="35"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="38" t="s">
         <v>55</v>
@@ -3284,7 +3296,7 @@
       <c r="F3" s="40"/>
       <c r="G3" s="41"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="38" t="s">
         <v>121</v>
@@ -3297,7 +3309,7 @@
       <c r="F4" s="40"/>
       <c r="G4" s="41"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="43" t="s">
         <v>53</v>
@@ -3310,12 +3322,12 @@
       <c r="F5" s="45"/>
       <c r="G5" s="46"/>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>3</v>
       </c>
@@ -3338,7 +3350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>46</v>
       </c>
@@ -3359,7 +3371,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>46</v>
       </c>
@@ -3381,7 +3393,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>55</v>
       </c>
@@ -3403,7 +3415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>46</v>
       </c>
@@ -3516,7 +3528,7 @@
       </c>
       <c r="F15" s="29"/>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>46</v>
       </c>
@@ -3584,7 +3596,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>46</v>
       </c>
@@ -3700,7 +3712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>53</v>
       </c>
@@ -3767,7 +3779,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>53</v>
       </c>
@@ -4121,7 +4133,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>53</v>
       </c>
@@ -4166,7 +4178,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>121</v>
       </c>
@@ -4187,7 +4199,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>121</v>
       </c>
@@ -4283,7 +4295,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
         <v>53</v>
       </c>
@@ -4355,7 +4367,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>46</v>
       </c>
@@ -4610,7 +4622,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
         <v>53</v>
       </c>
@@ -4673,7 +4685,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>325</v>
       </c>
@@ -4716,7 +4728,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
         <v>654</v>
       </c>
@@ -4739,7 +4751,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27" t="s">
         <v>46</v>
       </c>
@@ -4759,7 +4771,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B71" s="28">
         <v>163</v>
       </c>
@@ -4790,7 +4802,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
         <v>53</v>
       </c>
@@ -4824,7 +4836,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
         <v>53</v>
       </c>
@@ -4904,7 +4916,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
         <v>53</v>
       </c>
@@ -5050,7 +5062,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
         <v>46</v>
       </c>
@@ -5337,7 +5349,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B99" s="28">
         <v>190</v>
       </c>
@@ -5371,7 +5383,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B101" s="28">
         <v>192</v>
       </c>
@@ -5454,9 +5466,9 @@
         <v>620</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="27" t="s">
-        <v>654</v>
+        <v>46</v>
       </c>
       <c r="B105" s="28">
         <v>196</v>
@@ -5477,7 +5489,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B106" s="28">
         <v>197</v>
       </c>
@@ -5514,7 +5526,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="B108" s="28">
         <v>199</v>
       </c>
@@ -5531,7 +5543,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="27" t="s">
         <v>53</v>
       </c>
@@ -5823,7 +5835,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B126" s="28">
         <v>217</v>
       </c>
@@ -5840,7 +5852,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B127" s="28">
         <v>218</v>
       </c>
@@ -5851,7 +5863,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="27" t="s">
         <v>53</v>
       </c>
@@ -5913,7 +5925,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="B132" s="28">
         <v>223</v>
       </c>
@@ -5930,7 +5942,10 @@
         <v>679</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B133" s="28">
         <v>224</v>
       </c>
@@ -5944,7 +5959,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="27" t="s">
         <v>46</v>
       </c>
@@ -5961,7 +5976,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="28">
         <v>226</v>
       </c>
@@ -5975,7 +5990,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="27" t="s">
         <v>46</v>
       </c>
@@ -5995,7 +6010,10 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A137" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B137" s="28">
         <v>228</v>
       </c>
@@ -6012,7 +6030,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B138" s="28">
         <v>229</v>
       </c>
@@ -6029,7 +6047,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="27" t="s">
         <v>46</v>
       </c>
@@ -6049,7 +6067,10 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A140" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B140" s="28">
         <v>231</v>
       </c>
@@ -6066,7 +6087,10 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A141" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B141" s="28">
         <v>232</v>
       </c>
@@ -6083,7 +6107,10 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A142" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B142" s="28">
         <v>233</v>
       </c>
@@ -6097,8 +6124,30 @@
         <v>1302</v>
       </c>
     </row>
+    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B143" s="28">
+        <v>234</v>
+      </c>
+      <c r="C143" s="29" t="s">
+        <v>662</v>
+      </c>
+      <c r="E143" s="30" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="B144" s="28">
+        <v>235</v>
+      </c>
+      <c r="C144" s="29" t="s">
+        <v>662</v>
+      </c>
+      <c r="E144" s="30" t="s">
+        <v>691</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:G142">
+  <autoFilter ref="A7:G142" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="D"/>
@@ -6117,23 +6166,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6231,7 +6280,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>66</v>
@@ -6248,7 +6297,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>46</v>
       </c>
@@ -6265,7 +6314,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -6309,7 +6358,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>77</v>
@@ -6343,7 +6392,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>83</v>
@@ -6377,7 +6426,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>90</v>
@@ -6394,7 +6443,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>93</v>
@@ -6607,7 +6656,7 @@
       </c>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
         <v>108</v>
@@ -6626,7 +6675,7 @@
       </c>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="10" t="s">
         <v>160</v>
@@ -6645,7 +6694,7 @@
       </c>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>46</v>
       </c>
@@ -6702,7 +6751,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="10" t="s">
         <v>164</v>
@@ -6772,7 +6821,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
         <v>168</v>
@@ -6933,7 +6982,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>256</v>
       </c>
@@ -7034,7 +7083,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
@@ -7059,7 +7108,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>302</v>
       </c>
@@ -7191,7 +7240,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>392</v>
       </c>
@@ -7203,7 +7252,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G63"/>
+  <autoFilter ref="A1:G63" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -7213,27 +7262,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I93"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="12" customWidth="1"/>
     <col min="3" max="3" width="8" style="69" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="12"/>
-    <col min="6" max="6" width="5.81640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="69"/>
-    <col min="8" max="8" width="52.1796875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="12"/>
+    <col min="4" max="4" width="5.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="12"/>
+    <col min="6" max="6" width="5.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="69"/>
+    <col min="8" max="8" width="52.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I1" s="12" t="s">
         <v>28</v>
       </c>
@@ -7252,7 +7301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -7260,7 +7309,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="72" t="s">
         <v>361</v>
       </c>
@@ -7271,7 +7320,7 @@
       <c r="G4" s="73"/>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="2:9" ht="83.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
         <v>362</v>
       </c>
@@ -7282,7 +7331,7 @@
       <c r="G5" s="74"/>
       <c r="H5" s="74"/>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
@@ -7290,12 +7339,12 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>1</v>
       </c>
@@ -7321,7 +7370,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
@@ -7336,7 +7385,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>594</v>
       </c>
@@ -7347,7 +7396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>592</v>
       </c>
@@ -7358,7 +7407,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>593</v>
       </c>
@@ -7369,7 +7418,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>331</v>
       </c>
@@ -7380,7 +7429,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>583</v>
       </c>
@@ -7391,7 +7440,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
@@ -7402,7 +7451,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>202</v>
       </c>
@@ -7413,7 +7462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -7424,7 +7473,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
@@ -7438,7 +7487,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>584</v>
       </c>
@@ -7449,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>596</v>
       </c>
@@ -7460,7 +7509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>453</v>
       </c>
@@ -7471,7 +7520,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>591</v>
       </c>
@@ -7485,7 +7534,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>597</v>
       </c>
@@ -7496,7 +7545,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>575</v>
       </c>
@@ -7507,7 +7556,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
@@ -7518,7 +7567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>599</v>
       </c>
@@ -7532,7 +7581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>582</v>
       </c>
@@ -7543,7 +7592,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>585</v>
       </c>
@@ -7557,7 +7606,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>600</v>
       </c>
@@ -7571,7 +7620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
@@ -7582,7 +7631,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>586</v>
       </c>
@@ -7596,7 +7645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>587</v>
       </c>
@@ -7610,7 +7659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
@@ -7621,7 +7670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>588</v>
       </c>
@@ -7635,7 +7684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>595</v>
       </c>
@@ -7649,7 +7698,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>589</v>
       </c>
@@ -7663,7 +7712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
@@ -7674,7 +7723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>23</v>
       </c>
@@ -7685,7 +7734,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>590</v>
       </c>
@@ -7699,7 +7748,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>598</v>
       </c>
@@ -7713,7 +7762,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>152</v>
       </c>
@@ -7724,7 +7773,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>24</v>
       </c>
@@ -7735,7 +7784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
@@ -7746,7 +7795,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>25</v>
       </c>
@@ -7757,7 +7806,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>230</v>
       </c>
@@ -7768,7 +7817,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>58</v>
       </c>
@@ -7779,7 +7828,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
@@ -7793,7 +7842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>287</v>
       </c>
@@ -7807,270 +7856,270 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="I49" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="I50" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="I51" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="I52" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="I53" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="I54" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="I55" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="I56" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="I57" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="I58" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="I59" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="I60" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="I61" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="I62" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="I63" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="I64" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="I65" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="I66" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="I67" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="I68" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="I69" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="I70" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="I71" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="I72" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="I73" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="I74" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="I75" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="I76" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="I77" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="I78" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="I79" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="I80" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="I81" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="I82" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="I83" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="I84" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="I85" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="I86" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="I87" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="I88" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="I89" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I90" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="I91" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="I92" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I93" s="12" t="s">
         <v>28</v>
       </c>
@@ -8090,24 +8139,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:N63"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>377</v>
       </c>
@@ -8118,7 +8167,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>373</v>
       </c>
@@ -8156,7 +8205,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1117</v>
       </c>
@@ -8197,7 +8246,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1127</v>
       </c>
@@ -8238,7 +8287,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1137</v>
       </c>
@@ -8279,7 +8328,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1139</v>
       </c>
@@ -8320,7 +8369,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1141</v>
       </c>
@@ -8364,7 +8413,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>422</v>
       </c>
@@ -8405,7 +8454,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1144</v>
       </c>
@@ -8446,7 +8495,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>428</v>
       </c>
@@ -8487,7 +8536,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1145</v>
       </c>
@@ -8528,7 +8577,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>434</v>
       </c>
@@ -8545,7 +8594,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>437</v>
       </c>
@@ -8556,7 +8605,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>438</v>
       </c>
@@ -8564,7 +8613,7 @@
         <v>14057</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1153</v>
       </c>
@@ -8605,7 +8654,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>450</v>
       </c>
@@ -8646,7 +8695,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>437</v>
       </c>
@@ -8687,7 +8736,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>453</v>
       </c>
@@ -8728,7 +8777,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1154</v>
       </c>
@@ -8769,7 +8818,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>466</v>
       </c>
@@ -8810,7 +8859,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1160</v>
       </c>
@@ -8851,7 +8900,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1167</v>
       </c>
@@ -8892,7 +8941,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>487</v>
       </c>
@@ -8933,7 +8982,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>488</v>
       </c>
@@ -8974,7 +9023,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>479</v>
       </c>
@@ -9015,7 +9064,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>484</v>
       </c>
@@ -9056,7 +9105,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1173</v>
       </c>
@@ -9097,7 +9146,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>479</v>
       </c>
@@ -9138,7 +9187,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>487</v>
       </c>
@@ -9179,7 +9228,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>488</v>
       </c>
@@ -9220,7 +9269,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>484</v>
       </c>
@@ -9261,7 +9310,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1177</v>
       </c>
@@ -9302,7 +9351,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
         <v>479</v>
       </c>
@@ -9343,7 +9392,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
         <v>487</v>
       </c>
@@ -9384,7 +9433,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
         <v>488</v>
       </c>
@@ -9425,7 +9474,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1182</v>
       </c>
@@ -9469,7 +9518,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>518</v>
       </c>
@@ -9510,7 +9559,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>479</v>
       </c>
@@ -9551,7 +9600,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>487</v>
       </c>
@@ -9592,7 +9641,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>488</v>
       </c>
@@ -9633,7 +9682,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>484</v>
       </c>
@@ -9674,7 +9723,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>531</v>
       </c>
@@ -9715,7 +9764,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>532</v>
       </c>
@@ -9756,7 +9805,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1190</v>
       </c>
@@ -9800,7 +9849,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>518</v>
       </c>
@@ -9841,7 +9890,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>479</v>
       </c>
@@ -9882,7 +9931,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>487</v>
       </c>
@@ -9923,7 +9972,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>488</v>
       </c>
@@ -9964,7 +10013,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>484</v>
       </c>
@@ -10005,7 +10054,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>531</v>
       </c>
@@ -10046,7 +10095,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>532</v>
       </c>
@@ -10087,7 +10136,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1203</v>
       </c>
@@ -10131,7 +10180,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>518</v>
       </c>
@@ -10172,7 +10221,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>479</v>
       </c>
@@ -10213,27 +10262,27 @@
         <v>627</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>532</v>
       </c>

</xml_diff>

<commit_message>
Updated Issue List.  Major Update of Technical Spec.md  Please see note on Slack before editing/reading.
</commit_message>
<xml_diff>
--- a/.A2osX Issue List.xlsx
+++ b/.A2osX Issue List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\brfs\PKProjects\A20sX-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53075BE1-52E0-4F09-A167-972C7610676A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DFE573-CDDD-4280-81FE-B5EA189B63CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24645" yWindow="510" windowWidth="19560" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="693">
   <si>
     <t>Issue No.</t>
   </si>
@@ -2392,6 +2392,9 @@
   </si>
   <si>
     <t>Memory corruption or something.  Using latest MAKE mounted.  Boot BUILD.  RM ../ETC/PASSWD to be sure you do not have one.  Then ADMIN.  Option 6 (usermenu) then L to List users.  It will prompt you to make PASSWD, say yes then notice that User list display is all corrupted,    BUT exit out (pressing return X for exit 0 to exit, etc.) until back at $ prompt of root.  Do ADMIN again, and list users, it is clean and fine.  Corruption happens to mem only executing create of file commands then display.</t>
+  </si>
+  <si>
+    <t>Update:  if you boot BUILD then RM passwd then CD /MAKE/USR/SHARE/ADMIN and do LISTUSERS (bypassing all the menus) everything works fine.  More hints that it is a memmgt/pointer problem.  It only happens when script calls scrupt calls scipt that then does this set of commands.</t>
   </si>
 </sst>
 </file>
@@ -3252,7 +3255,7 @@
   <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6144,6 +6147,9 @@
       </c>
       <c r="E144" s="30" t="s">
         <v>691</v>
+      </c>
+      <c r="F144" s="30" t="s">
+        <v>692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>